<commit_message>
Nhóm Bảo,Tuấn,Tú nộp bài Defect Log.xlsx
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="8580"/>
@@ -13,12 +13,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Defect Log'!$B$4:$T$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Defect Log'!$B$2:$T$54</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
   <si>
     <t>Project Code:</t>
   </si>
@@ -333,16 +333,64 @@
   </si>
   <si>
     <t>Warning: This session is created only for doing value validation. Please do not do modify this.</t>
+  </si>
+  <si>
+    <t>Media Option_Permission</t>
+  </si>
+  <si>
+    <t>Phân quyền Media cho user, dư thừa không cần thiết.</t>
+  </si>
+  <si>
+    <t>Media Option_Component</t>
+  </si>
+  <si>
+    <t>Cấu hình media, dư thừa không cần thiết.</t>
+  </si>
+  <si>
+    <t>Category và section</t>
+  </si>
+  <si>
+    <t>Lỗi giá trị không đồng nhất (giá trị liên kết giữa 2 bảng)</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Thiếu catid</t>
+  </si>
+  <si>
+    <t>Event trong Article</t>
+  </si>
+  <si>
+    <t>Thiếu event select change của combox section</t>
+  </si>
+  <si>
+    <t>Media Manager</t>
+  </si>
+  <si>
+    <t>chkThumbnailView và chkDetailView không thể dùng checkbox</t>
+  </si>
+  <si>
+    <t>txtFilePath bị dư</t>
+  </si>
+  <si>
+    <t>chkSelectFile không cần thiết</t>
+  </si>
+  <si>
+    <t>Thiếu sự kiện select chọn trong folder</t>
+  </si>
+  <si>
+    <t>CMS Click and Change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -637,7 +685,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -672,7 +719,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -848,14 +894,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AF54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
@@ -884,16 +930,18 @@
     <col min="32" max="32" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32">
       <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="17" t="s">
+        <v>120</v>
+      </c>
       <c r="E2" s="16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="2:32" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:32" s="2" customFormat="1" ht="27.75" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
@@ -964,11 +1012,19 @@
       <c r="AE4"/>
       <c r="AF4"/>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+    <row r="5" spans="2:32">
+      <c r="B5" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -985,11 +1041,19 @@
       <c r="S5" s="14"/>
       <c r="T5" s="11"/>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+    <row r="6" spans="2:32">
+      <c r="B6" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1036,11 +1100,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+    <row r="7" spans="2:32">
+      <c r="B7" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1084,11 +1156,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+    <row r="8" spans="2:32">
+      <c r="B8" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -1132,11 +1212,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+    <row r="9" spans="2:32">
+      <c r="B9" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1180,11 +1268,19 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+    <row r="10" spans="2:32">
+      <c r="B10" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1228,11 +1324,19 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+    <row r="11" spans="2:32">
+      <c r="B11" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1270,11 +1374,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+    <row r="12" spans="2:32">
+      <c r="B12" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1312,11 +1424,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+    <row r="13" spans="2:32">
+      <c r="B13" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1354,7 +1474,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32">
       <c r="B14" s="8"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1393,7 +1513,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:32">
       <c r="B15" s="8"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1432,7 +1552,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:32">
       <c r="B16" s="8"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1468,7 +1588,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:31">
       <c r="B17" s="8"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1504,7 +1624,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:31">
       <c r="B18" s="8"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1534,7 +1654,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:31">
       <c r="B19" s="8"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1564,7 +1684,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:31">
       <c r="B20" s="8"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1591,7 +1711,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:31">
       <c r="B21" s="8"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1618,7 +1738,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:31">
       <c r="B22" s="8"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1642,7 +1762,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:31">
       <c r="B23" s="8"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1666,7 +1786,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:31">
       <c r="B24" s="8"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1690,7 +1810,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:31">
       <c r="B25" s="8"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1714,7 +1834,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:31">
       <c r="B26" s="8"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1738,7 +1858,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:31">
       <c r="B27" s="8"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1759,7 +1879,7 @@
       <c r="S27" s="14"/>
       <c r="T27" s="11"/>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:31">
       <c r="B28" s="8"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1780,7 +1900,7 @@
       <c r="S28" s="14"/>
       <c r="T28" s="11"/>
     </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:31">
       <c r="B29" s="8"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1801,7 +1921,7 @@
       <c r="S29" s="14"/>
       <c r="T29" s="11"/>
     </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:31">
       <c r="B30" s="8"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1822,7 +1942,7 @@
       <c r="S30" s="14"/>
       <c r="T30" s="11"/>
     </row>
-    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:31">
       <c r="B31" s="8"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -1843,7 +1963,7 @@
       <c r="S31" s="14"/>
       <c r="T31" s="11"/>
     </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:31">
       <c r="B32" s="8"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -1864,7 +1984,7 @@
       <c r="S32" s="14"/>
       <c r="T32" s="11"/>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20">
       <c r="B33" s="8"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -1885,7 +2005,7 @@
       <c r="S33" s="14"/>
       <c r="T33" s="11"/>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20">
       <c r="B34" s="8"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1906,7 +2026,7 @@
       <c r="S34" s="14"/>
       <c r="T34" s="11"/>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20">
       <c r="B35" s="8"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -1927,7 +2047,7 @@
       <c r="S35" s="14"/>
       <c r="T35" s="11"/>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20">
       <c r="B36" s="8"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1948,7 +2068,7 @@
       <c r="S36" s="14"/>
       <c r="T36" s="11"/>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20">
       <c r="B37" s="8"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -1969,7 +2089,7 @@
       <c r="S37" s="14"/>
       <c r="T37" s="11"/>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20">
       <c r="B38" s="8"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -1990,7 +2110,7 @@
       <c r="S38" s="14"/>
       <c r="T38" s="11"/>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20">
       <c r="B39" s="8"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -2011,7 +2131,7 @@
       <c r="S39" s="14"/>
       <c r="T39" s="11"/>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20">
       <c r="B40" s="8"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -2032,7 +2152,7 @@
       <c r="S40" s="14"/>
       <c r="T40" s="11"/>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20">
       <c r="B41" s="8"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -2053,7 +2173,7 @@
       <c r="S41" s="14"/>
       <c r="T41" s="11"/>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:20">
       <c r="B42" s="8"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -2074,7 +2194,7 @@
       <c r="S42" s="14"/>
       <c r="T42" s="11"/>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:20">
       <c r="B43" s="8"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -2095,7 +2215,7 @@
       <c r="S43" s="14"/>
       <c r="T43" s="11"/>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20">
       <c r="B44" s="8"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -2116,7 +2236,7 @@
       <c r="S44" s="14"/>
       <c r="T44" s="11"/>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:20">
       <c r="B45" s="8"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -2137,7 +2257,7 @@
       <c r="S45" s="14"/>
       <c r="T45" s="11"/>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:20">
       <c r="B46" s="8"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -2158,7 +2278,7 @@
       <c r="S46" s="14"/>
       <c r="T46" s="11"/>
     </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:20">
       <c r="B47" s="8"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -2179,7 +2299,7 @@
       <c r="S47" s="14"/>
       <c r="T47" s="11"/>
     </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:20">
       <c r="B48" s="8"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -2200,7 +2320,7 @@
       <c r="S48" s="14"/>
       <c r="T48" s="11"/>
     </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:20">
       <c r="B49" s="8"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -2221,7 +2341,7 @@
       <c r="S49" s="14"/>
       <c r="T49" s="11"/>
     </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:20">
       <c r="B50" s="8"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -2242,7 +2362,7 @@
       <c r="S50" s="14"/>
       <c r="T50" s="11"/>
     </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:20">
       <c r="B51" s="8"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
@@ -2263,7 +2383,7 @@
       <c r="S51" s="14"/>
       <c r="T51" s="11"/>
     </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:20">
       <c r="B52" s="8"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -2284,7 +2404,7 @@
       <c r="S52" s="14"/>
       <c r="T52" s="11"/>
     </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:20">
       <c r="B53" s="8"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -2305,7 +2425,7 @@
       <c r="S53" s="14"/>
       <c r="T53" s="11"/>
     </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:20">
       <c r="B54" s="9"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -2355,7 +2475,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="62" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="62" orientation="portrait" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="9" min="1" max="53" man="1"/>
   </colBreaks>

</xml_diff>

<commit_message>
Nhóm ThanhChV, HuyDV, DucNH, LinhTA nộp bài Defect Log.xlsx
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="140">
   <si>
     <t>Project Code:</t>
   </si>
@@ -381,6 +381,63 @@
   </si>
   <si>
     <t>CMS Click and Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language manager </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dư column Version </t>
+  </si>
+  <si>
+    <t>Dư column Date</t>
+  </si>
+  <si>
+    <t>New &amp; Edit user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dư phần Basic Setting  </t>
+  </si>
+  <si>
+    <t>Dư các  group user :  publisher, editor, super administrator, author, editor.</t>
+  </si>
+  <si>
+    <t>New &amp; Edit user(mapping items to db)</t>
+  </si>
+  <si>
+    <t>Dư column Cofirm password trong phần mapping to db</t>
+  </si>
+  <si>
+    <t>new &amp; edit user</t>
+  </si>
+  <si>
+    <t>Dùng các radion button thay cho cac check box trong Assigned User Groups</t>
+  </si>
+  <si>
+    <t>Contend manager _ Article manager(Item Definition)</t>
+  </si>
+  <si>
+    <t>Contend manager_ Article manager(events)</t>
+  </si>
+  <si>
+    <t>Mô tả sai event của btnpublishArticle</t>
+  </si>
+  <si>
+    <t>Mô tả sai event của btnunpublishArticle</t>
+  </si>
+  <si>
+    <t>Contend manager_ Article manager(item definition)</t>
+  </si>
+  <si>
+    <t>các items : pageNumberList, itemNotes có type là : html, mô tả type của item  chưa rõ.!</t>
+  </si>
+  <si>
+    <t>Contend manager_ Article manager(event)</t>
+  </si>
+  <si>
+    <t>Mô tả chưa chính xác event của btnreset</t>
+  </si>
+  <si>
+    <t>mô tả thiếu item btnhelp trong phần item definiton</t>
   </si>
 </sst>
 </file>
@@ -898,7 +955,7 @@
   <dimension ref="B2:AF54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1514,10 +1571,18 @@
       </c>
     </row>
     <row r="15" spans="2:32">
-      <c r="B15" s="8"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="B15" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1553,10 +1618,18 @@
       </c>
     </row>
     <row r="16" spans="2:32">
-      <c r="B16" s="8"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -1589,10 +1662,18 @@
       </c>
     </row>
     <row r="17" spans="2:31">
-      <c r="B17" s="8"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="B17" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -1625,10 +1706,18 @@
       </c>
     </row>
     <row r="18" spans="2:31">
-      <c r="B18" s="8"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="B18" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -1655,10 +1744,18 @@
       </c>
     </row>
     <row r="19" spans="2:31">
-      <c r="B19" s="8"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="B19" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -1685,10 +1782,18 @@
       </c>
     </row>
     <row r="20" spans="2:31">
-      <c r="B20" s="8"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="B20" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -1712,10 +1817,18 @@
       </c>
     </row>
     <row r="21" spans="2:31">
-      <c r="B21" s="8"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="B21" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1739,10 +1852,18 @@
       </c>
     </row>
     <row r="22" spans="2:31">
-      <c r="B22" s="8"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="B22" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1763,10 +1884,18 @@
       </c>
     </row>
     <row r="23" spans="2:31">
-      <c r="B23" s="8"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="B23" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1787,10 +1916,18 @@
       </c>
     </row>
     <row r="24" spans="2:31">
-      <c r="B24" s="8"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="B24" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1811,10 +1948,18 @@
       </c>
     </row>
     <row r="25" spans="2:31">
-      <c r="B25" s="8"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="B25" s="8">
+        <v>40837</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>

</xml_diff>

<commit_message>
nhóm : ThanhChV, LinhTA, DucNH, HuyDV update file defect log.xlsx
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="8580"/>
@@ -13,7 +13,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Defect Log'!$B$4:$T$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Defect Log'!$B$2:$T$54</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="177">
   <si>
     <t>Project Code:</t>
   </si>
@@ -866,9 +866,6 @@
   </si>
   <si>
     <t>Contend manager_ Article manager(event)</t>
-  </si>
-  <si>
-    <t>Mô tả chưa chính xác event của btnreset</t>
   </si>
   <si>
     <t>mô tả thiếu item btnhelp trong phần item definiton</t>
@@ -957,16 +954,91 @@
   <si>
     <t>Closed Date
 (*)</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>SDD_Language manager.xlsx, revesion 126</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HuyDV</t>
+  </si>
+  <si>
+    <t>LinhTA</t>
+  </si>
+  <si>
+    <t>Bỏ Column Version ( sửa lại các phần : giao diện, definition items, mapping item to db, events có liên quan tới phần bị bỏ này).</t>
+  </si>
+  <si>
+    <t>Rặp khuôn theo Joomla</t>
+  </si>
+  <si>
+    <t>ThanhChV</t>
+  </si>
+  <si>
+    <t>Bỏ Column Date( sửa lại các phần : giao diện, definition items, mapping item to db, events có liên quan tới phần bị bỏ này).</t>
+  </si>
+  <si>
+    <t>SDD_New&amp;EditUser.xls, revesion 126</t>
+  </si>
+  <si>
+    <t>HuyDV</t>
+  </si>
+  <si>
+    <t>Bỏ phần Basic setting(( sửa lại các phần : giao diện, definition items, mapping item to db, events có liên quan tới phần bị bỏ này).</t>
+  </si>
+  <si>
+    <t>SDD_New&amp;EditUser.xls,revesion 126</t>
+  </si>
+  <si>
+    <t>Bỏ các group user bị dư.</t>
+  </si>
+  <si>
+    <t>Bỏ  column " cofirm password " trong thiết kế db User.</t>
+  </si>
+  <si>
+    <t>Sai sót của developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LinhTA</t>
+  </si>
+  <si>
+    <t>Thay các check box trong   Assigned User Groups bằng radion button (( sửa lại các phần : giao diện, definition items, mapping item to db, events có liên quan tới phần bi sửa này).</t>
+  </si>
+  <si>
+    <t>SDD_ContentManager_DucNH.xls,revesion 126</t>
+  </si>
+  <si>
+    <t>DucNH</t>
+  </si>
+  <si>
+    <t>Bổ sung mô tả  btnhelp vào phần definition item.</t>
+  </si>
+  <si>
+    <t>Sửa lại  event của btnpublishArticle</t>
+  </si>
+  <si>
+    <t>Sửa lại  event của btnunpublishArticle</t>
+  </si>
+  <si>
+    <t>sai sót của developer</t>
+  </si>
+  <si>
+    <t>mô tả ( giải thích rõ hơn )  type  của các items :  pageNumberList, itemNotes .</t>
+  </si>
+  <si>
+    <t>mô tả lại event của btnreset.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1316,7 +1388,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1351,7 +1422,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1527,14 +1597,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AF54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="K4" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -1551,7 +1621,7 @@
     <col min="13" max="13" width="12.28515625" style="3" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" style="3" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="3"/>
-    <col min="16" max="16" width="16.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="35" style="3" customWidth="1"/>
     <col min="17" max="17" width="14.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.42578125" style="3" customWidth="1"/>
     <col min="19" max="19" width="13.5703125" style="5" customWidth="1"/>
@@ -1570,7 +1640,7 @@
     <col min="33" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" ht="30">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1579,18 +1649,18 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1">
       <c r="B4" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>142</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>1</v>
@@ -1599,31 +1669,31 @@
         <v>2</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M4" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>7</v>
@@ -1632,10 +1702,10 @@
         <v>9</v>
       </c>
       <c r="S4" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="T4" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="T4" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="W4" s="4" t="s">
         <v>93</v>
@@ -1650,7 +1720,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:32">
       <c r="B5" s="11">
         <v>40837</v>
       </c>
@@ -1676,10 +1746,12 @@
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
-      <c r="S5" s="13"/>
+      <c r="S5" s="13" t="s">
+        <v>152</v>
+      </c>
       <c r="T5" s="14"/>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:32">
       <c r="B6" s="11">
         <v>40837</v>
       </c>
@@ -1738,7 +1810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:32">
       <c r="B7" s="11">
         <v>40837</v>
       </c>
@@ -1794,7 +1866,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:32">
       <c r="B8" s="11">
         <v>40837</v>
       </c>
@@ -1850,7 +1922,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:32">
       <c r="B9" s="11">
         <v>40837</v>
       </c>
@@ -1906,7 +1978,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:32">
       <c r="B10" s="11">
         <v>40837</v>
       </c>
@@ -1962,7 +2034,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:32">
       <c r="B11" s="11">
         <v>40837</v>
       </c>
@@ -2012,7 +2084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:32">
       <c r="B12" s="11">
         <v>40837</v>
       </c>
@@ -2062,7 +2134,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32">
       <c r="B13" s="11">
         <v>40837</v>
       </c>
@@ -2112,7 +2184,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32">
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -2151,7 +2223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:32" ht="35.25" customHeight="1">
       <c r="B15" s="11">
         <v>40837</v>
       </c>
@@ -2164,19 +2236,43 @@
       <c r="E15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
+      <c r="F15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
+      <c r="P15" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="R15" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="S15" s="13"/>
       <c r="T15" s="14"/>
       <c r="X15" s="3" t="s">
@@ -2198,7 +2294,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:32" ht="36" customHeight="1">
       <c r="B16" s="11">
         <v>40837</v>
       </c>
@@ -2211,19 +2307,43 @@
       <c r="E16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
+      <c r="F16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
+      <c r="P16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="S16" s="13"/>
       <c r="T16" s="14"/>
       <c r="X16" s="3" t="s">
@@ -2242,7 +2362,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:31" ht="47.25" customHeight="1">
       <c r="B17" s="11">
         <v>40837</v>
       </c>
@@ -2255,19 +2375,43 @@
       <c r="E17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="F17" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
+      <c r="P17" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="R17" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="S17" s="13"/>
       <c r="T17" s="14"/>
       <c r="X17" s="3" t="s">
@@ -2286,7 +2430,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:31" ht="30">
       <c r="B18" s="11">
         <v>40837</v>
       </c>
@@ -2299,19 +2443,43 @@
       <c r="E18" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
+      <c r="F18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
+      <c r="P18" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="R18" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="S18" s="13"/>
       <c r="T18" s="14"/>
       <c r="Y18" s="3" t="s">
@@ -2324,7 +2492,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:31" ht="36.75" customHeight="1">
       <c r="B19" s="11">
         <v>40837</v>
       </c>
@@ -2337,19 +2505,43 @@
       <c r="E19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
+      <c r="F19" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
+      <c r="P19" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q19" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="R19" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="S19" s="13"/>
       <c r="T19" s="14"/>
       <c r="Y19" s="3" t="s">
@@ -2362,7 +2554,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:31" ht="29.25" customHeight="1">
       <c r="B20" s="11">
         <v>40837</v>
       </c>
@@ -2375,19 +2567,43 @@
       <c r="E20" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
+      <c r="F20" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="12"/>
+      <c r="P20" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="R20" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="S20" s="13"/>
       <c r="T20" s="14"/>
       <c r="Y20" s="3" t="s">
@@ -2397,7 +2613,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:31" ht="33" customHeight="1">
       <c r="B21" s="11">
         <v>40837</v>
       </c>
@@ -2405,24 +2621,48 @@
         <v>120</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
+      <c r="F21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>170</v>
+      </c>
       <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
+      <c r="P21" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q21" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="R21" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="S21" s="13"/>
       <c r="T21" s="14"/>
       <c r="Y21" s="3" t="s">
@@ -2432,7 +2672,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:31" ht="30">
       <c r="B22" s="11">
         <v>40837</v>
       </c>
@@ -2445,26 +2685,50 @@
       <c r="E22" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
+      <c r="F22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>170</v>
+      </c>
       <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
+      <c r="P22" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q22" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="R22" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="S22" s="13"/>
       <c r="T22" s="14"/>
       <c r="AB22" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:31" ht="37.5" customHeight="1">
       <c r="B23" s="11">
         <v>40837</v>
       </c>
@@ -2477,26 +2741,50 @@
       <c r="E23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
+      <c r="F23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>170</v>
+      </c>
       <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
+      <c r="P23" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q23" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="R23" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="S23" s="13"/>
       <c r="T23" s="14"/>
       <c r="AB23" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:31" ht="43.5" customHeight="1">
       <c r="B24" s="11">
         <v>40837</v>
       </c>
@@ -2509,26 +2797,50 @@
       <c r="E24" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
+      <c r="F24" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>170</v>
+      </c>
       <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12"/>
+      <c r="P24" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q24" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="R24" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="S24" s="13"/>
       <c r="T24" s="14"/>
       <c r="AB24" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:31" ht="30">
       <c r="B25" s="11">
         <v>40837</v>
       </c>
@@ -2536,37 +2848,59 @@
         <v>126</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
+      <c r="F25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>170</v>
+      </c>
       <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12"/>
+      <c r="P25" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q25" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="R25" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="S25" s="13"/>
       <c r="T25" s="14"/>
       <c r="AB25" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:31">
       <c r="B26" s="11"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
@@ -2586,15 +2920,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:31">
       <c r="B27" s="11">
         <v>40837</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>11</v>
@@ -2615,15 +2949,15 @@
       <c r="S27" s="13"/>
       <c r="T27" s="14"/>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:31">
       <c r="B28" s="11">
         <v>40837</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>11</v>
@@ -2644,15 +2978,15 @@
       <c r="S28" s="13"/>
       <c r="T28" s="14"/>
     </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:31">
       <c r="B29" s="11">
         <v>40837</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>11</v>
@@ -2673,15 +3007,15 @@
       <c r="S29" s="13"/>
       <c r="T29" s="14"/>
     </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:31">
       <c r="B30" s="11">
         <v>40837</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>11</v>
@@ -2702,15 +3036,15 @@
       <c r="S30" s="13"/>
       <c r="T30" s="14"/>
     </row>
-    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:31">
       <c r="B31" s="11">
         <v>40837</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>11</v>
@@ -2731,15 +3065,15 @@
       <c r="S31" s="13"/>
       <c r="T31" s="14"/>
     </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:31">
       <c r="B32" s="11">
         <v>40837</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>11</v>
@@ -2760,15 +3094,15 @@
       <c r="S32" s="13"/>
       <c r="T32" s="14"/>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20">
       <c r="B33" s="11">
         <v>40837</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>11</v>
@@ -2789,15 +3123,15 @@
       <c r="S33" s="13"/>
       <c r="T33" s="14"/>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20">
       <c r="B34" s="11">
         <v>40837</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>11</v>
@@ -2818,7 +3152,7 @@
       <c r="S34" s="13"/>
       <c r="T34" s="14"/>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20">
       <c r="B35" s="11"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
@@ -2839,7 +3173,7 @@
       <c r="S35" s="13"/>
       <c r="T35" s="14"/>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20">
       <c r="B36" s="11"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -2860,7 +3194,7 @@
       <c r="S36" s="13"/>
       <c r="T36" s="14"/>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20">
       <c r="B37" s="11"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
@@ -2881,7 +3215,7 @@
       <c r="S37" s="13"/>
       <c r="T37" s="14"/>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20">
       <c r="B38" s="11"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -2902,7 +3236,7 @@
       <c r="S38" s="13"/>
       <c r="T38" s="14"/>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20">
       <c r="B39" s="11"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -2923,7 +3257,7 @@
       <c r="S39" s="13"/>
       <c r="T39" s="14"/>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20">
       <c r="B40" s="11"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
@@ -2944,7 +3278,7 @@
       <c r="S40" s="13"/>
       <c r="T40" s="14"/>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20">
       <c r="B41" s="11"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
@@ -2965,7 +3299,7 @@
       <c r="S41" s="13"/>
       <c r="T41" s="14"/>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:20">
       <c r="B42" s="11"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
@@ -2986,7 +3320,7 @@
       <c r="S42" s="13"/>
       <c r="T42" s="14"/>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:20">
       <c r="B43" s="11"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
@@ -3007,7 +3341,7 @@
       <c r="S43" s="13"/>
       <c r="T43" s="14"/>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20">
       <c r="B44" s="11"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
@@ -3028,7 +3362,7 @@
       <c r="S44" s="13"/>
       <c r="T44" s="14"/>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:20">
       <c r="B45" s="11"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
@@ -3049,7 +3383,7 @@
       <c r="S45" s="13"/>
       <c r="T45" s="14"/>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:20">
       <c r="B46" s="11"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
@@ -3070,7 +3404,7 @@
       <c r="S46" s="13"/>
       <c r="T46" s="14"/>
     </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:20">
       <c r="B47" s="11"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
@@ -3091,7 +3425,7 @@
       <c r="S47" s="13"/>
       <c r="T47" s="14"/>
     </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:20">
       <c r="B48" s="11"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
@@ -3112,7 +3446,7 @@
       <c r="S48" s="13"/>
       <c r="T48" s="14"/>
     </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:20">
       <c r="B49" s="11"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
@@ -3133,7 +3467,7 @@
       <c r="S49" s="13"/>
       <c r="T49" s="14"/>
     </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:20">
       <c r="B50" s="11"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
@@ -3154,7 +3488,7 @@
       <c r="S50" s="13"/>
       <c r="T50" s="14"/>
     </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:20">
       <c r="B51" s="11"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
@@ -3175,7 +3509,7 @@
       <c r="S51" s="13"/>
       <c r="T51" s="14"/>
     </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:20">
       <c r="B52" s="11"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -3196,7 +3530,7 @@
       <c r="S52" s="13"/>
       <c r="T52" s="14"/>
     </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:20">
       <c r="B53" s="11"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
@@ -3217,7 +3551,7 @@
       <c r="S53" s="13"/>
       <c r="T53" s="14"/>
     </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:20">
       <c r="B54" s="16"/>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>

</xml_diff>

<commit_message>
Thêm chi tiết vào Defect Log.xlsx của nhóm Bảo,Tuấn,Tú
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="189">
   <si>
     <t>Project Code:</t>
   </si>
@@ -956,9 +956,6 @@
 (*)</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>SDD_Language manager.xlsx, revesion 126</t>
   </si>
   <si>
@@ -1029,6 +1026,45 @@
   </si>
   <si>
     <t>mô tả lại event của btnreset.</t>
+  </si>
+  <si>
+    <t>TuTM</t>
+  </si>
+  <si>
+    <t>BaoNDD</t>
+  </si>
+  <si>
+    <t>TuanVA</t>
+  </si>
+  <si>
+    <t>SDD_MediaManager.xls, revesion 128</t>
+  </si>
+  <si>
+    <t>SDD_ContentManager_New&amp;Edit.xls, revesion 128</t>
+  </si>
+  <si>
+    <t>Phần này không cần làm</t>
+  </si>
+  <si>
+    <t>Sửa lại giá trị tương ứng cho đồng nhất</t>
+  </si>
+  <si>
+    <t>Thêm catid</t>
+  </si>
+  <si>
+    <t>Thêm event select change của combox section</t>
+  </si>
+  <si>
+    <t>Dùng button hoặc dùng link</t>
+  </si>
+  <si>
+    <t>Bỏ giá trị này</t>
+  </si>
+  <si>
+    <t>Thêm event select chọn trong folder</t>
+  </si>
+  <si>
+    <t>Không cần quá chi tiết như vậy</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1297,6 +1333,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1600,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AF54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="K4" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="J2" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1616,11 +1655,11 @@
     <col min="8" max="8" width="9.140625" style="3"/>
     <col min="9" max="9" width="21" style="3" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="23.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="34.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" style="3" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="3"/>
+    <col min="15" max="15" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="35" style="3" customWidth="1"/>
     <col min="17" max="17" width="14.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.42578125" style="3" customWidth="1"/>
@@ -1720,7 +1759,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="2:32">
+    <row r="5" spans="2:32" ht="45">
       <c r="B5" s="11">
         <v>40837</v>
       </c>
@@ -1733,25 +1772,51 @@
       <c r="E5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
+      <c r="F5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="O5" s="20">
+        <v>40838</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>188</v>
+      </c>
       <c r="R5" s="12"/>
-      <c r="S5" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="T5" s="14"/>
-    </row>
-    <row r="6" spans="2:32">
+      <c r="S5" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T5" s="14">
+        <v>40838</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" ht="45">
       <c r="B6" s="11">
         <v>40837</v>
       </c>
@@ -1764,21 +1829,49 @@
       <c r="E6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="O6" s="20">
+        <v>40838</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>188</v>
+      </c>
       <c r="R6" s="12"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="14"/>
+      <c r="S6" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T6" s="14">
+        <v>40838</v>
+      </c>
       <c r="W6" s="15" t="s">
         <v>10</v>
       </c>
@@ -1810,7 +1903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:32">
+    <row r="7" spans="2:32" ht="30">
       <c r="B7" s="11">
         <v>40837</v>
       </c>
@@ -1823,21 +1916,49 @@
       <c r="E7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="O7" s="20">
+        <v>40838</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="R7" s="12"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="14"/>
+      <c r="S7" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T7" s="14">
+        <v>40838</v>
+      </c>
       <c r="X7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1866,7 +1987,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:32">
+    <row r="8" spans="2:32" ht="30">
       <c r="B8" s="11">
         <v>40837</v>
       </c>
@@ -1879,21 +2000,49 @@
       <c r="E8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="O8" s="20">
+        <v>40838</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="R8" s="12"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="14"/>
+      <c r="S8" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T8" s="14">
+        <v>40838</v>
+      </c>
       <c r="X8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1922,7 +2071,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:32">
+    <row r="9" spans="2:32" ht="30">
       <c r="B9" s="11">
         <v>40837</v>
       </c>
@@ -1935,21 +2084,49 @@
       <c r="E9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="O9" s="20">
+        <v>40838</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="R9" s="12"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="14"/>
+      <c r="S9" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T9" s="14">
+        <v>40838</v>
+      </c>
       <c r="X9" s="3" t="s">
         <v>12</v>
       </c>
@@ -1978,7 +2155,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:32">
+    <row r="10" spans="2:32" ht="30">
       <c r="B10" s="11">
         <v>40837</v>
       </c>
@@ -1991,21 +2168,49 @@
       <c r="E10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
+      <c r="F10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="O10" s="20">
+        <v>40838</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="R10" s="12"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="14"/>
+      <c r="S10" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T10" s="14">
+        <v>40838</v>
+      </c>
       <c r="X10" s="3" t="s">
         <v>20</v>
       </c>
@@ -2034,7 +2239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:32">
+    <row r="11" spans="2:32" ht="30">
       <c r="B11" s="11">
         <v>40837</v>
       </c>
@@ -2047,21 +2252,49 @@
       <c r="E11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="O11" s="20">
+        <v>40838</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="R11" s="12"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="14"/>
+      <c r="S11" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T11" s="14">
+        <v>40838</v>
+      </c>
       <c r="X11" s="3" t="s">
         <v>18</v>
       </c>
@@ -2084,7 +2317,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:32">
+    <row r="12" spans="2:32" ht="30">
       <c r="B12" s="11">
         <v>40837</v>
       </c>
@@ -2097,21 +2330,49 @@
       <c r="E12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
+      <c r="F12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="O12" s="20">
+        <v>40838</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="R12" s="12"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="14"/>
+      <c r="S12" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T12" s="14">
+        <v>40838</v>
+      </c>
       <c r="X12" s="3" t="s">
         <v>19</v>
       </c>
@@ -2134,7 +2395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:32">
+    <row r="13" spans="2:32" ht="30">
       <c r="B13" s="11">
         <v>40837</v>
       </c>
@@ -2147,21 +2408,49 @@
       <c r="E13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
+      <c r="F13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="O13" s="20">
+        <v>40838</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q13" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="R13" s="12"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="14"/>
+      <c r="S13" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T13" s="14">
+        <v>40838</v>
+      </c>
       <c r="X13" s="3" t="s">
         <v>14</v>
       </c>
@@ -2184,7 +2473,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="2:32">
+    <row r="14" spans="2:32" ht="36" customHeight="1">
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -2223,7 +2512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:32" ht="35.25" customHeight="1">
+    <row r="15" spans="2:32" ht="60">
       <c r="B15" s="11">
         <v>40837</v>
       </c>
@@ -2252,23 +2541,23 @@
         <v>76</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M15" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="N15" s="12" t="s">
         <v>154</v>
-      </c>
-      <c r="N15" s="12" t="s">
-        <v>155</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q15" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="Q15" s="12" t="s">
-        <v>157</v>
       </c>
       <c r="R15" s="12" t="s">
         <v>24</v>
@@ -2323,23 +2612,23 @@
         <v>76</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O16" s="12"/>
       <c r="P16" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R16" s="12" t="s">
         <v>24</v>
@@ -2391,23 +2680,23 @@
         <v>76</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q17" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R17" s="12" t="s">
         <v>24</v>
@@ -2459,23 +2748,23 @@
         <v>77</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L18" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O18" s="12"/>
       <c r="P18" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R18" s="12" t="s">
         <v>24</v>
@@ -2521,23 +2810,23 @@
         <v>77</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L19" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q19" s="12" t="s">
         <v>165</v>
-      </c>
-      <c r="Q19" s="12" t="s">
-        <v>166</v>
       </c>
       <c r="R19" s="12" t="s">
         <v>92</v>
@@ -2583,23 +2872,23 @@
         <v>77</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R20" s="12" t="s">
         <v>24</v>
@@ -2642,23 +2931,23 @@
         <v>76</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L21" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O21" s="12"/>
       <c r="P21" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q21" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R21" s="12" t="s">
         <v>92</v>
@@ -2701,23 +2990,23 @@
         <v>77</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L22" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O22" s="12"/>
       <c r="P22" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q22" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R22" s="12" t="s">
         <v>92</v>
@@ -2757,23 +3046,23 @@
         <v>77</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L23" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O23" s="12"/>
       <c r="P23" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q23" s="12" t="s">
         <v>173</v>
-      </c>
-      <c r="Q23" s="12" t="s">
-        <v>174</v>
       </c>
       <c r="R23" s="12" t="s">
         <v>92</v>
@@ -2813,23 +3102,23 @@
         <v>78</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L24" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O24" s="12"/>
       <c r="P24" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Q24" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R24" s="12" t="s">
         <v>92</v>
@@ -2869,23 +3158,23 @@
         <v>76</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>84</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O25" s="12"/>
       <c r="P25" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q25" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R25" s="12" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Nhóm ThanhChV, HuyDV, DuoNH, LinhTA update thêm lỗi
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Defect Log'!$B$4:$T$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Defect Log'!$B$2:$T$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Defect Log'!$B$2:$T$55</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="191">
   <si>
     <t>Project Code:</t>
   </si>
@@ -698,9 +698,6 @@
   </si>
   <si>
     <t>Test plan</t>
-  </si>
-  <si>
-    <t>Test report</t>
   </si>
   <si>
     <t>Meeting minute</t>
@@ -1065,6 +1062,15 @@
   </si>
   <si>
     <t>Không cần quá chi tiết như vậy</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Nên gộp phần Name và Login nam lại làm một.</t>
+  </si>
+  <si>
+    <t>Bỏ text box name, sửa textbox login nam thành username ( sửa lại các phần : giao diện, definition items, mapping item to db, events có liên quan tới phần bị bỏ và bị sửa này).</t>
   </si>
 </sst>
 </file>
@@ -1637,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:AF54"/>
+  <dimension ref="B1:AF55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="J2" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="J21" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1679,27 +1685,32 @@
     <col min="33" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:32">
+      <c r="R1" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
     <row r="2" spans="2:32" ht="30">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1">
       <c r="B4" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>1</v>
@@ -1708,31 +1719,31 @@
         <v>2</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M4" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>7</v>
@@ -1741,13 +1752,13 @@
         <v>9</v>
       </c>
       <c r="S4" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="T4" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="T4" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="W4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
@@ -1764,10 +1775,10 @@
         <v>40837</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>94</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>95</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>11</v>
@@ -1785,28 +1796,28 @@
         <v>67</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M5" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="N5" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>177</v>
       </c>
       <c r="O5" s="20">
         <v>40838</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="13">
@@ -1821,10 +1832,10 @@
         <v>40837</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>96</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>97</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>11</v>
@@ -1842,28 +1853,28 @@
         <v>67</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M6" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="N6" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>177</v>
       </c>
       <c r="O6" s="20">
         <v>40838</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R6" s="12"/>
       <c r="S6" s="13">
@@ -1908,10 +1919,10 @@
         <v>40837</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>99</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>11</v>
@@ -1929,28 +1940,28 @@
         <v>67</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O7" s="20">
         <v>40838</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="13">
@@ -1975,10 +1986,10 @@
         <v>61</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AD7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AE7" s="3" t="s">
         <v>11</v>
@@ -1992,10 +2003,10 @@
         <v>40837</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>100</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>101</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>11</v>
@@ -2013,28 +2024,28 @@
         <v>67</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O8" s="20">
         <v>40838</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="13">
@@ -2059,10 +2070,10 @@
         <v>57</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD8" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AE8" s="3" t="s">
         <v>12</v>
@@ -2076,10 +2087,10 @@
         <v>40837</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>103</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>11</v>
@@ -2097,28 +2108,28 @@
         <v>67</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O9" s="20">
         <v>40838</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R9" s="12"/>
       <c r="S9" s="13">
@@ -2143,10 +2154,10 @@
         <v>62</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AD9" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE9" s="3" t="s">
         <v>13</v>
@@ -2160,10 +2171,10 @@
         <v>40837</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>104</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>105</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>11</v>
@@ -2181,28 +2192,28 @@
         <v>67</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O10" s="20">
         <v>40838</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R10" s="12"/>
       <c r="S10" s="13">
@@ -2227,10 +2238,10 @@
         <v>63</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AE10" s="3" t="s">
         <v>14</v>
@@ -2244,10 +2255,10 @@
         <v>40837</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>11</v>
@@ -2265,28 +2276,28 @@
         <v>67</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O11" s="20">
         <v>40838</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R11" s="12"/>
       <c r="S11" s="13">
@@ -2308,10 +2319,10 @@
         <v>64</v>
       </c>
       <c r="AD11" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AE11" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF11" s="3" t="s">
         <v>25</v>
@@ -2322,10 +2333,10 @@
         <v>40837</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>11</v>
@@ -2343,28 +2354,28 @@
         <v>67</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O12" s="20">
         <v>40838</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R12" s="12"/>
       <c r="S12" s="13">
@@ -2386,7 +2397,7 @@
         <v>66</v>
       </c>
       <c r="AD12" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AE12" s="3" t="s">
         <v>16</v>
@@ -2400,10 +2411,10 @@
         <v>40837</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>11</v>
@@ -2421,28 +2432,28 @@
         <v>67</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M13" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="N13" s="12" t="s">
         <v>177</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>178</v>
       </c>
       <c r="O13" s="20">
         <v>40838</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13">
@@ -2464,13 +2475,13 @@
         <v>65</v>
       </c>
       <c r="AD13" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AE13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="AF13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="2:32" ht="36" customHeight="1">
@@ -2517,10 +2528,10 @@
         <v>40837</v>
       </c>
       <c r="C15" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>11</v>
@@ -2538,26 +2549,26 @@
         <v>67</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K15" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M15" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="L15" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="M15" s="12" t="s">
+      <c r="N15" s="12" t="s">
         <v>153</v>
-      </c>
-      <c r="N15" s="12" t="s">
-        <v>154</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q15" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="Q15" s="12" t="s">
-        <v>156</v>
       </c>
       <c r="R15" s="12" t="s">
         <v>24</v>
@@ -2577,7 +2588,7 @@
         <v>68</v>
       </c>
       <c r="AD15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AE15" s="3" t="s">
         <v>19</v>
@@ -2588,10 +2599,10 @@
         <v>40837</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>11</v>
@@ -2609,26 +2620,26 @@
         <v>67</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O16" s="12"/>
       <c r="P16" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R16" s="12" t="s">
         <v>24</v>
@@ -2642,10 +2653,10 @@
         <v>31</v>
       </c>
       <c r="AB16" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD16" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AE16" s="3" t="s">
         <v>20</v>
@@ -2656,10 +2667,10 @@
         <v>40837</v>
       </c>
       <c r="C17" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>113</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>114</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>11</v>
@@ -2677,26 +2688,26 @@
         <v>67</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K17" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M17" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="L17" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>160</v>
-      </c>
       <c r="N17" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q17" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R17" s="12" t="s">
         <v>24</v>
@@ -2713,7 +2724,7 @@
         <v>24</v>
       </c>
       <c r="AD17" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AE17" s="3" t="s">
         <v>21</v>
@@ -2724,10 +2735,10 @@
         <v>40837</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>11</v>
@@ -2745,26 +2756,26 @@
         <v>67</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O18" s="12"/>
       <c r="P18" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R18" s="12" t="s">
         <v>24</v>
@@ -2775,10 +2786,10 @@
         <v>39</v>
       </c>
       <c r="AB18" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AD18" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="2:31" ht="36.75" customHeight="1">
@@ -2786,10 +2797,10 @@
         <v>40837</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>11</v>
@@ -2807,29 +2818,29 @@
         <v>67</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q19" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="Q19" s="12" t="s">
-        <v>165</v>
-      </c>
       <c r="R19" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S19" s="13"/>
       <c r="T19" s="14"/>
@@ -2837,10 +2848,10 @@
         <v>36</v>
       </c>
       <c r="AB19" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AD19" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="2:31" ht="29.25" customHeight="1">
@@ -2848,10 +2859,10 @@
         <v>40837</v>
       </c>
       <c r="C20" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>118</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>119</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>11</v>
@@ -2869,26 +2880,26 @@
         <v>67</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R20" s="12" t="s">
         <v>24</v>
@@ -2907,10 +2918,10 @@
         <v>40837</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>11</v>
@@ -2928,29 +2939,29 @@
         <v>67</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K21" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="N21" s="12" t="s">
         <v>168</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="N21" s="12" t="s">
-        <v>169</v>
       </c>
       <c r="O21" s="12"/>
       <c r="P21" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q21" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R21" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S21" s="13"/>
       <c r="T21" s="14"/>
@@ -2966,10 +2977,10 @@
         <v>40837</v>
       </c>
       <c r="C22" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>121</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>122</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>11</v>
@@ -2987,29 +2998,29 @@
         <v>67</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K22" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="N22" s="12" t="s">
         <v>168</v>
-      </c>
-      <c r="L22" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="N22" s="12" t="s">
-        <v>169</v>
       </c>
       <c r="O22" s="12"/>
       <c r="P22" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q22" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R22" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S22" s="13"/>
       <c r="T22" s="14"/>
@@ -3022,10 +3033,10 @@
         <v>40837</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>11</v>
@@ -3043,29 +3054,29 @@
         <v>67</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K23" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="N23" s="12" t="s">
         <v>168</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="M23" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="N23" s="12" t="s">
-        <v>169</v>
       </c>
       <c r="O23" s="12"/>
       <c r="P23" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q23" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="Q23" s="12" t="s">
-        <v>173</v>
-      </c>
       <c r="R23" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S23" s="13"/>
       <c r="T23" s="14"/>
@@ -3078,10 +3089,10 @@
         <v>40837</v>
       </c>
       <c r="C24" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>124</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>125</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>11</v>
@@ -3099,29 +3110,29 @@
         <v>67</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K24" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="N24" s="12" t="s">
         <v>168</v>
-      </c>
-      <c r="L24" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="M24" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="N24" s="12" t="s">
-        <v>169</v>
       </c>
       <c r="O24" s="12"/>
       <c r="P24" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q24" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R24" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S24" s="13"/>
       <c r="T24" s="14"/>
@@ -3134,10 +3145,10 @@
         <v>40837</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>11</v>
@@ -3155,29 +3166,29 @@
         <v>67</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K25" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="N25" s="12" t="s">
         <v>168</v>
-      </c>
-      <c r="L25" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="N25" s="12" t="s">
-        <v>169</v>
       </c>
       <c r="O25" s="12"/>
       <c r="P25" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Q25" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R25" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S25" s="13"/>
       <c r="T25" s="14"/>
@@ -3185,43 +3196,79 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:31">
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
+    <row r="26" spans="2:31" ht="36.75" customHeight="1">
+      <c r="B26" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
+      <c r="P26" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q26" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="R26" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="S26" s="13"/>
       <c r="T26" s="14"/>
+      <c r="X26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="AB26" s="3" t="s">
-        <v>71</v>
+        <v>24</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE26" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="2:31">
-      <c r="B27" s="11">
-        <v>40837</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
@@ -3243,10 +3290,10 @@
         <v>40837</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>11</v>
@@ -3272,10 +3319,10 @@
         <v>40837</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>11</v>
@@ -3301,10 +3348,10 @@
         <v>40837</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>11</v>
@@ -3330,10 +3377,10 @@
         <v>40837</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>11</v>
@@ -3359,10 +3406,10 @@
         <v>40837</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>11</v>
@@ -3388,10 +3435,10 @@
         <v>40837</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>11</v>
@@ -3417,10 +3464,10 @@
         <v>40837</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>11</v>
@@ -3442,10 +3489,18 @@
       <c r="T34" s="14"/>
     </row>
     <row r="35" spans="2:20">
-      <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
+      <c r="B35" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -3841,51 +3896,72 @@
       <c r="T53" s="14"/>
     </row>
     <row r="54" spans="2:20">
-      <c r="B54" s="16"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
-      <c r="J54" s="17"/>
-      <c r="K54" s="17"/>
-      <c r="L54" s="17"/>
-      <c r="M54" s="17"/>
-      <c r="N54" s="17"/>
-      <c r="O54" s="17"/>
-      <c r="P54" s="17"/>
-      <c r="Q54" s="17"/>
-      <c r="R54" s="17"/>
-      <c r="S54" s="18"/>
-      <c r="T54" s="19"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+      <c r="O54" s="12"/>
+      <c r="P54" s="12"/>
+      <c r="Q54" s="12"/>
+      <c r="R54" s="12"/>
+      <c r="S54" s="13"/>
+      <c r="T54" s="14"/>
+    </row>
+    <row r="55" spans="2:20">
+      <c r="B55" s="16"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17"/>
+      <c r="R55" s="17"/>
+      <c r="S55" s="18"/>
+      <c r="T55" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="B4:T4"/>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E55">
       <formula1>$X$7:$X$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F55">
       <formula1>$Y$7:$Y$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G55">
       <formula1>$Z$7:$Z$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H55">
       <formula1>$AA$7:$AA$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I55">
       <formula1>$AB$7:$AB$26</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J55">
       <formula1>$AC$7:$AC$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L55">
       <formula1>$AD$7:$AD$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R55">
       <formula1>$AF$7:$AF$13</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
ThaoNX,KhoaVT,ThiVT,DungDV: update Defect Log.xlsx
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="8580"/>
@@ -11,7 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Defect Log'!$B$4:$T$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Defect Log'!$B$2:$T$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Defect Log'!$B$2:$T$103</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="240">
   <si>
     <t>Project Code:</t>
   </si>
@@ -872,30 +872,6 @@
   </si>
   <si>
     <t>MenuManager</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> database: dư Item Name checkbox"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> database: dư Item Namen cboSelectGroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> database: dư  Item Name cboSelectLogStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> database: dư  Item Name colTitle</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> database: dư  Item Name colType</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> database: dư  Item Name col#publish</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> database: dư  Item Name col#unpublish</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> database: dư Item Name colMenuItems</t>
   </si>
   <si>
     <t>Created Date (*)</t>
@@ -1071,16 +1047,187 @@
   </si>
   <si>
     <t>Bỏ text box name, sửa textbox login nam thành username ( sửa lại các phần : giao diện, definition items, mapping item to db, events có liên quan tới phần bị bỏ và bị sửa này).</t>
+  </si>
+  <si>
+    <t>MenuManager_Copy/Mapping Item to database: thiếu Type</t>
+  </si>
+  <si>
+    <t>SDD_MenuManager.xls, revision 116</t>
+  </si>
+  <si>
+    <t>ThaoNX</t>
+  </si>
+  <si>
+    <t>ThiVT</t>
+  </si>
+  <si>
+    <t>MenuManager_Copy/tbxTitile: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>MenuManager_Copy/tbxModuleName: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>MenuManager_Edit/Mapping Item to database: thiếu Type</t>
+  </si>
+  <si>
+    <t>MenuManager_Edit/tbxUniqueName: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>MenuManager_Edit/tbxDescription: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>MenuManager_Edit/tbxTitle: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>MenuManager_New/Mapping Item to database: thiếu Type</t>
+  </si>
+  <si>
+    <t>MenuManager_New/tbxUniqueName: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>MenuManager_New/tbxTitle: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>MenuManager_New/tbxDescription: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>MenuManager_New/tbxModuleName: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>CreatedMenu_Edit/Mapping Item to database: thiếu Type</t>
+  </si>
+  <si>
+    <t>CreatedMenu_Edit/tbxTitle: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>CreatedMenu_Edit/tbxLink: thiếu format, thiếu lenght, error check</t>
+  </si>
+  <si>
+    <t>CreatedMenus_New_NewMenuItem/Mapping Item to database: thiếu Type</t>
+  </si>
+  <si>
+    <t>CreatedMenus_New_NewMenuItem/tbxTitle: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>CreatedMenus_New_NewMenuItem/tbxAlias: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>CreatedMenus_New_NewMenuItem/tbxLink: thiếu format, thiếu lenght,error check</t>
+  </si>
+  <si>
+    <t>CreatedMenus_New_NewMenuItem/: thiếu format, thiếu lenght</t>
+  </si>
+  <si>
+    <t>Content/Menu Manager:   chưa có link</t>
+  </si>
+  <si>
+    <t>Content/Menu Trash:          chưa có link</t>
+  </si>
+  <si>
+    <t>Content: thiếu MenuManager_Copy link</t>
+  </si>
+  <si>
+    <t>Content: thiếu MenuManager_New link</t>
+  </si>
+  <si>
+    <t>Content: thiếu MenuManager_Edit link</t>
+  </si>
+  <si>
+    <t>Content: thiếu MenuTrash link</t>
+  </si>
+  <si>
+    <t>Content : thiếu CreatedMenu_Copy  link</t>
+  </si>
+  <si>
+    <t>Content : thiếu CreatedMenus link</t>
+  </si>
+  <si>
+    <t>Content : thiếu CreatedMenu_Move  link</t>
+  </si>
+  <si>
+    <t>Content : thiếu CreatedMenus_New_NewMenuItem  link</t>
+  </si>
+  <si>
+    <t>Content : thiếu CreatedMenu_New_SeclectType  link</t>
+  </si>
+  <si>
+    <t>thiếu RECORD OF CHANGES</t>
+  </si>
+  <si>
+    <t>SDD_UserManager.xls, revision 120</t>
+  </si>
+  <si>
+    <t>KhoaVT</t>
+  </si>
+  <si>
+    <t>User Manager</t>
+  </si>
+  <si>
+    <t>database: Chưa map item colName tới CSDL người dùng</t>
+  </si>
+  <si>
+    <t>database: Chưa map item colUserName tới CSDL người dùng</t>
+  </si>
+  <si>
+    <t>database: Chưa map item colLoggedIn tới CSDL người dùng</t>
+  </si>
+  <si>
+    <t>database: Chưa map item colEnable tới CSDL người dùng</t>
+  </si>
+  <si>
+    <t>database: Chưa map item colGroup tới CSDL người dùng</t>
+  </si>
+  <si>
+    <t>database: Chưa map item colEmail tới CSDL người dùng</t>
+  </si>
+  <si>
+    <t>database: Chưa map item colLastVisted tới CSDL người dùng</t>
+  </si>
+  <si>
+    <t>database: Item cboSelectGroup không cần map tới CSDL</t>
+  </si>
+  <si>
+    <t>database: Item cbocboSelectLogStatus không cần map tới CSDL</t>
+  </si>
+  <si>
+    <t>Configuration Global</t>
+  </si>
+  <si>
+    <t>Item ttdFtpPassword: Thiếu error check các ký tự đặc biệt trong mật khẩu</t>
+  </si>
+  <si>
+    <t>SDD_GlobalConfiguration.xlsx</t>
+  </si>
+  <si>
+    <t>Section Manager</t>
+  </si>
+  <si>
+    <t>database: Item GirdView không cần map tới CSDL vì đã map từng trường</t>
+  </si>
+  <si>
+    <t>SDD_ContentManager_DungDV.xlsx</t>
+  </si>
+  <si>
+    <t>DungDV</t>
+  </si>
+  <si>
+    <t>database: Item colCatagory không map tới bảng Section mà lấy từ bảng Section_Catagory</t>
+  </si>
+  <si>
+    <t>Catagory Manager</t>
+  </si>
+  <si>
+    <t>Font Page Manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1129,6 +1276,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1144,7 +1297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1278,11 +1431,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1343,6 +1507,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1433,6 +1600,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1467,6 +1635,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1642,14 +1811,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AF55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AF103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="E61" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -1685,12 +1854,12 @@
     <col min="33" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32">
+    <row r="1" spans="2:32" x14ac:dyDescent="0.25">
       <c r="R1" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="2:32" ht="30">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1699,18 +1868,18 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1">
+    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>1</v>
@@ -1719,31 +1888,31 @@
         <v>2</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>7</v>
@@ -1752,10 +1921,10 @@
         <v>9</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="W4" s="4" t="s">
         <v>92</v>
@@ -1770,7 +1939,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="2:32" ht="45">
+    <row r="5" spans="2:32" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
         <v>40837</v>
       </c>
@@ -1799,25 +1968,25 @@
         <v>75</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="O5" s="20">
         <v>40838</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="13">
@@ -1827,7 +1996,7 @@
         <v>40838</v>
       </c>
     </row>
-    <row r="6" spans="2:32" ht="45">
+    <row r="6" spans="2:32" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>40837</v>
       </c>
@@ -1856,25 +2025,25 @@
         <v>75</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="O6" s="20">
         <v>40838</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="R6" s="12"/>
       <c r="S6" s="13">
@@ -1914,7 +2083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:32" ht="30">
+    <row r="7" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>40837</v>
       </c>
@@ -1943,25 +2112,25 @@
         <v>75</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="O7" s="20">
         <v>40838</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="13">
@@ -1998,7 +2167,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:32" ht="30">
+    <row r="8" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>40837</v>
       </c>
@@ -2027,25 +2196,25 @@
         <v>75</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="O8" s="20">
         <v>40838</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="13">
@@ -2082,7 +2251,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:32" ht="30">
+    <row r="9" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>40837</v>
       </c>
@@ -2111,25 +2280,25 @@
         <v>75</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="O9" s="20">
         <v>40838</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="R9" s="12"/>
       <c r="S9" s="13">
@@ -2166,7 +2335,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:32" ht="30">
+    <row r="10" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
         <v>40837</v>
       </c>
@@ -2195,25 +2364,25 @@
         <v>75</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="O10" s="20">
         <v>40838</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="R10" s="12"/>
       <c r="S10" s="13">
@@ -2250,7 +2419,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:32" ht="30">
+    <row r="11" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <v>40837</v>
       </c>
@@ -2279,25 +2448,25 @@
         <v>75</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="L11" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="O11" s="20">
         <v>40838</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="R11" s="12"/>
       <c r="S11" s="13">
@@ -2328,7 +2497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:32" ht="30">
+    <row r="12" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <v>40837</v>
       </c>
@@ -2357,25 +2526,25 @@
         <v>75</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="O12" s="20">
         <v>40838</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="R12" s="12"/>
       <c r="S12" s="13">
@@ -2406,7 +2575,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:32" ht="30">
+    <row r="13" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>40837</v>
       </c>
@@ -2435,25 +2604,25 @@
         <v>75</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="O13" s="20">
         <v>40838</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13">
@@ -2484,7 +2653,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="2:32" ht="36" customHeight="1">
+    <row r="14" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -2523,7 +2692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:32" ht="60">
+    <row r="15" spans="2:32" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
         <v>40837</v>
       </c>
@@ -2552,23 +2721,23 @@
         <v>75</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="12" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="Q15" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="R15" s="12" t="s">
         <v>24</v>
@@ -2594,7 +2763,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:32" ht="36" customHeight="1">
+    <row r="16" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <v>40837</v>
       </c>
@@ -2623,23 +2792,23 @@
         <v>75</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="O16" s="12"/>
       <c r="P16" s="12" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="R16" s="12" t="s">
         <v>24</v>
@@ -2662,7 +2831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:31" ht="47.25" customHeight="1">
+    <row r="17" spans="2:31" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>40837</v>
       </c>
@@ -2691,23 +2860,23 @@
         <v>75</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="Q17" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="R17" s="12" t="s">
         <v>24</v>
@@ -2730,7 +2899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:31" ht="30">
+    <row r="18" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
         <v>40837</v>
       </c>
@@ -2759,23 +2928,23 @@
         <v>76</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="L18" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="O18" s="12"/>
       <c r="P18" s="12" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="R18" s="12" t="s">
         <v>24</v>
@@ -2792,7 +2961,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="2:31" ht="36.75" customHeight="1">
+    <row r="19" spans="2:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
         <v>40837</v>
       </c>
@@ -2821,23 +2990,23 @@
         <v>76</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="L19" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="Q19" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="R19" s="12" t="s">
         <v>91</v>
@@ -2854,7 +3023,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="2:31" ht="29.25" customHeight="1">
+    <row r="20" spans="2:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <v>40837</v>
       </c>
@@ -2883,23 +3052,23 @@
         <v>76</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="R20" s="12" t="s">
         <v>24</v>
@@ -2913,7 +3082,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:31" ht="33" customHeight="1">
+    <row r="21" spans="2:31" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
         <v>40837</v>
       </c>
@@ -2942,23 +3111,23 @@
         <v>75</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="L21" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="O21" s="12"/>
       <c r="P21" s="12" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="Q21" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="R21" s="12" t="s">
         <v>91</v>
@@ -2972,7 +3141,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:31" ht="30">
+    <row r="22" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <v>40837</v>
       </c>
@@ -3001,23 +3170,23 @@
         <v>76</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="L22" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="O22" s="12"/>
       <c r="P22" s="12" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="Q22" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="R22" s="12" t="s">
         <v>91</v>
@@ -3028,7 +3197,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="2:31" ht="37.5" customHeight="1">
+    <row r="23" spans="2:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
         <v>40837</v>
       </c>
@@ -3057,23 +3226,23 @@
         <v>76</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="L23" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="O23" s="12"/>
       <c r="P23" s="12" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="Q23" s="12" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="R23" s="12" t="s">
         <v>91</v>
@@ -3084,7 +3253,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:31" ht="43.5" customHeight="1">
+    <row r="24" spans="2:31" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <v>40837</v>
       </c>
@@ -3113,23 +3282,23 @@
         <v>77</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="L24" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="O24" s="12"/>
       <c r="P24" s="12" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="Q24" s="12" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="R24" s="12" t="s">
         <v>91</v>
@@ -3140,7 +3309,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:31" ht="30">
+    <row r="25" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
         <v>40837</v>
       </c>
@@ -3169,23 +3338,23 @@
         <v>75</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="O25" s="12"/>
       <c r="P25" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="Q25" s="12" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="R25" s="12" t="s">
         <v>91</v>
@@ -3196,7 +3365,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:31" ht="36.75" customHeight="1">
+    <row r="26" spans="2:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <v>40837</v>
       </c>
@@ -3204,7 +3373,7 @@
         <v>112</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>11</v>
@@ -3225,23 +3394,23 @@
         <v>75</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>83</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="O26" s="12"/>
       <c r="P26" s="12" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="Q26" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="R26" s="12" t="s">
         <v>24</v>
@@ -3264,7 +3433,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:31">
+    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -3285,94 +3454,130 @@
       <c r="S27" s="13"/>
       <c r="T27" s="14"/>
     </row>
-    <row r="28" spans="2:31">
+    <row r="28" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
         <v>40837</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>129</v>
+        <v>183</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
+      <c r="H28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
+      <c r="K28" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
+      <c r="M28" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O28" s="20"/>
       <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
+      <c r="Q28" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R28" s="12"/>
       <c r="S28" s="13"/>
       <c r="T28" s="14"/>
     </row>
-    <row r="29" spans="2:31">
+    <row r="29" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
         <v>40837</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
+      <c r="H29" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
+      <c r="K29" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
+      <c r="M29" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O29" s="20"/>
       <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
+      <c r="Q29" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R29" s="12"/>
       <c r="S29" s="13"/>
       <c r="T29" s="14"/>
     </row>
-    <row r="30" spans="2:31">
+    <row r="30" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
         <v>40837</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
+      <c r="H30" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
+      <c r="K30" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
+      <c r="M30" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O30" s="20"/>
       <c r="P30" s="12"/>
-      <c r="Q30" s="12"/>
+      <c r="Q30" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R30" s="12"/>
       <c r="S30" s="13"/>
       <c r="T30" s="14"/>
     </row>
-    <row r="31" spans="2:31">
+    <row r="31" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
         <v>40837</v>
       </c>
@@ -3380,28 +3585,40 @@
         <v>128</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>132</v>
+        <v>188</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
+      <c r="H31" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
+      <c r="K31" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
+      <c r="M31" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O31" s="20"/>
       <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
+      <c r="Q31" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R31" s="12"/>
       <c r="S31" s="13"/>
       <c r="T31" s="14"/>
     </row>
-    <row r="32" spans="2:31">
+    <row r="32" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
         <v>40837</v>
       </c>
@@ -3409,28 +3626,40 @@
         <v>128</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>133</v>
+        <v>189</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
+      <c r="H32" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
+      <c r="K32" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
+      <c r="M32" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O32" s="20"/>
       <c r="P32" s="12"/>
-      <c r="Q32" s="12"/>
+      <c r="Q32" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R32" s="12"/>
       <c r="S32" s="13"/>
       <c r="T32" s="14"/>
     </row>
-    <row r="33" spans="2:20">
+    <row r="33" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
         <v>40837</v>
       </c>
@@ -3438,28 +3667,40 @@
         <v>128</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>134</v>
+        <v>190</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
+      <c r="H33" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
+      <c r="K33" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
+      <c r="M33" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O33" s="20"/>
       <c r="P33" s="12"/>
-      <c r="Q33" s="12"/>
+      <c r="Q33" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R33" s="12"/>
       <c r="S33" s="13"/>
       <c r="T33" s="14"/>
     </row>
-    <row r="34" spans="2:20">
+    <row r="34" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
         <v>40837</v>
       </c>
@@ -3467,28 +3708,40 @@
         <v>128</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>135</v>
+        <v>191</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
+      <c r="H34" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
+      <c r="K34" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
+      <c r="M34" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O34" s="20"/>
       <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
+      <c r="Q34" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R34" s="12"/>
       <c r="S34" s="13"/>
       <c r="T34" s="14"/>
     </row>
-    <row r="35" spans="2:20">
+    <row r="35" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
         <v>40837</v>
       </c>
@@ -3496,473 +3749,2440 @@
         <v>128</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>136</v>
+        <v>192</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
+      <c r="H35" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
+      <c r="K35" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
+      <c r="M35" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O35" s="20"/>
       <c r="P35" s="12"/>
-      <c r="Q35" s="12"/>
+      <c r="Q35" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R35" s="12"/>
       <c r="S35" s="13"/>
       <c r="T35" s="14"/>
     </row>
-    <row r="36" spans="2:20">
-      <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
+    <row r="36" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
+      <c r="H36" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
+      <c r="K36" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
+      <c r="M36" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O36" s="20"/>
       <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
+      <c r="Q36" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R36" s="12"/>
       <c r="S36" s="13"/>
       <c r="T36" s="14"/>
     </row>
-    <row r="37" spans="2:20">
-      <c r="B37" s="11"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
+    <row r="37" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
+      <c r="H37" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
+      <c r="K37" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
+      <c r="M37" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O37" s="20"/>
       <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
+      <c r="Q37" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R37" s="12"/>
       <c r="S37" s="13"/>
       <c r="T37" s="14"/>
     </row>
-    <row r="38" spans="2:20">
-      <c r="B38" s="11"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
+    <row r="38" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
+      <c r="H38" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
+      <c r="K38" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
+      <c r="M38" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O38" s="20"/>
       <c r="P38" s="12"/>
-      <c r="Q38" s="12"/>
+      <c r="Q38" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R38" s="12"/>
       <c r="S38" s="13"/>
       <c r="T38" s="14"/>
     </row>
-    <row r="39" spans="2:20">
-      <c r="B39" s="11"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
+    <row r="39" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
+      <c r="H39" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
+      <c r="K39" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
+      <c r="M39" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O39" s="20"/>
       <c r="P39" s="12"/>
-      <c r="Q39" s="12"/>
+      <c r="Q39" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R39" s="12"/>
       <c r="S39" s="13"/>
       <c r="T39" s="14"/>
     </row>
-    <row r="40" spans="2:20">
-      <c r="B40" s="11"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
+    <row r="40" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
+      <c r="H40" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
+      <c r="K40" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
-      <c r="O40" s="12"/>
+      <c r="M40" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O40" s="20"/>
       <c r="P40" s="12"/>
-      <c r="Q40" s="12"/>
+      <c r="Q40" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R40" s="12"/>
       <c r="S40" s="13"/>
       <c r="T40" s="14"/>
     </row>
-    <row r="41" spans="2:20">
-      <c r="B41" s="11"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
+    <row r="41" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
+      <c r="H41" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
+      <c r="K41" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
+      <c r="M41" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N41" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O41" s="20"/>
       <c r="P41" s="12"/>
-      <c r="Q41" s="12"/>
+      <c r="Q41" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R41" s="12"/>
       <c r="S41" s="13"/>
       <c r="T41" s="14"/>
     </row>
-    <row r="42" spans="2:20">
-      <c r="B42" s="11"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
+    <row r="42" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
+      <c r="H42" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
+      <c r="K42" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
-      <c r="O42" s="12"/>
+      <c r="M42" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O42" s="20"/>
       <c r="P42" s="12"/>
-      <c r="Q42" s="12"/>
+      <c r="Q42" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R42" s="12"/>
       <c r="S42" s="13"/>
       <c r="T42" s="14"/>
     </row>
-    <row r="43" spans="2:20">
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
+    <row r="43" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
+      <c r="H43" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
+      <c r="K43" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
+      <c r="M43" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O43" s="20"/>
       <c r="P43" s="12"/>
-      <c r="Q43" s="12"/>
+      <c r="Q43" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R43" s="12"/>
       <c r="S43" s="13"/>
       <c r="T43" s="14"/>
     </row>
-    <row r="44" spans="2:20">
-      <c r="B44" s="11"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
+    <row r="44" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
+      <c r="H44" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
+      <c r="K44" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
+      <c r="M44" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O44" s="20"/>
       <c r="P44" s="12"/>
-      <c r="Q44" s="12"/>
+      <c r="Q44" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R44" s="12"/>
       <c r="S44" s="13"/>
       <c r="T44" s="14"/>
     </row>
-    <row r="45" spans="2:20">
-      <c r="B45" s="11"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
+    <row r="45" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
+      <c r="H45" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
+      <c r="K45" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
+      <c r="M45" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O45" s="20"/>
       <c r="P45" s="12"/>
-      <c r="Q45" s="12"/>
+      <c r="Q45" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R45" s="12"/>
       <c r="S45" s="13"/>
       <c r="T45" s="14"/>
     </row>
-    <row r="46" spans="2:20">
-      <c r="B46" s="11"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
+    <row r="46" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
+      <c r="H46" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J46" s="12"/>
-      <c r="K46" s="12"/>
+      <c r="K46" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-      <c r="O46" s="12"/>
+      <c r="M46" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O46" s="20"/>
       <c r="P46" s="12"/>
-      <c r="Q46" s="12"/>
+      <c r="Q46" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R46" s="12"/>
       <c r="S46" s="13"/>
       <c r="T46" s="14"/>
     </row>
-    <row r="47" spans="2:20">
-      <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
+    <row r="47" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
+      <c r="H47" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J47" s="12"/>
-      <c r="K47" s="12"/>
+      <c r="K47" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-      <c r="O47" s="12"/>
+      <c r="M47" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N47" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O47" s="20"/>
       <c r="P47" s="12"/>
-      <c r="Q47" s="12"/>
+      <c r="Q47" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R47" s="12"/>
       <c r="S47" s="13"/>
       <c r="T47" s="14"/>
     </row>
-    <row r="48" spans="2:20">
-      <c r="B48" s="11"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
+    <row r="48" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
+      <c r="H48" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J48" s="12"/>
-      <c r="K48" s="12"/>
+      <c r="K48" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
-      <c r="O48" s="12"/>
+      <c r="M48" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O48" s="20"/>
       <c r="P48" s="12"/>
-      <c r="Q48" s="12"/>
+      <c r="Q48" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R48" s="12"/>
       <c r="S48" s="13"/>
       <c r="T48" s="14"/>
     </row>
-    <row r="49" spans="2:20">
-      <c r="B49" s="11"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
+    <row r="49" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
+      <c r="H49" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J49" s="12"/>
-      <c r="K49" s="12"/>
+      <c r="K49" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L49" s="12"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-      <c r="O49" s="12"/>
+      <c r="M49" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O49" s="20"/>
       <c r="P49" s="12"/>
-      <c r="Q49" s="12"/>
+      <c r="Q49" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R49" s="12"/>
       <c r="S49" s="13"/>
       <c r="T49" s="14"/>
     </row>
-    <row r="50" spans="2:20">
-      <c r="B50" s="11"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
+    <row r="50" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
+      <c r="H50" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J50" s="12"/>
-      <c r="K50" s="12"/>
+      <c r="K50" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L50" s="12"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-      <c r="O50" s="12"/>
+      <c r="M50" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N50" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O50" s="20"/>
       <c r="P50" s="12"/>
-      <c r="Q50" s="12"/>
+      <c r="Q50" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R50" s="12"/>
       <c r="S50" s="13"/>
       <c r="T50" s="14"/>
     </row>
-    <row r="51" spans="2:20">
-      <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
+    <row r="51" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
+      <c r="H51" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J51" s="12"/>
-      <c r="K51" s="12"/>
+      <c r="K51" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L51" s="12"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="12"/>
+      <c r="M51" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O51" s="20"/>
       <c r="P51" s="12"/>
-      <c r="Q51" s="12"/>
+      <c r="Q51" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R51" s="12"/>
       <c r="S51" s="13"/>
       <c r="T51" s="14"/>
     </row>
-    <row r="52" spans="2:20">
-      <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
+    <row r="52" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
+      <c r="H52" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J52" s="12"/>
-      <c r="K52" s="12"/>
+      <c r="K52" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L52" s="12"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
-      <c r="O52" s="12"/>
+      <c r="M52" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O52" s="20"/>
       <c r="P52" s="12"/>
-      <c r="Q52" s="12"/>
+      <c r="Q52" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R52" s="12"/>
       <c r="S52" s="13"/>
       <c r="T52" s="14"/>
     </row>
-    <row r="53" spans="2:20">
-      <c r="B53" s="11"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
+    <row r="53" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
+      <c r="H53" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
+      <c r="K53" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-      <c r="O53" s="12"/>
+      <c r="M53" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N53" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O53" s="20"/>
       <c r="P53" s="12"/>
-      <c r="Q53" s="12"/>
+      <c r="Q53" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R53" s="12"/>
       <c r="S53" s="13"/>
       <c r="T53" s="14"/>
     </row>
-    <row r="54" spans="2:20">
-      <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
+    <row r="54" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
+      <c r="H54" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
+      <c r="K54" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L54" s="12"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-      <c r="O54" s="12"/>
+      <c r="M54" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N54" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O54" s="20"/>
       <c r="P54" s="12"/>
-      <c r="Q54" s="12"/>
+      <c r="Q54" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R54" s="12"/>
       <c r="S54" s="13"/>
       <c r="T54" s="14"/>
     </row>
-    <row r="55" spans="2:20">
-      <c r="B55" s="16"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17"/>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="17"/>
-      <c r="O55" s="17"/>
-      <c r="P55" s="17"/>
-      <c r="Q55" s="17"/>
-      <c r="R55" s="17"/>
-      <c r="S55" s="18"/>
-      <c r="T55" s="19"/>
+    <row r="55" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B55" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N55" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O55" s="20"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R55" s="12"/>
+      <c r="S55" s="13"/>
+      <c r="T55" s="14"/>
+    </row>
+    <row r="56" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N56" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O56" s="20"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R56" s="12"/>
+      <c r="S56" s="13"/>
+      <c r="T56" s="14"/>
+    </row>
+    <row r="57" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B57" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L57" s="12"/>
+      <c r="M57" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O57" s="20"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R57" s="12"/>
+      <c r="S57" s="13"/>
+      <c r="T57" s="14"/>
+    </row>
+    <row r="58" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L58" s="12"/>
+      <c r="M58" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N58" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O58" s="20"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R58" s="12"/>
+      <c r="S58" s="13"/>
+      <c r="T58" s="14"/>
+    </row>
+    <row r="59" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L59" s="12"/>
+      <c r="M59" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N59" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O59" s="20"/>
+      <c r="P59" s="12"/>
+      <c r="Q59" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R59" s="12"/>
+      <c r="S59" s="13"/>
+      <c r="T59" s="14"/>
+    </row>
+    <row r="60" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B60" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N60" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O60" s="20"/>
+      <c r="P60" s="12"/>
+      <c r="Q60" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R60" s="12"/>
+      <c r="S60" s="13"/>
+      <c r="T60" s="14"/>
+    </row>
+    <row r="61" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B61" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="L61" s="12"/>
+      <c r="M61" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="N61" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O61" s="20"/>
+      <c r="P61" s="12"/>
+      <c r="Q61" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R61" s="12"/>
+      <c r="S61" s="13"/>
+      <c r="T61" s="14"/>
+    </row>
+    <row r="62" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B62" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L62" s="12"/>
+      <c r="M62" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N62" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O62" s="20"/>
+      <c r="P62" s="12"/>
+      <c r="Q62" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R62" s="12"/>
+      <c r="S62" s="13"/>
+      <c r="T62" s="14"/>
+      <c r="U62"/>
+      <c r="V62"/>
+      <c r="W62"/>
+      <c r="X62"/>
+      <c r="Y62"/>
+      <c r="Z62"/>
+      <c r="AA62"/>
+      <c r="AB62"/>
+      <c r="AC62"/>
+      <c r="AD62"/>
+      <c r="AE62"/>
+      <c r="AF62"/>
+    </row>
+    <row r="63" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B63" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L63" s="12"/>
+      <c r="M63" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N63" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O63" s="20"/>
+      <c r="P63" s="12"/>
+      <c r="Q63" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R63" s="12"/>
+      <c r="S63" s="13"/>
+      <c r="T63" s="14"/>
+      <c r="U63"/>
+      <c r="V63"/>
+      <c r="W63"/>
+      <c r="X63"/>
+      <c r="Y63"/>
+      <c r="Z63"/>
+      <c r="AA63"/>
+      <c r="AB63"/>
+      <c r="AC63"/>
+      <c r="AD63"/>
+      <c r="AE63"/>
+      <c r="AF63"/>
+    </row>
+    <row r="64" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B64" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L64" s="12"/>
+      <c r="M64" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N64" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O64" s="20"/>
+      <c r="P64" s="12"/>
+      <c r="Q64" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R64" s="12"/>
+      <c r="S64" s="13"/>
+      <c r="T64" s="14"/>
+      <c r="U64"/>
+      <c r="V64"/>
+      <c r="W64"/>
+      <c r="X64"/>
+      <c r="Y64"/>
+      <c r="Z64"/>
+      <c r="AA64"/>
+      <c r="AB64"/>
+      <c r="AC64"/>
+      <c r="AD64"/>
+      <c r="AE64"/>
+      <c r="AF64"/>
+    </row>
+    <row r="65" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B65" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I65" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N65" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O65" s="20"/>
+      <c r="P65" s="12"/>
+      <c r="Q65" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R65" s="12"/>
+      <c r="S65" s="13"/>
+      <c r="T65" s="14"/>
+      <c r="U65"/>
+      <c r="V65"/>
+      <c r="W65"/>
+      <c r="X65"/>
+      <c r="Y65"/>
+      <c r="Z65"/>
+      <c r="AA65"/>
+      <c r="AB65"/>
+      <c r="AC65"/>
+      <c r="AD65"/>
+      <c r="AE65"/>
+      <c r="AF65"/>
+    </row>
+    <row r="66" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B66" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I66" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L66" s="12"/>
+      <c r="M66" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N66" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O66" s="12"/>
+      <c r="P66" s="12"/>
+      <c r="Q66" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R66" s="12"/>
+      <c r="S66" s="13"/>
+      <c r="T66" s="14"/>
+      <c r="U66"/>
+      <c r="V66"/>
+      <c r="W66"/>
+      <c r="X66"/>
+      <c r="Y66"/>
+      <c r="Z66"/>
+      <c r="AA66"/>
+      <c r="AB66"/>
+      <c r="AC66"/>
+      <c r="AD66"/>
+      <c r="AE66"/>
+      <c r="AF66"/>
+    </row>
+    <row r="67" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B67" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L67" s="12"/>
+      <c r="M67" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N67" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O67" s="12"/>
+      <c r="P67" s="12"/>
+      <c r="Q67" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R67" s="12"/>
+      <c r="S67" s="13"/>
+      <c r="T67" s="14"/>
+      <c r="U67"/>
+      <c r="V67"/>
+      <c r="W67"/>
+      <c r="X67"/>
+      <c r="Y67"/>
+      <c r="Z67"/>
+      <c r="AA67"/>
+      <c r="AB67"/>
+      <c r="AC67"/>
+      <c r="AD67"/>
+      <c r="AE67"/>
+      <c r="AF67"/>
+    </row>
+    <row r="68" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B68" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I68" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L68" s="12"/>
+      <c r="M68" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N68" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O68" s="12"/>
+      <c r="P68" s="12"/>
+      <c r="Q68" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R68" s="12"/>
+      <c r="S68" s="13"/>
+      <c r="T68" s="14"/>
+      <c r="U68"/>
+      <c r="V68"/>
+      <c r="W68"/>
+      <c r="X68"/>
+      <c r="Y68"/>
+      <c r="Z68"/>
+      <c r="AA68"/>
+      <c r="AB68"/>
+      <c r="AC68"/>
+      <c r="AD68"/>
+      <c r="AE68"/>
+      <c r="AF68"/>
+    </row>
+    <row r="69" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B69" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L69" s="12"/>
+      <c r="M69" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N69" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O69" s="12"/>
+      <c r="P69" s="12"/>
+      <c r="Q69" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R69" s="12"/>
+      <c r="S69" s="13"/>
+      <c r="T69" s="14"/>
+      <c r="U69"/>
+      <c r="V69"/>
+      <c r="W69"/>
+      <c r="X69"/>
+      <c r="Y69"/>
+      <c r="Z69"/>
+      <c r="AA69"/>
+      <c r="AB69"/>
+      <c r="AC69"/>
+      <c r="AD69"/>
+      <c r="AE69"/>
+      <c r="AF69"/>
+    </row>
+    <row r="70" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B70" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I70" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L70" s="12"/>
+      <c r="M70" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N70" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O70" s="12"/>
+      <c r="P70" s="12"/>
+      <c r="Q70" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R70" s="12"/>
+      <c r="S70" s="13"/>
+      <c r="T70" s="14"/>
+      <c r="U70"/>
+      <c r="V70"/>
+      <c r="W70"/>
+      <c r="X70"/>
+      <c r="Y70"/>
+      <c r="Z70"/>
+      <c r="AA70"/>
+      <c r="AB70"/>
+      <c r="AC70"/>
+      <c r="AD70"/>
+      <c r="AE70"/>
+      <c r="AF70"/>
+    </row>
+    <row r="71" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B71" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I71" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="L71" s="12"/>
+      <c r="M71" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N71" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="O71" s="12"/>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R71" s="12"/>
+      <c r="S71" s="13"/>
+      <c r="T71" s="14"/>
+      <c r="U71"/>
+      <c r="V71"/>
+      <c r="W71"/>
+      <c r="X71"/>
+      <c r="Y71"/>
+      <c r="Z71"/>
+      <c r="AA71"/>
+      <c r="AB71"/>
+      <c r="AC71"/>
+      <c r="AD71"/>
+      <c r="AE71"/>
+      <c r="AF71"/>
+    </row>
+    <row r="72" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B72" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I72" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="L72" s="12"/>
+      <c r="M72" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N72" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="O72" s="12"/>
+      <c r="P72" s="12"/>
+      <c r="Q72" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R72" s="12"/>
+      <c r="S72" s="13"/>
+      <c r="T72" s="14"/>
+      <c r="U72"/>
+      <c r="V72"/>
+      <c r="W72"/>
+      <c r="X72"/>
+      <c r="Y72"/>
+      <c r="Z72"/>
+      <c r="AA72"/>
+      <c r="AB72"/>
+      <c r="AC72"/>
+      <c r="AD72"/>
+      <c r="AE72"/>
+      <c r="AF72"/>
+    </row>
+    <row r="73" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B73" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="D73" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I73" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J73" s="12"/>
+      <c r="K73" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="L73" s="12"/>
+      <c r="M73" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N73" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="O73" s="12"/>
+      <c r="P73" s="12"/>
+      <c r="Q73" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R73" s="12"/>
+      <c r="S73" s="13"/>
+      <c r="T73" s="14"/>
+      <c r="U73"/>
+      <c r="V73"/>
+      <c r="W73"/>
+      <c r="X73"/>
+      <c r="Y73"/>
+      <c r="Z73"/>
+      <c r="AA73"/>
+      <c r="AB73"/>
+      <c r="AC73"/>
+      <c r="AD73"/>
+      <c r="AE73"/>
+      <c r="AF73"/>
+    </row>
+    <row r="74" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B74" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I74" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="L74" s="12"/>
+      <c r="M74" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N74" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="O74" s="12"/>
+      <c r="P74" s="12"/>
+      <c r="Q74" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R74" s="12"/>
+      <c r="S74" s="13"/>
+      <c r="T74" s="14"/>
+    </row>
+    <row r="75" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B75" s="11">
+        <v>40837</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I75" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J75" s="12"/>
+      <c r="K75" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="L75" s="12"/>
+      <c r="M75" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="N75" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="O75" s="12"/>
+      <c r="P75" s="12"/>
+      <c r="Q75" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R75" s="12"/>
+      <c r="S75" s="13"/>
+      <c r="T75" s="14"/>
+    </row>
+    <row r="76" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B76" s="11"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12"/>
+      <c r="M76" s="12"/>
+      <c r="N76" s="12"/>
+      <c r="O76" s="12"/>
+      <c r="P76" s="12"/>
+      <c r="Q76" s="12"/>
+      <c r="R76" s="12"/>
+      <c r="S76" s="13"/>
+      <c r="T76" s="14"/>
+    </row>
+    <row r="77" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B77" s="11"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="12"/>
+      <c r="K77" s="12"/>
+      <c r="L77" s="12"/>
+      <c r="M77" s="12"/>
+      <c r="N77" s="12"/>
+      <c r="O77" s="12"/>
+      <c r="P77" s="12"/>
+      <c r="Q77" s="12"/>
+      <c r="R77" s="12"/>
+      <c r="S77" s="13"/>
+      <c r="T77" s="14"/>
+    </row>
+    <row r="78" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B78" s="11"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="12"/>
+      <c r="K78" s="12"/>
+      <c r="L78" s="12"/>
+      <c r="M78" s="12"/>
+      <c r="N78" s="12"/>
+      <c r="O78" s="12"/>
+      <c r="P78" s="12"/>
+      <c r="Q78" s="12"/>
+      <c r="R78" s="12"/>
+      <c r="S78" s="13"/>
+      <c r="T78" s="14"/>
+    </row>
+    <row r="79" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B79" s="11"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
+      <c r="K79" s="12"/>
+      <c r="L79" s="12"/>
+      <c r="M79" s="12"/>
+      <c r="N79" s="12"/>
+      <c r="O79" s="12"/>
+      <c r="P79" s="12"/>
+      <c r="Q79" s="12"/>
+      <c r="R79" s="12"/>
+      <c r="S79" s="13"/>
+      <c r="T79" s="14"/>
+    </row>
+    <row r="80" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B80" s="11"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="12"/>
+      <c r="K80" s="12"/>
+      <c r="L80" s="12"/>
+      <c r="M80" s="12"/>
+      <c r="N80" s="12"/>
+      <c r="O80" s="12"/>
+      <c r="P80" s="12"/>
+      <c r="Q80" s="12"/>
+      <c r="R80" s="12"/>
+      <c r="S80" s="13"/>
+      <c r="T80" s="14"/>
+    </row>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B81" s="11"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="12"/>
+      <c r="K81" s="12"/>
+      <c r="L81" s="12"/>
+      <c r="M81" s="12"/>
+      <c r="N81" s="12"/>
+      <c r="O81" s="12"/>
+      <c r="P81" s="12"/>
+      <c r="Q81" s="12"/>
+      <c r="R81" s="12"/>
+      <c r="S81" s="13"/>
+      <c r="T81" s="14"/>
+    </row>
+    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B82" s="11"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="12"/>
+      <c r="K82" s="12"/>
+      <c r="L82" s="12"/>
+      <c r="M82" s="12"/>
+      <c r="N82" s="12"/>
+      <c r="O82" s="12"/>
+      <c r="P82" s="12"/>
+      <c r="Q82" s="12"/>
+      <c r="R82" s="12"/>
+      <c r="S82" s="13"/>
+      <c r="T82" s="14"/>
+    </row>
+    <row r="83" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B83" s="11"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="12"/>
+      <c r="K83" s="12"/>
+      <c r="L83" s="12"/>
+      <c r="M83" s="12"/>
+      <c r="N83" s="12"/>
+      <c r="O83" s="12"/>
+      <c r="P83" s="12"/>
+      <c r="Q83" s="12"/>
+      <c r="R83" s="12"/>
+      <c r="S83" s="13"/>
+      <c r="T83" s="14"/>
+    </row>
+    <row r="84" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B84" s="11"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
+      <c r="L84" s="12"/>
+      <c r="M84" s="12"/>
+      <c r="N84" s="12"/>
+      <c r="O84" s="12"/>
+      <c r="P84" s="12"/>
+      <c r="Q84" s="12"/>
+      <c r="R84" s="12"/>
+      <c r="S84" s="13"/>
+      <c r="T84" s="14"/>
+    </row>
+    <row r="85" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B85" s="11"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="12"/>
+      <c r="K85" s="12"/>
+      <c r="L85" s="12"/>
+      <c r="M85" s="12"/>
+      <c r="N85" s="12"/>
+      <c r="O85" s="12"/>
+      <c r="P85" s="12"/>
+      <c r="Q85" s="12"/>
+      <c r="R85" s="12"/>
+      <c r="S85" s="13"/>
+      <c r="T85" s="14"/>
+    </row>
+    <row r="86" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B86" s="11"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12"/>
+      <c r="J86" s="12"/>
+      <c r="K86" s="12"/>
+      <c r="L86" s="12"/>
+      <c r="M86" s="12"/>
+      <c r="N86" s="12"/>
+      <c r="O86" s="12"/>
+      <c r="P86" s="12"/>
+      <c r="Q86" s="12"/>
+      <c r="R86" s="12"/>
+      <c r="S86" s="13"/>
+      <c r="T86" s="14"/>
+    </row>
+    <row r="87" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B87" s="11"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="12"/>
+      <c r="J87" s="12"/>
+      <c r="K87" s="12"/>
+      <c r="L87" s="12"/>
+      <c r="M87" s="12"/>
+      <c r="N87" s="12"/>
+      <c r="O87" s="12"/>
+      <c r="P87" s="12"/>
+      <c r="Q87" s="12"/>
+      <c r="R87" s="12"/>
+      <c r="S87" s="13"/>
+      <c r="T87" s="14"/>
+    </row>
+    <row r="88" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B88" s="11"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="12"/>
+      <c r="J88" s="12"/>
+      <c r="K88" s="12"/>
+      <c r="L88" s="12"/>
+      <c r="M88" s="12"/>
+      <c r="N88" s="12"/>
+      <c r="O88" s="12"/>
+      <c r="P88" s="12"/>
+      <c r="Q88" s="12"/>
+      <c r="R88" s="12"/>
+      <c r="S88" s="13"/>
+      <c r="T88" s="14"/>
+    </row>
+    <row r="89" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B89" s="11"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="12"/>
+      <c r="I89" s="12"/>
+      <c r="J89" s="12"/>
+      <c r="K89" s="12"/>
+      <c r="L89" s="12"/>
+      <c r="M89" s="12"/>
+      <c r="N89" s="12"/>
+      <c r="O89" s="12"/>
+      <c r="P89" s="12"/>
+      <c r="Q89" s="12"/>
+      <c r="R89" s="12"/>
+      <c r="S89" s="13"/>
+      <c r="T89" s="14"/>
+    </row>
+    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B90" s="11"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="12"/>
+      <c r="I90" s="12"/>
+      <c r="J90" s="12"/>
+      <c r="K90" s="12"/>
+      <c r="L90" s="12"/>
+      <c r="M90" s="12"/>
+      <c r="N90" s="12"/>
+      <c r="O90" s="12"/>
+      <c r="P90" s="12"/>
+      <c r="Q90" s="12"/>
+      <c r="R90" s="12"/>
+      <c r="S90" s="13"/>
+      <c r="T90" s="14"/>
+    </row>
+    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B91" s="11"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="12"/>
+      <c r="J91" s="12"/>
+      <c r="K91" s="12"/>
+      <c r="L91" s="12"/>
+      <c r="M91" s="12"/>
+      <c r="N91" s="12"/>
+      <c r="O91" s="12"/>
+      <c r="P91" s="12"/>
+      <c r="Q91" s="12"/>
+      <c r="R91" s="12"/>
+      <c r="S91" s="13"/>
+      <c r="T91" s="14"/>
+    </row>
+    <row r="92" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B92" s="11"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="12"/>
+      <c r="J92" s="12"/>
+      <c r="K92" s="12"/>
+      <c r="L92" s="12"/>
+      <c r="M92" s="12"/>
+      <c r="N92" s="12"/>
+      <c r="O92" s="12"/>
+      <c r="P92" s="12"/>
+      <c r="Q92" s="12"/>
+      <c r="R92" s="12"/>
+      <c r="S92" s="13"/>
+      <c r="T92" s="14"/>
+    </row>
+    <row r="93" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B93" s="11"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="12"/>
+      <c r="J93" s="12"/>
+      <c r="K93" s="12"/>
+      <c r="L93" s="12"/>
+      <c r="M93" s="12"/>
+      <c r="N93" s="12"/>
+      <c r="O93" s="12"/>
+      <c r="P93" s="12"/>
+      <c r="Q93" s="12"/>
+      <c r="R93" s="12"/>
+      <c r="S93" s="13"/>
+      <c r="T93" s="14"/>
+    </row>
+    <row r="94" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B94" s="11"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="12"/>
+      <c r="J94" s="12"/>
+      <c r="K94" s="12"/>
+      <c r="L94" s="12"/>
+      <c r="M94" s="12"/>
+      <c r="N94" s="12"/>
+      <c r="O94" s="12"/>
+      <c r="P94" s="12"/>
+      <c r="Q94" s="12"/>
+      <c r="R94" s="12"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="14"/>
+    </row>
+    <row r="95" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B95" s="11"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="12"/>
+      <c r="K95" s="12"/>
+      <c r="L95" s="12"/>
+      <c r="M95" s="12"/>
+      <c r="N95" s="12"/>
+      <c r="O95" s="12"/>
+      <c r="P95" s="12"/>
+      <c r="Q95" s="12"/>
+      <c r="R95" s="12"/>
+      <c r="S95" s="13"/>
+      <c r="T95" s="14"/>
+    </row>
+    <row r="96" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B96" s="11"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12"/>
+      <c r="I96" s="12"/>
+      <c r="J96" s="12"/>
+      <c r="K96" s="12"/>
+      <c r="L96" s="12"/>
+      <c r="M96" s="12"/>
+      <c r="N96" s="12"/>
+      <c r="O96" s="12"/>
+      <c r="P96" s="12"/>
+      <c r="Q96" s="12"/>
+      <c r="R96" s="12"/>
+      <c r="S96" s="13"/>
+      <c r="T96" s="14"/>
+    </row>
+    <row r="97" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B97" s="11"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
+      <c r="L97" s="12"/>
+      <c r="M97" s="12"/>
+      <c r="N97" s="12"/>
+      <c r="O97" s="12"/>
+      <c r="P97" s="12"/>
+      <c r="Q97" s="12"/>
+      <c r="R97" s="12"/>
+      <c r="S97" s="13"/>
+      <c r="T97" s="14"/>
+    </row>
+    <row r="98" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B98" s="11"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+      <c r="I98" s="12"/>
+      <c r="J98" s="12"/>
+      <c r="K98" s="12"/>
+      <c r="L98" s="12"/>
+      <c r="M98" s="12"/>
+      <c r="N98" s="12"/>
+      <c r="O98" s="12"/>
+      <c r="P98" s="12"/>
+      <c r="Q98" s="12"/>
+      <c r="R98" s="12"/>
+      <c r="S98" s="13"/>
+      <c r="T98" s="14"/>
+    </row>
+    <row r="99" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B99" s="11"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="12"/>
+      <c r="I99" s="12"/>
+      <c r="J99" s="12"/>
+      <c r="K99" s="12"/>
+      <c r="L99" s="12"/>
+      <c r="M99" s="12"/>
+      <c r="N99" s="12"/>
+      <c r="O99" s="12"/>
+      <c r="P99" s="12"/>
+      <c r="Q99" s="12"/>
+      <c r="R99" s="12"/>
+      <c r="S99" s="13"/>
+      <c r="T99" s="14"/>
+    </row>
+    <row r="100" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B100" s="11"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="12"/>
+      <c r="I100" s="12"/>
+      <c r="J100" s="12"/>
+      <c r="K100" s="12"/>
+      <c r="L100" s="12"/>
+      <c r="M100" s="12"/>
+      <c r="N100" s="12"/>
+      <c r="O100" s="12"/>
+      <c r="P100" s="12"/>
+      <c r="Q100" s="12"/>
+      <c r="R100" s="12"/>
+      <c r="S100" s="13"/>
+      <c r="T100" s="14"/>
+    </row>
+    <row r="101" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B101" s="11"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12"/>
+      <c r="H101" s="12"/>
+      <c r="I101" s="12"/>
+      <c r="J101" s="12"/>
+      <c r="K101" s="12"/>
+      <c r="L101" s="12"/>
+      <c r="M101" s="12"/>
+      <c r="N101" s="12"/>
+      <c r="O101" s="12"/>
+      <c r="P101" s="12"/>
+      <c r="Q101" s="12"/>
+      <c r="R101" s="12"/>
+      <c r="S101" s="13"/>
+      <c r="T101" s="14"/>
+    </row>
+    <row r="102" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B102" s="11"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
+      <c r="H102" s="12"/>
+      <c r="I102" s="12"/>
+      <c r="J102" s="12"/>
+      <c r="K102" s="12"/>
+      <c r="L102" s="12"/>
+      <c r="M102" s="12"/>
+      <c r="N102" s="12"/>
+      <c r="O102" s="12"/>
+      <c r="P102" s="12"/>
+      <c r="Q102" s="12"/>
+      <c r="R102" s="12"/>
+      <c r="S102" s="13"/>
+      <c r="T102" s="14"/>
+    </row>
+    <row r="103" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B103" s="16"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="17"/>
+      <c r="J103" s="17"/>
+      <c r="K103" s="17"/>
+      <c r="L103" s="17"/>
+      <c r="M103" s="17"/>
+      <c r="N103" s="17"/>
+      <c r="O103" s="17"/>
+      <c r="P103" s="17"/>
+      <c r="Q103" s="17"/>
+      <c r="R103" s="17"/>
+      <c r="S103" s="18"/>
+      <c r="T103" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="B4:T4"/>
-  <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E55">
+  <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E27 E61:E103">
       <formula1>$X$7:$X$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F27 F63:F103">
       <formula1>$Y$7:$Y$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G27 G63:G103">
       <formula1>$Z$7:$Z$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H103">
       <formula1>$AA$7:$AA$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I103">
       <formula1>$AB$7:$AB$26</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J27 J63:J103">
       <formula1>$AC$7:$AC$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L27 L63:L103">
       <formula1>$AD$7:$AD$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R27 R63:R103">
       <formula1>$AF$7:$AF$13</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F61:G62 R28:R62 L28:L62 J28:J62 E28:G60">
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nhom ThanhChV, LinhTA, HuyDV, DucNH cap nhat fie Defect Log.xlsx sau khi sua loi.
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="8580"/>
@@ -1223,11 +1223,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1600,7 +1600,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1635,7 +1634,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1811,14 +1809,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AF103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="E61" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="L13" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -1854,12 +1852,12 @@
     <col min="33" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:32">
       <c r="R1" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" ht="30">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1868,7 +1866,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>129</v>
       </c>
@@ -1939,7 +1937,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="2:32" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:32" ht="45">
       <c r="B5" s="11">
         <v>40837</v>
       </c>
@@ -1996,7 +1994,7 @@
         <v>40838</v>
       </c>
     </row>
-    <row r="6" spans="2:32" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:32" ht="45">
       <c r="B6" s="11">
         <v>40837</v>
       </c>
@@ -2083,7 +2081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:32" ht="30">
       <c r="B7" s="11">
         <v>40837</v>
       </c>
@@ -2167,7 +2165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:32" ht="30">
       <c r="B8" s="11">
         <v>40837</v>
       </c>
@@ -2251,7 +2249,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:32" ht="30">
       <c r="B9" s="11">
         <v>40837</v>
       </c>
@@ -2335,7 +2333,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:32" ht="30">
       <c r="B10" s="11">
         <v>40837</v>
       </c>
@@ -2419,7 +2417,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:32" ht="30">
       <c r="B11" s="11">
         <v>40837</v>
       </c>
@@ -2497,7 +2495,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:32" ht="30">
       <c r="B12" s="11">
         <v>40837</v>
       </c>
@@ -2575,7 +2573,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32" ht="30">
       <c r="B13" s="11">
         <v>40837</v>
       </c>
@@ -2653,7 +2651,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32" ht="36" customHeight="1">
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -2692,7 +2690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:32" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:32" ht="60">
       <c r="B15" s="11">
         <v>40837</v>
       </c>
@@ -2703,7 +2701,7 @@
         <v>110</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>30</v>
@@ -2742,8 +2740,12 @@
       <c r="R15" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="S15" s="13"/>
-      <c r="T15" s="14"/>
+      <c r="S15" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T15" s="13">
+        <v>40838</v>
+      </c>
       <c r="X15" s="3" t="s">
         <v>11</v>
       </c>
@@ -2763,7 +2765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:32" ht="36" customHeight="1">
       <c r="B16" s="11">
         <v>40837</v>
       </c>
@@ -2774,7 +2776,7 @@
         <v>111</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>30</v>
@@ -2813,8 +2815,12 @@
       <c r="R16" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="S16" s="13"/>
-      <c r="T16" s="14"/>
+      <c r="S16" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T16" s="13">
+        <v>40838</v>
+      </c>
       <c r="X16" s="3" t="s">
         <v>13</v>
       </c>
@@ -2831,7 +2837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:31" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:31" ht="47.25" customHeight="1">
       <c r="B17" s="11">
         <v>40837</v>
       </c>
@@ -2842,7 +2848,7 @@
         <v>113</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>30</v>
@@ -2881,8 +2887,12 @@
       <c r="R17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="S17" s="13"/>
-      <c r="T17" s="14"/>
+      <c r="S17" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T17" s="13">
+        <v>40838</v>
+      </c>
       <c r="X17" s="3" t="s">
         <v>16</v>
       </c>
@@ -2899,7 +2909,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:31" ht="30">
       <c r="B18" s="11">
         <v>40837</v>
       </c>
@@ -2910,7 +2920,7 @@
         <v>114</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>30</v>
@@ -2949,8 +2959,12 @@
       <c r="R18" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="S18" s="13"/>
-      <c r="T18" s="14"/>
+      <c r="S18" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T18" s="13">
+        <v>40838</v>
+      </c>
       <c r="Y18" s="3" t="s">
         <v>39</v>
       </c>
@@ -2961,7 +2975,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="2:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:31" ht="36.75" customHeight="1">
       <c r="B19" s="11">
         <v>40837</v>
       </c>
@@ -2972,7 +2986,7 @@
         <v>116</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>30</v>
@@ -3011,8 +3025,12 @@
       <c r="R19" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="S19" s="13"/>
-      <c r="T19" s="14"/>
+      <c r="S19" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T19" s="13">
+        <v>40838</v>
+      </c>
       <c r="Y19" s="3" t="s">
         <v>36</v>
       </c>
@@ -3023,7 +3041,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="2:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:31" ht="29.25" customHeight="1">
       <c r="B20" s="11">
         <v>40837</v>
       </c>
@@ -3034,7 +3052,7 @@
         <v>118</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>30</v>
@@ -3073,8 +3091,12 @@
       <c r="R20" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="S20" s="13"/>
-      <c r="T20" s="14"/>
+      <c r="S20" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T20" s="13">
+        <v>40838</v>
+      </c>
       <c r="Y20" s="3" t="s">
         <v>34</v>
       </c>
@@ -3082,7 +3104,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:31" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:31" ht="33" customHeight="1">
       <c r="B21" s="11">
         <v>40837</v>
       </c>
@@ -3093,7 +3115,7 @@
         <v>126</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>30</v>
@@ -3132,8 +3154,12 @@
       <c r="R21" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="S21" s="13"/>
-      <c r="T21" s="14"/>
+      <c r="S21" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T21" s="13">
+        <v>40838</v>
+      </c>
       <c r="Y21" s="3" t="s">
         <v>32</v>
       </c>
@@ -3141,7 +3167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:31" ht="30">
       <c r="B22" s="11">
         <v>40837</v>
       </c>
@@ -3152,7 +3178,7 @@
         <v>121</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>30</v>
@@ -3191,13 +3217,17 @@
       <c r="R22" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="S22" s="13"/>
-      <c r="T22" s="14"/>
+      <c r="S22" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T22" s="13">
+        <v>40838</v>
+      </c>
       <c r="AB22" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="2:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:31" ht="37.5" customHeight="1">
       <c r="B23" s="11">
         <v>40837</v>
       </c>
@@ -3208,7 +3238,7 @@
         <v>122</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>30</v>
@@ -3247,13 +3277,17 @@
       <c r="R23" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="S23" s="13"/>
-      <c r="T23" s="14"/>
+      <c r="S23" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T23" s="13">
+        <v>40838</v>
+      </c>
       <c r="AB23" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:31" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:31" ht="43.5" customHeight="1">
       <c r="B24" s="11">
         <v>40837</v>
       </c>
@@ -3264,7 +3298,7 @@
         <v>124</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>30</v>
@@ -3303,13 +3337,17 @@
       <c r="R24" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="S24" s="13"/>
-      <c r="T24" s="14"/>
+      <c r="S24" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T24" s="13">
+        <v>40838</v>
+      </c>
       <c r="AB24" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:31" ht="30">
       <c r="B25" s="11">
         <v>40837</v>
       </c>
@@ -3320,7 +3358,7 @@
         <v>124</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>30</v>
@@ -3359,13 +3397,17 @@
       <c r="R25" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="S25" s="13"/>
-      <c r="T25" s="14"/>
+      <c r="S25" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T25" s="13">
+        <v>40838</v>
+      </c>
       <c r="AB25" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:31" ht="36.75" customHeight="1">
       <c r="B26" s="11">
         <v>40837</v>
       </c>
@@ -3376,7 +3418,7 @@
         <v>181</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>30</v>
@@ -3415,8 +3457,12 @@
       <c r="R26" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="S26" s="13"/>
-      <c r="T26" s="14"/>
+      <c r="S26" s="13">
+        <v>40838</v>
+      </c>
+      <c r="T26" s="13">
+        <v>40838</v>
+      </c>
       <c r="X26" s="3" t="s">
         <v>16</v>
       </c>
@@ -3433,7 +3479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:31">
       <c r="B27" s="11"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -3454,7 +3500,7 @@
       <c r="S27" s="13"/>
       <c r="T27" s="14"/>
     </row>
-    <row r="28" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:31" ht="30">
       <c r="B28" s="11">
         <v>40837</v>
       </c>
@@ -3495,7 +3541,7 @@
       <c r="S28" s="13"/>
       <c r="T28" s="14"/>
     </row>
-    <row r="29" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:31" ht="30">
       <c r="B29" s="11">
         <v>40837</v>
       </c>
@@ -3536,7 +3582,7 @@
       <c r="S29" s="13"/>
       <c r="T29" s="14"/>
     </row>
-    <row r="30" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:31" ht="30">
       <c r="B30" s="11">
         <v>40837</v>
       </c>
@@ -3577,7 +3623,7 @@
       <c r="S30" s="13"/>
       <c r="T30" s="14"/>
     </row>
-    <row r="31" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:31" ht="30">
       <c r="B31" s="11">
         <v>40837</v>
       </c>
@@ -3618,7 +3664,7 @@
       <c r="S31" s="13"/>
       <c r="T31" s="14"/>
     </row>
-    <row r="32" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:31" ht="30">
       <c r="B32" s="11">
         <v>40837</v>
       </c>
@@ -3659,7 +3705,7 @@
       <c r="S32" s="13"/>
       <c r="T32" s="14"/>
     </row>
-    <row r="33" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20" ht="30">
       <c r="B33" s="11">
         <v>40837</v>
       </c>
@@ -3700,7 +3746,7 @@
       <c r="S33" s="13"/>
       <c r="T33" s="14"/>
     </row>
-    <row r="34" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20" ht="30">
       <c r="B34" s="11">
         <v>40837</v>
       </c>
@@ -3741,7 +3787,7 @@
       <c r="S34" s="13"/>
       <c r="T34" s="14"/>
     </row>
-    <row r="35" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20" ht="30">
       <c r="B35" s="11">
         <v>40837</v>
       </c>
@@ -3782,7 +3828,7 @@
       <c r="S35" s="13"/>
       <c r="T35" s="14"/>
     </row>
-    <row r="36" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20" ht="30">
       <c r="B36" s="11">
         <v>40837</v>
       </c>
@@ -3823,7 +3869,7 @@
       <c r="S36" s="13"/>
       <c r="T36" s="14"/>
     </row>
-    <row r="37" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20" ht="30">
       <c r="B37" s="11">
         <v>40837</v>
       </c>
@@ -3864,7 +3910,7 @@
       <c r="S37" s="13"/>
       <c r="T37" s="14"/>
     </row>
-    <row r="38" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20" ht="30">
       <c r="B38" s="11">
         <v>40837</v>
       </c>
@@ -3905,7 +3951,7 @@
       <c r="S38" s="13"/>
       <c r="T38" s="14"/>
     </row>
-    <row r="39" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20" ht="30">
       <c r="B39" s="11">
         <v>40837</v>
       </c>
@@ -3946,7 +3992,7 @@
       <c r="S39" s="13"/>
       <c r="T39" s="14"/>
     </row>
-    <row r="40" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20" ht="30">
       <c r="B40" s="11">
         <v>40837</v>
       </c>
@@ -3987,7 +4033,7 @@
       <c r="S40" s="13"/>
       <c r="T40" s="14"/>
     </row>
-    <row r="41" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20" ht="30">
       <c r="B41" s="11">
         <v>40837</v>
       </c>
@@ -4028,7 +4074,7 @@
       <c r="S41" s="13"/>
       <c r="T41" s="14"/>
     </row>
-    <row r="42" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:20" ht="30">
       <c r="B42" s="11">
         <v>40837</v>
       </c>
@@ -4069,7 +4115,7 @@
       <c r="S42" s="13"/>
       <c r="T42" s="14"/>
     </row>
-    <row r="43" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:20" ht="30">
       <c r="B43" s="11">
         <v>40837</v>
       </c>
@@ -4110,7 +4156,7 @@
       <c r="S43" s="13"/>
       <c r="T43" s="14"/>
     </row>
-    <row r="44" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20" ht="27.75" customHeight="1">
       <c r="B44" s="11">
         <v>40837</v>
       </c>
@@ -4151,7 +4197,7 @@
       <c r="S44" s="13"/>
       <c r="T44" s="14"/>
     </row>
-    <row r="45" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:20" ht="30">
       <c r="B45" s="11">
         <v>40837</v>
       </c>
@@ -4192,7 +4238,7 @@
       <c r="S45" s="13"/>
       <c r="T45" s="14"/>
     </row>
-    <row r="46" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:20" ht="30">
       <c r="B46" s="11">
         <v>40837</v>
       </c>
@@ -4233,7 +4279,7 @@
       <c r="S46" s="13"/>
       <c r="T46" s="14"/>
     </row>
-    <row r="47" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:20" ht="30">
       <c r="B47" s="11">
         <v>40837</v>
       </c>
@@ -4274,7 +4320,7 @@
       <c r="S47" s="13"/>
       <c r="T47" s="14"/>
     </row>
-    <row r="48" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:20" ht="30">
       <c r="B48" s="11">
         <v>40837</v>
       </c>
@@ -4315,7 +4361,7 @@
       <c r="S48" s="13"/>
       <c r="T48" s="14"/>
     </row>
-    <row r="49" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:32" ht="30">
       <c r="B49" s="11">
         <v>40837</v>
       </c>
@@ -4356,7 +4402,7 @@
       <c r="S49" s="13"/>
       <c r="T49" s="14"/>
     </row>
-    <row r="50" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:32" ht="30">
       <c r="B50" s="11">
         <v>40837</v>
       </c>
@@ -4397,7 +4443,7 @@
       <c r="S50" s="13"/>
       <c r="T50" s="14"/>
     </row>
-    <row r="51" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:32" ht="30">
       <c r="B51" s="11">
         <v>40837</v>
       </c>
@@ -4438,7 +4484,7 @@
       <c r="S51" s="13"/>
       <c r="T51" s="14"/>
     </row>
-    <row r="52" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:32" ht="30">
       <c r="B52" s="11">
         <v>40837</v>
       </c>
@@ -4479,7 +4525,7 @@
       <c r="S52" s="13"/>
       <c r="T52" s="14"/>
     </row>
-    <row r="53" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:32" ht="30">
       <c r="B53" s="11">
         <v>40837</v>
       </c>
@@ -4520,7 +4566,7 @@
       <c r="S53" s="13"/>
       <c r="T53" s="14"/>
     </row>
-    <row r="54" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:32" ht="30">
       <c r="B54" s="11">
         <v>40837</v>
       </c>
@@ -4561,7 +4607,7 @@
       <c r="S54" s="13"/>
       <c r="T54" s="14"/>
     </row>
-    <row r="55" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:32" ht="30">
       <c r="B55" s="11">
         <v>40837</v>
       </c>
@@ -4602,7 +4648,7 @@
       <c r="S55" s="13"/>
       <c r="T55" s="14"/>
     </row>
-    <row r="56" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:32" ht="30">
       <c r="B56" s="11">
         <v>40837</v>
       </c>
@@ -4643,7 +4689,7 @@
       <c r="S56" s="13"/>
       <c r="T56" s="14"/>
     </row>
-    <row r="57" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:32" ht="30">
       <c r="B57" s="11">
         <v>40837</v>
       </c>
@@ -4684,7 +4730,7 @@
       <c r="S57" s="13"/>
       <c r="T57" s="14"/>
     </row>
-    <row r="58" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:32" ht="30">
       <c r="B58" s="11">
         <v>40837</v>
       </c>
@@ -4725,7 +4771,7 @@
       <c r="S58" s="13"/>
       <c r="T58" s="14"/>
     </row>
-    <row r="59" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:32" ht="30">
       <c r="B59" s="11">
         <v>40837</v>
       </c>
@@ -4766,7 +4812,7 @@
       <c r="S59" s="13"/>
       <c r="T59" s="14"/>
     </row>
-    <row r="60" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:32" ht="30">
       <c r="B60" s="11">
         <v>40837</v>
       </c>
@@ -4807,7 +4853,7 @@
       <c r="S60" s="13"/>
       <c r="T60" s="14"/>
     </row>
-    <row r="61" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:32" ht="30">
       <c r="B61" s="11">
         <v>40837</v>
       </c>
@@ -4848,7 +4894,7 @@
       <c r="S61" s="13"/>
       <c r="T61" s="14"/>
     </row>
-    <row r="62" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:32" ht="30">
       <c r="B62" s="11">
         <v>40837</v>
       </c>
@@ -4901,7 +4947,7 @@
       <c r="AE62"/>
       <c r="AF62"/>
     </row>
-    <row r="63" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:32" ht="30">
       <c r="B63" s="11">
         <v>40837</v>
       </c>
@@ -4954,7 +5000,7 @@
       <c r="AE63"/>
       <c r="AF63"/>
     </row>
-    <row r="64" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:32" ht="30">
       <c r="B64" s="11">
         <v>40837</v>
       </c>
@@ -5007,7 +5053,7 @@
       <c r="AE64"/>
       <c r="AF64"/>
     </row>
-    <row r="65" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:32" ht="30">
       <c r="B65" s="11">
         <v>40837</v>
       </c>
@@ -5060,7 +5106,7 @@
       <c r="AE65"/>
       <c r="AF65"/>
     </row>
-    <row r="66" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:32" ht="30">
       <c r="B66" s="11">
         <v>40837</v>
       </c>
@@ -5113,7 +5159,7 @@
       <c r="AE66"/>
       <c r="AF66"/>
     </row>
-    <row r="67" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:32" ht="30">
       <c r="B67" s="11">
         <v>40837</v>
       </c>
@@ -5166,7 +5212,7 @@
       <c r="AE67"/>
       <c r="AF67"/>
     </row>
-    <row r="68" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:32" ht="30">
       <c r="B68" s="11">
         <v>40837</v>
       </c>
@@ -5219,7 +5265,7 @@
       <c r="AE68"/>
       <c r="AF68"/>
     </row>
-    <row r="69" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:32" ht="30">
       <c r="B69" s="11">
         <v>40837</v>
       </c>
@@ -5272,7 +5318,7 @@
       <c r="AE69"/>
       <c r="AF69"/>
     </row>
-    <row r="70" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:32" ht="30">
       <c r="B70" s="11">
         <v>40837</v>
       </c>
@@ -5325,7 +5371,7 @@
       <c r="AE70"/>
       <c r="AF70"/>
     </row>
-    <row r="71" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:32" ht="30">
       <c r="B71" s="11">
         <v>40837</v>
       </c>
@@ -5378,7 +5424,7 @@
       <c r="AE71"/>
       <c r="AF71"/>
     </row>
-    <row r="72" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:32" ht="30">
       <c r="B72" s="11">
         <v>40837</v>
       </c>
@@ -5431,7 +5477,7 @@
       <c r="AE72"/>
       <c r="AF72"/>
     </row>
-    <row r="73" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:32" ht="30">
       <c r="B73" s="11">
         <v>40837</v>
       </c>
@@ -5484,7 +5530,7 @@
       <c r="AE73"/>
       <c r="AF73"/>
     </row>
-    <row r="74" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:32" ht="30">
       <c r="B74" s="11">
         <v>40837</v>
       </c>
@@ -5525,7 +5571,7 @@
       <c r="S74" s="13"/>
       <c r="T74" s="14"/>
     </row>
-    <row r="75" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:32" ht="30">
       <c r="B75" s="11">
         <v>40837</v>
       </c>
@@ -5566,7 +5612,7 @@
       <c r="S75" s="13"/>
       <c r="T75" s="14"/>
     </row>
-    <row r="76" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:32">
       <c r="B76" s="11"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
@@ -5587,7 +5633,7 @@
       <c r="S76" s="13"/>
       <c r="T76" s="14"/>
     </row>
-    <row r="77" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:32">
       <c r="B77" s="11"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
@@ -5608,7 +5654,7 @@
       <c r="S77" s="13"/>
       <c r="T77" s="14"/>
     </row>
-    <row r="78" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:32">
       <c r="B78" s="11"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
@@ -5629,7 +5675,7 @@
       <c r="S78" s="13"/>
       <c r="T78" s="14"/>
     </row>
-    <row r="79" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:32">
       <c r="B79" s="11"/>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
@@ -5650,7 +5696,7 @@
       <c r="S79" s="13"/>
       <c r="T79" s="14"/>
     </row>
-    <row r="80" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:32">
       <c r="B80" s="11"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
@@ -5671,7 +5717,7 @@
       <c r="S80" s="13"/>
       <c r="T80" s="14"/>
     </row>
-    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:20">
       <c r="B81" s="11"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
@@ -5692,7 +5738,7 @@
       <c r="S81" s="13"/>
       <c r="T81" s="14"/>
     </row>
-    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:20">
       <c r="B82" s="11"/>
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
@@ -5713,7 +5759,7 @@
       <c r="S82" s="13"/>
       <c r="T82" s="14"/>
     </row>
-    <row r="83" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:20">
       <c r="B83" s="11"/>
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
@@ -5734,7 +5780,7 @@
       <c r="S83" s="13"/>
       <c r="T83" s="14"/>
     </row>
-    <row r="84" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:20">
       <c r="B84" s="11"/>
       <c r="C84" s="12"/>
       <c r="D84" s="12"/>
@@ -5755,7 +5801,7 @@
       <c r="S84" s="13"/>
       <c r="T84" s="14"/>
     </row>
-    <row r="85" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:20">
       <c r="B85" s="11"/>
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
@@ -5776,7 +5822,7 @@
       <c r="S85" s="13"/>
       <c r="T85" s="14"/>
     </row>
-    <row r="86" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:20">
       <c r="B86" s="11"/>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
@@ -5797,7 +5843,7 @@
       <c r="S86" s="13"/>
       <c r="T86" s="14"/>
     </row>
-    <row r="87" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:20">
       <c r="B87" s="11"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
@@ -5818,7 +5864,7 @@
       <c r="S87" s="13"/>
       <c r="T87" s="14"/>
     </row>
-    <row r="88" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:20">
       <c r="B88" s="11"/>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
@@ -5839,7 +5885,7 @@
       <c r="S88" s="13"/>
       <c r="T88" s="14"/>
     </row>
-    <row r="89" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:20">
       <c r="B89" s="11"/>
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
@@ -5860,7 +5906,7 @@
       <c r="S89" s="13"/>
       <c r="T89" s="14"/>
     </row>
-    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:20">
       <c r="B90" s="11"/>
       <c r="C90" s="12"/>
       <c r="D90" s="12"/>
@@ -5881,7 +5927,7 @@
       <c r="S90" s="13"/>
       <c r="T90" s="14"/>
     </row>
-    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:20">
       <c r="B91" s="11"/>
       <c r="C91" s="12"/>
       <c r="D91" s="12"/>
@@ -5902,7 +5948,7 @@
       <c r="S91" s="13"/>
       <c r="T91" s="14"/>
     </row>
-    <row r="92" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:20">
       <c r="B92" s="11"/>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
@@ -5923,7 +5969,7 @@
       <c r="S92" s="13"/>
       <c r="T92" s="14"/>
     </row>
-    <row r="93" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:20">
       <c r="B93" s="11"/>
       <c r="C93" s="12"/>
       <c r="D93" s="12"/>
@@ -5944,7 +5990,7 @@
       <c r="S93" s="13"/>
       <c r="T93" s="14"/>
     </row>
-    <row r="94" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:20">
       <c r="B94" s="11"/>
       <c r="C94" s="12"/>
       <c r="D94" s="12"/>
@@ -5965,7 +6011,7 @@
       <c r="S94" s="13"/>
       <c r="T94" s="14"/>
     </row>
-    <row r="95" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:20">
       <c r="B95" s="11"/>
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
@@ -5986,7 +6032,7 @@
       <c r="S95" s="13"/>
       <c r="T95" s="14"/>
     </row>
-    <row r="96" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:20">
       <c r="B96" s="11"/>
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
@@ -6007,7 +6053,7 @@
       <c r="S96" s="13"/>
       <c r="T96" s="14"/>
     </row>
-    <row r="97" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:20">
       <c r="B97" s="11"/>
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
@@ -6028,7 +6074,7 @@
       <c r="S97" s="13"/>
       <c r="T97" s="14"/>
     </row>
-    <row r="98" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:20">
       <c r="B98" s="11"/>
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
@@ -6049,7 +6095,7 @@
       <c r="S98" s="13"/>
       <c r="T98" s="14"/>
     </row>
-    <row r="99" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:20">
       <c r="B99" s="11"/>
       <c r="C99" s="12"/>
       <c r="D99" s="12"/>
@@ -6070,7 +6116,7 @@
       <c r="S99" s="13"/>
       <c r="T99" s="14"/>
     </row>
-    <row r="100" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:20">
       <c r="B100" s="11"/>
       <c r="C100" s="12"/>
       <c r="D100" s="12"/>
@@ -6091,7 +6137,7 @@
       <c r="S100" s="13"/>
       <c r="T100" s="14"/>
     </row>
-    <row r="101" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:20">
       <c r="B101" s="11"/>
       <c r="C101" s="12"/>
       <c r="D101" s="12"/>
@@ -6112,7 +6158,7 @@
       <c r="S101" s="13"/>
       <c r="T101" s="14"/>
     </row>
-    <row r="102" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:20">
       <c r="B102" s="11"/>
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
@@ -6133,7 +6179,7 @@
       <c r="S102" s="13"/>
       <c r="T102" s="14"/>
     </row>
-    <row r="103" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:20">
       <c r="B103" s="16"/>
       <c r="C103" s="17"/>
       <c r="D103" s="17"/>

</xml_diff>

<commit_message>
KhoaVT up phan dl  do leader cua nhom ko onl
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="247">
   <si>
     <t>Project Code:</t>
   </si>
@@ -1218,6 +1218,27 @@
   </si>
   <si>
     <t>Font Page Manager</t>
+  </si>
+  <si>
+    <t>22/10/2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> database: các item trong phần này đều dư</t>
+  </si>
+  <si>
+    <t>Category Manager</t>
+  </si>
+  <si>
+    <t>Front Page Manager</t>
+  </si>
+  <si>
+    <t>Sheet Contents - Menu Manager:   chưa có link</t>
+  </si>
+  <si>
+    <t>Sheet Contents - Menu Trash:          chưa có link</t>
+  </si>
+  <si>
+    <t>Mapping Item to database : hình như không có thao tác cho phần này</t>
   </si>
 </sst>
 </file>
@@ -1812,8 +1833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AF103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="L13" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="K71" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q81" sqref="Q81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5612,130 +5633,262 @@
       <c r="S75" s="13"/>
       <c r="T75" s="14"/>
     </row>
-    <row r="76" spans="2:32">
-      <c r="B76" s="11"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12"/>
+    <row r="76" spans="2:32" ht="30">
+      <c r="B76" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F76" s="12"/>
       <c r="G76" s="12"/>
-      <c r="H76" s="12"/>
-      <c r="I76" s="12"/>
+      <c r="H76" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I76" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J76" s="12"/>
-      <c r="K76" s="12"/>
+      <c r="K76" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L76" s="12"/>
-      <c r="M76" s="12"/>
-      <c r="N76" s="12"/>
+      <c r="M76" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="N76" s="12" t="s">
+        <v>236</v>
+      </c>
       <c r="O76" s="12"/>
       <c r="P76" s="12"/>
-      <c r="Q76" s="12"/>
+      <c r="Q76" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R76" s="12"/>
-      <c r="S76" s="13"/>
+      <c r="S76" s="13" t="s">
+        <v>240</v>
+      </c>
       <c r="T76" s="14"/>
     </row>
-    <row r="77" spans="2:32">
-      <c r="B77" s="11"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
+    <row r="77" spans="2:32" ht="30">
+      <c r="B77" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E77" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F77" s="12"/>
       <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
+      <c r="H77" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I77" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J77" s="12"/>
-      <c r="K77" s="12"/>
+      <c r="K77" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L77" s="12"/>
-      <c r="M77" s="12"/>
-      <c r="N77" s="12"/>
+      <c r="M77" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="N77" s="12" t="s">
+        <v>236</v>
+      </c>
       <c r="O77" s="12"/>
       <c r="P77" s="12"/>
-      <c r="Q77" s="12"/>
+      <c r="Q77" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R77" s="12"/>
-      <c r="S77" s="13"/>
+      <c r="S77" s="13" t="s">
+        <v>240</v>
+      </c>
       <c r="T77" s="14"/>
     </row>
-    <row r="78" spans="2:32">
-      <c r="B78" s="11"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
+    <row r="78" spans="2:32" ht="30">
+      <c r="B78" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
+      <c r="H78" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I78" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J78" s="12"/>
-      <c r="K78" s="12"/>
+      <c r="K78" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L78" s="12"/>
-      <c r="M78" s="12"/>
-      <c r="N78" s="12"/>
+      <c r="M78" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="N78" s="12" t="s">
+        <v>236</v>
+      </c>
       <c r="O78" s="12"/>
       <c r="P78" s="12"/>
-      <c r="Q78" s="12"/>
+      <c r="Q78" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R78" s="12"/>
-      <c r="S78" s="13"/>
+      <c r="S78" s="13" t="s">
+        <v>240</v>
+      </c>
       <c r="T78" s="14"/>
     </row>
-    <row r="79" spans="2:32">
-      <c r="B79" s="11"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
+    <row r="79" spans="2:32" ht="30">
+      <c r="B79" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F79" s="12"/>
       <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
+      <c r="H79" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I79" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J79" s="12"/>
-      <c r="K79" s="12"/>
+      <c r="K79" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L79" s="12"/>
-      <c r="M79" s="12"/>
-      <c r="N79" s="12"/>
+      <c r="M79" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="N79" s="12" t="s">
+        <v>186</v>
+      </c>
       <c r="O79" s="12"/>
       <c r="P79" s="12"/>
-      <c r="Q79" s="12"/>
+      <c r="Q79" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R79" s="12"/>
-      <c r="S79" s="13"/>
+      <c r="S79" s="13" t="s">
+        <v>240</v>
+      </c>
       <c r="T79" s="14"/>
     </row>
-    <row r="80" spans="2:32">
-      <c r="B80" s="11"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
+    <row r="80" spans="2:32" ht="30">
+      <c r="B80" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F80" s="12"/>
       <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
+      <c r="H80" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I80" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J80" s="12"/>
-      <c r="K80" s="12"/>
+      <c r="K80" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L80" s="12"/>
-      <c r="M80" s="12"/>
-      <c r="N80" s="12"/>
+      <c r="M80" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="N80" s="12" t="s">
+        <v>186</v>
+      </c>
       <c r="O80" s="12"/>
       <c r="P80" s="12"/>
-      <c r="Q80" s="12"/>
+      <c r="Q80" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R80" s="12"/>
-      <c r="S80" s="13"/>
+      <c r="S80" s="13" t="s">
+        <v>240</v>
+      </c>
       <c r="T80" s="14"/>
     </row>
-    <row r="81" spans="2:20">
-      <c r="B81" s="11"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
+    <row r="81" spans="2:20" ht="30">
+      <c r="B81" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="E81" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
+      <c r="H81" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I81" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="J81" s="12"/>
-      <c r="K81" s="12"/>
+      <c r="K81" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="L81" s="12"/>
-      <c r="M81" s="12"/>
-      <c r="N81" s="12"/>
+      <c r="M81" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="N81" s="12" t="s">
+        <v>186</v>
+      </c>
       <c r="O81" s="12"/>
       <c r="P81" s="12"/>
-      <c r="Q81" s="12"/>
+      <c r="Q81" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="R81" s="12"/>
-      <c r="S81" s="13"/>
+      <c r="S81" s="13" t="s">
+        <v>240</v>
+      </c>
       <c r="T81" s="14"/>
     </row>
     <row r="82" spans="2:20">
@@ -6202,32 +6355,47 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:T4"/>
-  <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E27 E61:E103">
+  <dataValidations count="14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E27 E61:E75 E82:E103">
       <formula1>$X$7:$X$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F27 F63:F103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F27 F63:F75 F82:F103">
       <formula1>$Y$7:$Y$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G27 G63:G103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G27 G63:G75 G82:G103">
       <formula1>$Z$7:$Z$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H75 H82:H103">
       <formula1>$AA$7:$AA$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I75 I82:I103">
       <formula1>$AB$7:$AB$26</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J27 J63:J103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J27 J63:J75 J82:J103">
       <formula1>$AC$7:$AC$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L27 L63:L103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L27 L63:L75 L82:L103">
       <formula1>$AD$7:$AD$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R27 R63:R103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R27 R63:R75 R82:R103">
       <formula1>$AF$7:$AF$13</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F61:G62 R28:R62 L28:L62 J28:J62 E28:G60">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H76:H81">
+      <formula1>$AA$5:$AA$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I76:I81">
+      <formula1>$AB$5:$AB$20</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J76:J78 L76:L78 R76:R78 E76:G78">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J79:J81 L79:L81 R79:R80 E79:G80 E81">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R81 F81:G81">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update lại file DecfectLog.
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -1833,8 +1833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AF103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="K71" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q81" sqref="Q81"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="C2" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1969,7 +1969,7 @@
         <v>94</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>30</v>
@@ -2026,7 +2026,7 @@
         <v>96</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
ThaoNX: update Defect Log.xlsx
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="8580"/>
@@ -11,7 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Defect Log'!$B$4:$T$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Defect Log'!$B$2:$T$103</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Defect Log'!$B$2:$T$100</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="259">
   <si>
     <t>Project Code:</t>
   </si>
@@ -1112,12 +1112,6 @@
     <t>CreatedMenus_New_NewMenuItem/tbxAlias: thiếu format, thiếu lenght</t>
   </si>
   <si>
-    <t>CreatedMenus_New_NewMenuItem/tbxLink: thiếu format, thiếu lenght,error check</t>
-  </si>
-  <si>
-    <t>CreatedMenus_New_NewMenuItem/: thiếu format, thiếu lenght</t>
-  </si>
-  <si>
     <t>Content/Menu Manager:   chưa có link</t>
   </si>
   <si>
@@ -1239,16 +1233,58 @@
   </si>
   <si>
     <t>Mapping Item to database : hình như không có thao tác cho phần này</t>
+  </si>
+  <si>
+    <t>Thêm Type Column</t>
+  </si>
+  <si>
+    <t>Thêm Format, Length value</t>
+  </si>
+  <si>
+    <t>CreatedMenus_New_NewMenuItem/tbxLink: thiếu format, thiếu length</t>
+  </si>
+  <si>
+    <t>Thêm link to Menu Manager</t>
+  </si>
+  <si>
+    <t>Thêm link to Menu Trash</t>
+  </si>
+  <si>
+    <t>Thêm link to MenuManager_Copy link</t>
+  </si>
+  <si>
+    <t>Thêm link to enuManager_New link</t>
+  </si>
+  <si>
+    <t>Thêm link to MenuManager_Edit link</t>
+  </si>
+  <si>
+    <t>Thêm link to  MenuTrash link</t>
+  </si>
+  <si>
+    <t>Thêm link to CreatedMenu_Copy  link</t>
+  </si>
+  <si>
+    <t>Thêm link to CreatedMenus link</t>
+  </si>
+  <si>
+    <t>Thêm link to  CreatedMenu_Move  link</t>
+  </si>
+  <si>
+    <t>Thêm link to  CreatedMenus_New_NewMenuItem  link</t>
+  </si>
+  <si>
+    <t>Thêm link to CreatedMenu_New_SeclectType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1621,6 +1657,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1655,6 +1692,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1830,17 +1868,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AF103"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AF100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="C2" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B61" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="3" customWidth="1"/>
     <col min="4" max="4" width="67.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" style="3" customWidth="1"/>
@@ -1849,15 +1887,15 @@
     <col min="8" max="8" width="9.140625" style="3"/>
     <col min="9" max="9" width="21" style="3" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="34.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.140625" style="3" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" style="3" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="3" customWidth="1"/>
     <col min="16" max="16" width="35" style="3" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.42578125" style="5" customWidth="1"/>
     <col min="21" max="22" width="9.140625" style="3"/>
     <col min="23" max="23" width="13.42578125" style="3" customWidth="1"/>
@@ -1873,12 +1911,12 @@
     <col min="33" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32">
+    <row r="1" spans="2:32" x14ac:dyDescent="0.25">
       <c r="R1" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="2:32" ht="30">
+    <row r="2" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1887,7 +1925,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1">
+    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>129</v>
       </c>
@@ -1958,7 +1996,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="2:32" ht="45">
+    <row r="5" spans="2:32" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
         <v>40837</v>
       </c>
@@ -2015,7 +2053,7 @@
         <v>40838</v>
       </c>
     </row>
-    <row r="6" spans="2:32" ht="45">
+    <row r="6" spans="2:32" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>40837</v>
       </c>
@@ -2102,7 +2140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:32" ht="30">
+    <row r="7" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>40837</v>
       </c>
@@ -2186,7 +2224,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:32" ht="30">
+    <row r="8" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>40837</v>
       </c>
@@ -2270,7 +2308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:32" ht="30">
+    <row r="9" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>40837</v>
       </c>
@@ -2354,7 +2392,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:32" ht="30">
+    <row r="10" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
         <v>40837</v>
       </c>
@@ -2438,7 +2476,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:32" ht="30">
+    <row r="11" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <v>40837</v>
       </c>
@@ -2516,7 +2554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:32" ht="30">
+    <row r="12" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <v>40837</v>
       </c>
@@ -2594,7 +2632,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:32" ht="30">
+    <row r="13" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>40837</v>
       </c>
@@ -2672,7 +2710,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="2:32" ht="36" customHeight="1">
+    <row r="14" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -2711,7 +2749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:32" ht="60">
+    <row r="15" spans="2:32" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
         <v>40837</v>
       </c>
@@ -2786,7 +2824,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:32" ht="36" customHeight="1">
+    <row r="16" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <v>40837</v>
       </c>
@@ -2858,7 +2896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:31" ht="47.25" customHeight="1">
+    <row r="17" spans="2:31" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>40837</v>
       </c>
@@ -2930,7 +2968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:31" ht="30">
+    <row r="18" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
         <v>40837</v>
       </c>
@@ -2996,7 +3034,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="2:31" ht="36.75" customHeight="1">
+    <row r="19" spans="2:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
         <v>40837</v>
       </c>
@@ -3062,7 +3100,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="2:31" ht="29.25" customHeight="1">
+    <row r="20" spans="2:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <v>40837</v>
       </c>
@@ -3125,7 +3163,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:31" ht="33" customHeight="1">
+    <row r="21" spans="2:31" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
         <v>40837</v>
       </c>
@@ -3188,7 +3226,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:31" ht="30">
+    <row r="22" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <v>40837</v>
       </c>
@@ -3248,7 +3286,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="2:31" ht="37.5" customHeight="1">
+    <row r="23" spans="2:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
         <v>40837</v>
       </c>
@@ -3308,7 +3346,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:31" ht="43.5" customHeight="1">
+    <row r="24" spans="2:31" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <v>40837</v>
       </c>
@@ -3368,7 +3406,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:31" ht="30">
+    <row r="25" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
         <v>40837</v>
       </c>
@@ -3428,7 +3466,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:31" ht="36.75" customHeight="1">
+    <row r="26" spans="2:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <v>40837</v>
       </c>
@@ -3500,7 +3538,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:31">
+    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -3521,7 +3559,7 @@
       <c r="S27" s="13"/>
       <c r="T27" s="14"/>
     </row>
-    <row r="28" spans="2:31" ht="30">
+    <row r="28" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
         <v>40837</v>
       </c>
@@ -3532,12 +3570,16 @@
         <v>183</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H28" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>67</v>
@@ -3546,7 +3588,9 @@
       <c r="K28" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L28" s="12"/>
+      <c r="L28" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M28" s="12" t="s">
         <v>185</v>
       </c>
@@ -3554,15 +3598,21 @@
         <v>186</v>
       </c>
       <c r="O28" s="20"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R28" s="12"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="14"/>
-    </row>
-    <row r="29" spans="2:31" ht="30">
+      <c r="P28" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S28" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T28" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="29" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
         <v>40837</v>
       </c>
@@ -3573,12 +3623,16 @@
         <v>187</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H29" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>67</v>
@@ -3587,7 +3641,9 @@
       <c r="K29" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L29" s="12"/>
+      <c r="L29" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M29" s="12" t="s">
         <v>185</v>
       </c>
@@ -3595,15 +3651,21 @@
         <v>186</v>
       </c>
       <c r="O29" s="20"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R29" s="12"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="14"/>
-    </row>
-    <row r="30" spans="2:31" ht="30">
+      <c r="P29" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S29" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T29" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="30" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
         <v>40837</v>
       </c>
@@ -3614,12 +3676,16 @@
         <v>188</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H30" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>67</v>
@@ -3628,7 +3694,9 @@
       <c r="K30" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L30" s="12"/>
+      <c r="L30" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M30" s="12" t="s">
         <v>185</v>
       </c>
@@ -3636,15 +3704,21 @@
         <v>186</v>
       </c>
       <c r="O30" s="20"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R30" s="12"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="14"/>
-    </row>
-    <row r="31" spans="2:31" ht="30">
+      <c r="P30" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S30" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T30" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="31" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
         <v>40837</v>
       </c>
@@ -3652,15 +3726,19 @@
         <v>128</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H31" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>67</v>
@@ -3669,7 +3747,9 @@
       <c r="K31" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L31" s="12"/>
+      <c r="L31" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M31" s="12" t="s">
         <v>185</v>
       </c>
@@ -3677,15 +3757,21 @@
         <v>186</v>
       </c>
       <c r="O31" s="20"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R31" s="12"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="14"/>
-    </row>
-    <row r="32" spans="2:31" ht="30">
+      <c r="P31" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S31" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T31" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="32" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
         <v>40837</v>
       </c>
@@ -3693,15 +3779,19 @@
         <v>128</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H32" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I32" s="12" t="s">
         <v>67</v>
@@ -3710,7 +3800,9 @@
       <c r="K32" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L32" s="12"/>
+      <c r="L32" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M32" s="12" t="s">
         <v>185</v>
       </c>
@@ -3718,15 +3810,21 @@
         <v>186</v>
       </c>
       <c r="O32" s="20"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R32" s="12"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="14"/>
-    </row>
-    <row r="33" spans="2:20" ht="30">
+      <c r="P32" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S32" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T32" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="33" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
         <v>40837</v>
       </c>
@@ -3734,15 +3832,19 @@
         <v>128</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H33" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>67</v>
@@ -3751,7 +3853,9 @@
       <c r="K33" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L33" s="12"/>
+      <c r="L33" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M33" s="12" t="s">
         <v>185</v>
       </c>
@@ -3759,15 +3863,21 @@
         <v>186</v>
       </c>
       <c r="O33" s="20"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R33" s="12"/>
-      <c r="S33" s="13"/>
-      <c r="T33" s="14"/>
-    </row>
-    <row r="34" spans="2:20" ht="30">
+      <c r="P33" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S33" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T33" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="34" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
         <v>40837</v>
       </c>
@@ -3775,15 +3885,19 @@
         <v>128</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H34" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>67</v>
@@ -3792,7 +3906,9 @@
       <c r="K34" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L34" s="12"/>
+      <c r="L34" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M34" s="12" t="s">
         <v>185</v>
       </c>
@@ -3800,15 +3916,21 @@
         <v>186</v>
       </c>
       <c r="O34" s="20"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R34" s="12"/>
-      <c r="S34" s="13"/>
-      <c r="T34" s="14"/>
-    </row>
-    <row r="35" spans="2:20" ht="30">
+      <c r="P34" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S34" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T34" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
         <v>40837</v>
       </c>
@@ -3816,15 +3938,19 @@
         <v>128</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H35" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>67</v>
@@ -3833,7 +3959,9 @@
       <c r="K35" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L35" s="12"/>
+      <c r="L35" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M35" s="12" t="s">
         <v>185</v>
       </c>
@@ -3841,15 +3969,21 @@
         <v>186</v>
       </c>
       <c r="O35" s="20"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R35" s="12"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="14"/>
-    </row>
-    <row r="36" spans="2:20" ht="30">
+      <c r="P35" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S35" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T35" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
         <v>40837</v>
       </c>
@@ -3857,15 +3991,19 @@
         <v>128</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H36" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>67</v>
@@ -3874,7 +4012,9 @@
       <c r="K36" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L36" s="12"/>
+      <c r="L36" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M36" s="12" t="s">
         <v>185</v>
       </c>
@@ -3882,15 +4022,21 @@
         <v>186</v>
       </c>
       <c r="O36" s="20"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R36" s="12"/>
-      <c r="S36" s="13"/>
-      <c r="T36" s="14"/>
-    </row>
-    <row r="37" spans="2:20" ht="30">
+      <c r="P36" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S36" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T36" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
         <v>40837</v>
       </c>
@@ -3898,15 +4044,19 @@
         <v>128</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H37" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I37" s="12" t="s">
         <v>67</v>
@@ -3915,7 +4065,9 @@
       <c r="K37" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L37" s="12"/>
+      <c r="L37" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M37" s="12" t="s">
         <v>185</v>
       </c>
@@ -3923,15 +4075,21 @@
         <v>186</v>
       </c>
       <c r="O37" s="20"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R37" s="12"/>
-      <c r="S37" s="13"/>
-      <c r="T37" s="14"/>
-    </row>
-    <row r="38" spans="2:20" ht="30">
+      <c r="P37" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S37" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T37" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
         <v>40837</v>
       </c>
@@ -3939,15 +4097,19 @@
         <v>128</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H38" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I38" s="12" t="s">
         <v>67</v>
@@ -3956,7 +4118,9 @@
       <c r="K38" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L38" s="12"/>
+      <c r="L38" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M38" s="12" t="s">
         <v>185</v>
       </c>
@@ -3964,15 +4128,21 @@
         <v>186</v>
       </c>
       <c r="O38" s="20"/>
-      <c r="P38" s="12"/>
-      <c r="Q38" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R38" s="12"/>
-      <c r="S38" s="13"/>
-      <c r="T38" s="14"/>
-    </row>
-    <row r="39" spans="2:20" ht="30">
+      <c r="P38" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S38" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T38" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="39" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
         <v>40837</v>
       </c>
@@ -3980,15 +4150,19 @@
         <v>128</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H39" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I39" s="12" t="s">
         <v>67</v>
@@ -3997,7 +4171,9 @@
       <c r="K39" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L39" s="12"/>
+      <c r="L39" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M39" s="12" t="s">
         <v>185</v>
       </c>
@@ -4005,15 +4181,21 @@
         <v>186</v>
       </c>
       <c r="O39" s="20"/>
-      <c r="P39" s="12"/>
-      <c r="Q39" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R39" s="12"/>
-      <c r="S39" s="13"/>
-      <c r="T39" s="14"/>
-    </row>
-    <row r="40" spans="2:20" ht="30">
+      <c r="P39" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S39" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T39" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="40" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
         <v>40837</v>
       </c>
@@ -4021,15 +4203,19 @@
         <v>128</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H40" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I40" s="12" t="s">
         <v>67</v>
@@ -4038,7 +4224,9 @@
       <c r="K40" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L40" s="12"/>
+      <c r="L40" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M40" s="12" t="s">
         <v>185</v>
       </c>
@@ -4046,15 +4234,21 @@
         <v>186</v>
       </c>
       <c r="O40" s="20"/>
-      <c r="P40" s="12"/>
-      <c r="Q40" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R40" s="12"/>
-      <c r="S40" s="13"/>
-      <c r="T40" s="14"/>
-    </row>
-    <row r="41" spans="2:20" ht="30">
+      <c r="P40" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S40" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T40" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="41" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
         <v>40837</v>
       </c>
@@ -4062,15 +4256,19 @@
         <v>128</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H41" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I41" s="12" t="s">
         <v>67</v>
@@ -4079,7 +4277,9 @@
       <c r="K41" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L41" s="12"/>
+      <c r="L41" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M41" s="12" t="s">
         <v>185</v>
       </c>
@@ -4087,15 +4287,21 @@
         <v>186</v>
       </c>
       <c r="O41" s="20"/>
-      <c r="P41" s="12"/>
-      <c r="Q41" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R41" s="12"/>
-      <c r="S41" s="13"/>
-      <c r="T41" s="14"/>
-    </row>
-    <row r="42" spans="2:20" ht="30">
+      <c r="P41" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S41" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T41" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="42" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="11">
         <v>40837</v>
       </c>
@@ -4103,15 +4309,19 @@
         <v>128</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H42" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I42" s="12" t="s">
         <v>67</v>
@@ -4120,7 +4330,9 @@
       <c r="K42" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L42" s="12"/>
+      <c r="L42" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M42" s="12" t="s">
         <v>185</v>
       </c>
@@ -4128,15 +4340,21 @@
         <v>186</v>
       </c>
       <c r="O42" s="20"/>
-      <c r="P42" s="12"/>
-      <c r="Q42" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R42" s="12"/>
-      <c r="S42" s="13"/>
-      <c r="T42" s="14"/>
-    </row>
-    <row r="43" spans="2:20" ht="30">
+      <c r="P42" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S42" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T42" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="43" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11">
         <v>40837</v>
       </c>
@@ -4144,15 +4362,19 @@
         <v>128</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H43" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I43" s="12" t="s">
         <v>67</v>
@@ -4161,7 +4383,9 @@
       <c r="K43" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L43" s="12"/>
+      <c r="L43" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M43" s="12" t="s">
         <v>185</v>
       </c>
@@ -4169,15 +4393,21 @@
         <v>186</v>
       </c>
       <c r="O43" s="20"/>
-      <c r="P43" s="12"/>
-      <c r="Q43" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R43" s="12"/>
-      <c r="S43" s="13"/>
-      <c r="T43" s="14"/>
-    </row>
-    <row r="44" spans="2:20" ht="27.75" customHeight="1">
+      <c r="P43" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S43" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T43" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="44" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="11">
         <v>40837</v>
       </c>
@@ -4185,15 +4415,19 @@
         <v>128</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H44" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I44" s="12" t="s">
         <v>67</v>
@@ -4202,7 +4436,9 @@
       <c r="K44" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L44" s="12"/>
+      <c r="L44" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M44" s="12" t="s">
         <v>185</v>
       </c>
@@ -4210,15 +4446,21 @@
         <v>186</v>
       </c>
       <c r="O44" s="20"/>
-      <c r="P44" s="12"/>
-      <c r="Q44" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R44" s="12"/>
-      <c r="S44" s="13"/>
-      <c r="T44" s="14"/>
-    </row>
-    <row r="45" spans="2:20" ht="30">
+      <c r="P44" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S44" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T44" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="11">
         <v>40837</v>
       </c>
@@ -4226,15 +4468,19 @@
         <v>128</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H45" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I45" s="12" t="s">
         <v>67</v>
@@ -4243,7 +4489,9 @@
       <c r="K45" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L45" s="12"/>
+      <c r="L45" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M45" s="12" t="s">
         <v>185</v>
       </c>
@@ -4251,15 +4499,21 @@
         <v>186</v>
       </c>
       <c r="O45" s="20"/>
-      <c r="P45" s="12"/>
-      <c r="Q45" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R45" s="12"/>
-      <c r="S45" s="13"/>
-      <c r="T45" s="14"/>
-    </row>
-    <row r="46" spans="2:20" ht="30">
+      <c r="P45" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S45" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T45" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="11">
         <v>40837</v>
       </c>
@@ -4267,15 +4521,19 @@
         <v>128</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>203</v>
+        <v>247</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H46" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I46" s="12" t="s">
         <v>67</v>
@@ -4284,7 +4542,9 @@
       <c r="K46" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L46" s="12"/>
+      <c r="L46" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M46" s="12" t="s">
         <v>185</v>
       </c>
@@ -4292,15 +4552,21 @@
         <v>186</v>
       </c>
       <c r="O46" s="20"/>
-      <c r="P46" s="12"/>
-      <c r="Q46" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R46" s="12"/>
-      <c r="S46" s="13"/>
-      <c r="T46" s="14"/>
-    </row>
-    <row r="47" spans="2:20" ht="30">
+      <c r="P46" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S46" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T46" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="11">
         <v>40837</v>
       </c>
@@ -4311,12 +4577,16 @@
         <v>204</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H47" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I47" s="12" t="s">
         <v>67</v>
@@ -4325,7 +4595,9 @@
       <c r="K47" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L47" s="12"/>
+      <c r="L47" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M47" s="12" t="s">
         <v>185</v>
       </c>
@@ -4333,15 +4605,21 @@
         <v>186</v>
       </c>
       <c r="O47" s="20"/>
-      <c r="P47" s="12"/>
-      <c r="Q47" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R47" s="12"/>
-      <c r="S47" s="13"/>
-      <c r="T47" s="14"/>
-    </row>
-    <row r="48" spans="2:20" ht="30">
+      <c r="P47" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S47" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T47" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="48" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="11">
         <v>40837</v>
       </c>
@@ -4352,12 +4630,16 @@
         <v>205</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H48" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I48" s="12" t="s">
         <v>67</v>
@@ -4366,7 +4648,9 @@
       <c r="K48" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L48" s="12"/>
+      <c r="L48" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M48" s="12" t="s">
         <v>185</v>
       </c>
@@ -4374,15 +4658,21 @@
         <v>186</v>
       </c>
       <c r="O48" s="20"/>
-      <c r="P48" s="12"/>
-      <c r="Q48" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R48" s="12"/>
-      <c r="S48" s="13"/>
-      <c r="T48" s="14"/>
-    </row>
-    <row r="49" spans="2:32" ht="30">
+      <c r="P48" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S48" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T48" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="49" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="11">
         <v>40837</v>
       </c>
@@ -4390,15 +4680,19 @@
         <v>128</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H49" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I49" s="12" t="s">
         <v>67</v>
@@ -4407,7 +4701,9 @@
       <c r="K49" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L49" s="12"/>
+      <c r="L49" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M49" s="12" t="s">
         <v>185</v>
       </c>
@@ -4415,15 +4711,21 @@
         <v>186</v>
       </c>
       <c r="O49" s="20"/>
-      <c r="P49" s="12"/>
-      <c r="Q49" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R49" s="12"/>
-      <c r="S49" s="13"/>
-      <c r="T49" s="14"/>
-    </row>
-    <row r="50" spans="2:32" ht="30">
+      <c r="P49" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S49" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T49" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="50" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="11">
         <v>40837</v>
       </c>
@@ -4431,15 +4733,19 @@
         <v>128</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H50" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I50" s="12" t="s">
         <v>67</v>
@@ -4448,7 +4754,9 @@
       <c r="K50" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L50" s="12"/>
+      <c r="L50" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M50" s="12" t="s">
         <v>185</v>
       </c>
@@ -4456,15 +4764,21 @@
         <v>186</v>
       </c>
       <c r="O50" s="20"/>
-      <c r="P50" s="12"/>
-      <c r="Q50" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R50" s="12"/>
-      <c r="S50" s="13"/>
-      <c r="T50" s="14"/>
-    </row>
-    <row r="51" spans="2:32" ht="30">
+      <c r="P50" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S50" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T50" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="51" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="11">
         <v>40837</v>
       </c>
@@ -4472,15 +4786,19 @@
         <v>128</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H51" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I51" s="12" t="s">
         <v>67</v>
@@ -4489,7 +4807,9 @@
       <c r="K51" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L51" s="12"/>
+      <c r="L51" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M51" s="12" t="s">
         <v>185</v>
       </c>
@@ -4497,15 +4817,21 @@
         <v>186</v>
       </c>
       <c r="O51" s="20"/>
-      <c r="P51" s="12"/>
-      <c r="Q51" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R51" s="12"/>
-      <c r="S51" s="13"/>
-      <c r="T51" s="14"/>
-    </row>
-    <row r="52" spans="2:32" ht="30">
+      <c r="P51" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S51" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T51" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="52" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="11">
         <v>40837</v>
       </c>
@@ -4513,15 +4839,19 @@
         <v>128</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H52" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I52" s="12" t="s">
         <v>67</v>
@@ -4530,7 +4860,9 @@
       <c r="K52" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L52" s="12"/>
+      <c r="L52" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M52" s="12" t="s">
         <v>185</v>
       </c>
@@ -4538,15 +4870,21 @@
         <v>186</v>
       </c>
       <c r="O52" s="20"/>
-      <c r="P52" s="12"/>
-      <c r="Q52" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R52" s="12"/>
-      <c r="S52" s="13"/>
-      <c r="T52" s="14"/>
-    </row>
-    <row r="53" spans="2:32" ht="30">
+      <c r="P52" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S52" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T52" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="53" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="11">
         <v>40837</v>
       </c>
@@ -4554,15 +4892,19 @@
         <v>128</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H53" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I53" s="12" t="s">
         <v>67</v>
@@ -4571,7 +4913,9 @@
       <c r="K53" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L53" s="12"/>
+      <c r="L53" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M53" s="12" t="s">
         <v>185</v>
       </c>
@@ -4579,15 +4923,21 @@
         <v>186</v>
       </c>
       <c r="O53" s="20"/>
-      <c r="P53" s="12"/>
-      <c r="Q53" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R53" s="12"/>
-      <c r="S53" s="13"/>
-      <c r="T53" s="14"/>
-    </row>
-    <row r="54" spans="2:32" ht="30">
+      <c r="P53" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S53" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T53" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="54" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="11">
         <v>40837</v>
       </c>
@@ -4595,15 +4945,19 @@
         <v>128</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H54" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I54" s="12" t="s">
         <v>67</v>
@@ -4612,7 +4966,9 @@
       <c r="K54" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L54" s="12"/>
+      <c r="L54" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M54" s="12" t="s">
         <v>185</v>
       </c>
@@ -4620,15 +4976,21 @@
         <v>186</v>
       </c>
       <c r="O54" s="20"/>
-      <c r="P54" s="12"/>
-      <c r="Q54" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R54" s="12"/>
-      <c r="S54" s="13"/>
-      <c r="T54" s="14"/>
-    </row>
-    <row r="55" spans="2:32" ht="30">
+      <c r="P54" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q54" s="12"/>
+      <c r="R54" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S54" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T54" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="55" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="11">
         <v>40837</v>
       </c>
@@ -4636,15 +4998,19 @@
         <v>128</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H55" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I55" s="12" t="s">
         <v>67</v>
@@ -4653,7 +5019,9 @@
       <c r="K55" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L55" s="12"/>
+      <c r="L55" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M55" s="12" t="s">
         <v>185</v>
       </c>
@@ -4661,15 +5029,21 @@
         <v>186</v>
       </c>
       <c r="O55" s="20"/>
-      <c r="P55" s="12"/>
-      <c r="Q55" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R55" s="12"/>
-      <c r="S55" s="13"/>
-      <c r="T55" s="14"/>
-    </row>
-    <row r="56" spans="2:32" ht="30">
+      <c r="P55" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S55" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T55" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="56" spans="2:32" ht="45" x14ac:dyDescent="0.25">
       <c r="B56" s="11">
         <v>40837</v>
       </c>
@@ -4677,15 +5051,19 @@
         <v>128</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H56" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I56" s="12" t="s">
         <v>67</v>
@@ -4694,7 +5072,9 @@
       <c r="K56" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L56" s="12"/>
+      <c r="L56" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M56" s="12" t="s">
         <v>185</v>
       </c>
@@ -4702,15 +5082,21 @@
         <v>186</v>
       </c>
       <c r="O56" s="20"/>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R56" s="12"/>
-      <c r="S56" s="13"/>
-      <c r="T56" s="14"/>
-    </row>
-    <row r="57" spans="2:32" ht="30">
+      <c r="P56" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S56" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T56" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="57" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="11">
         <v>40837</v>
       </c>
@@ -4718,15 +5104,19 @@
         <v>128</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H57" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I57" s="12" t="s">
         <v>67</v>
@@ -4735,7 +5125,9 @@
       <c r="K57" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L57" s="12"/>
+      <c r="L57" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M57" s="12" t="s">
         <v>185</v>
       </c>
@@ -4743,29 +5135,39 @@
         <v>186</v>
       </c>
       <c r="O57" s="20"/>
-      <c r="P57" s="12"/>
-      <c r="Q57" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="R57" s="12"/>
-      <c r="S57" s="13"/>
-      <c r="T57" s="14"/>
-    </row>
-    <row r="58" spans="2:32" ht="30">
+      <c r="P57" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S57" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T57" s="13">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="58" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="11">
         <v>40837</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E58" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
+      <c r="F58" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H58" s="12" t="s">
         <v>54</v>
       </c>
@@ -4774,39 +5176,47 @@
       </c>
       <c r="J58" s="12"/>
       <c r="K58" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="L58" s="12"/>
+        <v>216</v>
+      </c>
+      <c r="L58" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M58" s="12" t="s">
         <v>185</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="O58" s="20"/>
       <c r="P58" s="12"/>
       <c r="Q58" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R58" s="12"/>
+      <c r="R58" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S58" s="13"/>
-      <c r="T58" s="14"/>
-    </row>
-    <row r="59" spans="2:32" ht="30">
+      <c r="T58" s="13"/>
+    </row>
+    <row r="59" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B59" s="11">
         <v>40837</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>128</v>
+        <v>218</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E59" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
+      <c r="F59" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H59" s="12" t="s">
         <v>54</v>
       </c>
@@ -4817,37 +5227,57 @@
       <c r="K59" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L59" s="12"/>
+      <c r="L59" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M59" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="O59" s="20"/>
       <c r="P59" s="12"/>
       <c r="Q59" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R59" s="12"/>
+      <c r="R59" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S59" s="13"/>
       <c r="T59" s="14"/>
-    </row>
-    <row r="60" spans="2:32" ht="30">
+      <c r="U59"/>
+      <c r="V59"/>
+      <c r="W59"/>
+      <c r="X59"/>
+      <c r="Y59"/>
+      <c r="Z59"/>
+      <c r="AA59"/>
+      <c r="AB59"/>
+      <c r="AC59"/>
+      <c r="AD59"/>
+      <c r="AE59"/>
+      <c r="AF59"/>
+    </row>
+    <row r="60" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="11">
         <v>40837</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>128</v>
+        <v>218</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="E60" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
+      <c r="F60" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H60" s="12" t="s">
         <v>54</v>
       </c>
@@ -4858,37 +5288,57 @@
       <c r="K60" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L60" s="12"/>
+      <c r="L60" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M60" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="O60" s="20"/>
       <c r="P60" s="12"/>
       <c r="Q60" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R60" s="12"/>
+      <c r="R60" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S60" s="13"/>
       <c r="T60" s="14"/>
-    </row>
-    <row r="61" spans="2:32" ht="30">
+      <c r="U60"/>
+      <c r="V60"/>
+      <c r="W60"/>
+      <c r="X60"/>
+      <c r="Y60"/>
+      <c r="Z60"/>
+      <c r="AA60"/>
+      <c r="AB60"/>
+      <c r="AC60"/>
+      <c r="AD60"/>
+      <c r="AE60"/>
+      <c r="AF60"/>
+    </row>
+    <row r="61" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="11">
         <v>40837</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>127</v>
+        <v>218</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E61" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
+      <c r="F61" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H61" s="12" t="s">
         <v>54</v>
       </c>
@@ -4897,39 +5347,59 @@
       </c>
       <c r="J61" s="12"/>
       <c r="K61" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="L61" s="12"/>
+        <v>184</v>
+      </c>
+      <c r="L61" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M61" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="N61" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O61" s="20"/>
       <c r="P61" s="12"/>
       <c r="Q61" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R61" s="12"/>
+      <c r="R61" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S61" s="13"/>
       <c r="T61" s="14"/>
-    </row>
-    <row r="62" spans="2:32" ht="30">
+      <c r="U61"/>
+      <c r="V61"/>
+      <c r="W61"/>
+      <c r="X61"/>
+      <c r="Y61"/>
+      <c r="Z61"/>
+      <c r="AA61"/>
+      <c r="AB61"/>
+      <c r="AC61"/>
+      <c r="AD61"/>
+      <c r="AE61"/>
+      <c r="AF61"/>
+    </row>
+    <row r="62" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="11">
         <v>40837</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
+      <c r="F62" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H62" s="12" t="s">
         <v>54</v>
       </c>
@@ -4940,19 +5410,23 @@
       <c r="K62" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L62" s="12"/>
+      <c r="L62" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M62" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O62" s="20"/>
       <c r="P62" s="12"/>
       <c r="Q62" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R62" s="12"/>
+      <c r="R62" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S62" s="13"/>
       <c r="T62" s="14"/>
       <c r="U62"/>
@@ -4968,21 +5442,25 @@
       <c r="AE62"/>
       <c r="AF62"/>
     </row>
-    <row r="63" spans="2:32" ht="30">
+    <row r="63" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="11">
         <v>40837</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
+      <c r="F63" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H63" s="12" t="s">
         <v>54</v>
       </c>
@@ -4993,19 +5471,23 @@
       <c r="K63" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L63" s="12"/>
+      <c r="L63" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M63" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="O63" s="20"/>
+        <v>217</v>
+      </c>
+      <c r="O63" s="12"/>
       <c r="P63" s="12"/>
       <c r="Q63" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R63" s="12"/>
+      <c r="R63" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S63" s="13"/>
       <c r="T63" s="14"/>
       <c r="U63"/>
@@ -5021,21 +5503,25 @@
       <c r="AE63"/>
       <c r="AF63"/>
     </row>
-    <row r="64" spans="2:32" ht="30">
+    <row r="64" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" s="11">
         <v>40837</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E64" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
+      <c r="F64" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H64" s="12" t="s">
         <v>54</v>
       </c>
@@ -5046,19 +5532,23 @@
       <c r="K64" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L64" s="12"/>
+      <c r="L64" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M64" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="O64" s="20"/>
+        <v>217</v>
+      </c>
+      <c r="O64" s="12"/>
       <c r="P64" s="12"/>
       <c r="Q64" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R64" s="12"/>
+      <c r="R64" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S64" s="13"/>
       <c r="T64" s="14"/>
       <c r="U64"/>
@@ -5074,21 +5564,25 @@
       <c r="AE64"/>
       <c r="AF64"/>
     </row>
-    <row r="65" spans="2:32" ht="30">
+    <row r="65" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="11">
         <v>40837</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
+      <c r="F65" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H65" s="12" t="s">
         <v>54</v>
       </c>
@@ -5099,19 +5593,23 @@
       <c r="K65" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L65" s="12"/>
+      <c r="L65" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M65" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N65" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="O65" s="20"/>
+        <v>217</v>
+      </c>
+      <c r="O65" s="12"/>
       <c r="P65" s="12"/>
       <c r="Q65" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R65" s="12"/>
+      <c r="R65" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S65" s="13"/>
       <c r="T65" s="14"/>
       <c r="U65"/>
@@ -5127,21 +5625,25 @@
       <c r="AE65"/>
       <c r="AF65"/>
     </row>
-    <row r="66" spans="2:32" ht="30">
+    <row r="66" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="11">
         <v>40837</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E66" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
+      <c r="F66" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H66" s="12" t="s">
         <v>54</v>
       </c>
@@ -5152,19 +5654,23 @@
       <c r="K66" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L66" s="12"/>
+      <c r="L66" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M66" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O66" s="12"/>
       <c r="P66" s="12"/>
       <c r="Q66" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R66" s="12"/>
+      <c r="R66" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S66" s="13"/>
       <c r="T66" s="14"/>
       <c r="U66"/>
@@ -5180,21 +5686,25 @@
       <c r="AE66"/>
       <c r="AF66"/>
     </row>
-    <row r="67" spans="2:32" ht="30">
+    <row r="67" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="11">
         <v>40837</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E67" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
+      <c r="F67" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H67" s="12" t="s">
         <v>54</v>
       </c>
@@ -5205,19 +5715,23 @@
       <c r="K67" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L67" s="12"/>
+      <c r="L67" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M67" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N67" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O67" s="12"/>
       <c r="P67" s="12"/>
       <c r="Q67" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R67" s="12"/>
+      <c r="R67" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S67" s="13"/>
       <c r="T67" s="14"/>
       <c r="U67"/>
@@ -5233,46 +5747,58 @@
       <c r="AE67"/>
       <c r="AF67"/>
     </row>
-    <row r="68" spans="2:32" ht="30">
+    <row r="68" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="11">
         <v>40837</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H68" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I68" s="12" t="s">
         <v>67</v>
       </c>
       <c r="J68" s="12"/>
       <c r="K68" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="L68" s="12"/>
+        <v>230</v>
+      </c>
+      <c r="L68" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M68" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N68" s="12" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="O68" s="12"/>
       <c r="P68" s="12"/>
       <c r="Q68" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R68" s="12"/>
-      <c r="S68" s="13"/>
-      <c r="T68" s="14"/>
+      <c r="R68" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S68" s="13">
+        <v>40843</v>
+      </c>
+      <c r="T68" s="13">
+        <v>40843</v>
+      </c>
       <c r="U68"/>
       <c r="V68"/>
       <c r="W68"/>
@@ -5286,21 +5812,25 @@
       <c r="AE68"/>
       <c r="AF68"/>
     </row>
-    <row r="69" spans="2:32" ht="30">
+    <row r="69" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="11">
         <v>40837</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E69" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
+      <c r="F69" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H69" s="12" t="s">
         <v>54</v>
       </c>
@@ -5309,21 +5839,25 @@
       </c>
       <c r="J69" s="12"/>
       <c r="K69" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="L69" s="12"/>
+        <v>233</v>
+      </c>
+      <c r="L69" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M69" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N69" s="12" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="O69" s="12"/>
       <c r="P69" s="12"/>
       <c r="Q69" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R69" s="12"/>
+      <c r="R69" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S69" s="13"/>
       <c r="T69" s="14"/>
       <c r="U69"/>
@@ -5339,21 +5873,25 @@
       <c r="AE69"/>
       <c r="AF69"/>
     </row>
-    <row r="70" spans="2:32" ht="30">
+    <row r="70" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="11">
         <v>40837</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>229</v>
+        <v>231</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>235</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
+      <c r="F70" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H70" s="12" t="s">
         <v>54</v>
       </c>
@@ -5362,21 +5900,25 @@
       </c>
       <c r="J70" s="12"/>
       <c r="K70" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="L70" s="12"/>
+        <v>233</v>
+      </c>
+      <c r="L70" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M70" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="O70" s="12"/>
       <c r="P70" s="12"/>
       <c r="Q70" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R70" s="12"/>
+      <c r="R70" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S70" s="13"/>
       <c r="T70" s="14"/>
       <c r="U70"/>
@@ -5392,21 +5934,25 @@
       <c r="AE70"/>
       <c r="AF70"/>
     </row>
-    <row r="71" spans="2:32" ht="30">
+    <row r="71" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B71" s="11">
         <v>40837</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
+      <c r="F71" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H71" s="12" t="s">
         <v>54</v>
       </c>
@@ -5415,51 +5961,47 @@
       </c>
       <c r="J71" s="12"/>
       <c r="K71" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="L71" s="12"/>
+        <v>233</v>
+      </c>
+      <c r="L71" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M71" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>185</v>
+        <v>234</v>
       </c>
       <c r="O71" s="12"/>
       <c r="P71" s="12"/>
       <c r="Q71" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R71" s="12"/>
+      <c r="R71" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S71" s="13"/>
       <c r="T71" s="14"/>
-      <c r="U71"/>
-      <c r="V71"/>
-      <c r="W71"/>
-      <c r="X71"/>
-      <c r="Y71"/>
-      <c r="Z71"/>
-      <c r="AA71"/>
-      <c r="AB71"/>
-      <c r="AC71"/>
-      <c r="AD71"/>
-      <c r="AE71"/>
-      <c r="AF71"/>
-    </row>
-    <row r="72" spans="2:32" ht="30">
+    </row>
+    <row r="72" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="11">
         <v>40837</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
+      <c r="F72" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H72" s="12" t="s">
         <v>54</v>
       </c>
@@ -5468,51 +6010,47 @@
       </c>
       <c r="J72" s="12"/>
       <c r="K72" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="L72" s="12"/>
+        <v>233</v>
+      </c>
+      <c r="L72" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M72" s="12" t="s">
         <v>186</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O72" s="12"/>
       <c r="P72" s="12"/>
       <c r="Q72" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R72" s="12"/>
+      <c r="R72" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S72" s="13"/>
       <c r="T72" s="14"/>
-      <c r="U72"/>
-      <c r="V72"/>
-      <c r="W72"/>
-      <c r="X72"/>
-      <c r="Y72"/>
-      <c r="Z72"/>
-      <c r="AA72"/>
-      <c r="AB72"/>
-      <c r="AC72"/>
-      <c r="AD72"/>
-      <c r="AE72"/>
-      <c r="AF72"/>
-    </row>
-    <row r="73" spans="2:32" ht="30">
-      <c r="B73" s="11">
-        <v>40837</v>
+    </row>
+    <row r="73" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B73" s="11" t="s">
+        <v>238</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="D73" s="21" t="s">
-        <v>237</v>
+        <v>231</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>239</v>
       </c>
       <c r="E73" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
+      <c r="F73" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H73" s="12" t="s">
         <v>54</v>
       </c>
@@ -5521,51 +6059,49 @@
       </c>
       <c r="J73" s="12"/>
       <c r="K73" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="L73" s="12"/>
+        <v>184</v>
+      </c>
+      <c r="L73" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M73" s="12" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="N73" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O73" s="12"/>
       <c r="P73" s="12"/>
       <c r="Q73" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R73" s="12"/>
-      <c r="S73" s="13"/>
+      <c r="R73" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S73" s="13" t="s">
+        <v>238</v>
+      </c>
       <c r="T73" s="14"/>
-      <c r="U73"/>
-      <c r="V73"/>
-      <c r="W73"/>
-      <c r="X73"/>
-      <c r="Y73"/>
-      <c r="Z73"/>
-      <c r="AA73"/>
-      <c r="AB73"/>
-      <c r="AC73"/>
-      <c r="AD73"/>
-      <c r="AE73"/>
-      <c r="AF73"/>
-    </row>
-    <row r="74" spans="2:32" ht="30">
-      <c r="B74" s="11">
-        <v>40837</v>
+    </row>
+    <row r="74" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B74" s="11" t="s">
+        <v>238</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="E74" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
+      <c r="F74" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H74" s="12" t="s">
         <v>54</v>
       </c>
@@ -5574,39 +6110,49 @@
       </c>
       <c r="J74" s="12"/>
       <c r="K74" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="L74" s="12"/>
+        <v>184</v>
+      </c>
+      <c r="L74" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M74" s="12" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="N74" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O74" s="12"/>
       <c r="P74" s="12"/>
       <c r="Q74" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R74" s="12"/>
-      <c r="S74" s="13"/>
+      <c r="R74" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S74" s="13" t="s">
+        <v>238</v>
+      </c>
       <c r="T74" s="14"/>
     </row>
-    <row r="75" spans="2:32" ht="30">
-      <c r="B75" s="11">
-        <v>40837</v>
+    <row r="75" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="B75" s="11" t="s">
+        <v>238</v>
       </c>
       <c r="C75" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="D75" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>234</v>
       </c>
       <c r="E75" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
+      <c r="F75" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H75" s="12" t="s">
         <v>54</v>
       </c>
@@ -5615,39 +6161,49 @@
       </c>
       <c r="J75" s="12"/>
       <c r="K75" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="L75" s="12"/>
+        <v>184</v>
+      </c>
+      <c r="L75" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M75" s="12" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="N75" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O75" s="12"/>
       <c r="P75" s="12"/>
       <c r="Q75" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R75" s="12"/>
-      <c r="S75" s="13"/>
+      <c r="R75" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S75" s="13" t="s">
+        <v>238</v>
+      </c>
       <c r="T75" s="14"/>
     </row>
-    <row r="76" spans="2:32" ht="30">
+    <row r="76" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>233</v>
+        <v>128</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E76" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
+      <c r="F76" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H76" s="12" t="s">
         <v>54</v>
       </c>
@@ -5658,39 +6214,47 @@
       <c r="K76" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L76" s="12"/>
+      <c r="L76" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M76" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N76" s="12" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="O76" s="12"/>
       <c r="P76" s="12"/>
       <c r="Q76" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R76" s="12"/>
+      <c r="R76" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S76" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="T76" s="14"/>
     </row>
-    <row r="77" spans="2:32" ht="30">
+    <row r="77" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>242</v>
+        <v>128</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E77" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
+      <c r="F77" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G77" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H77" s="12" t="s">
         <v>54</v>
       </c>
@@ -5701,39 +6265,47 @@
       <c r="K77" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L77" s="12"/>
+      <c r="L77" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M77" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N77" s="12" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="O77" s="12"/>
       <c r="P77" s="12"/>
       <c r="Q77" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R77" s="12"/>
+      <c r="R77" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S77" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="T77" s="14"/>
     </row>
-    <row r="78" spans="2:32" ht="30">
+    <row r="78" spans="2:32" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>243</v>
+        <v>128</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E78" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
+      <c r="F78" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G78" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H78" s="12" t="s">
         <v>54</v>
       </c>
@@ -5744,154 +6316,92 @@
       <c r="K78" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="L78" s="12"/>
+      <c r="L78" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="M78" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N78" s="12" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="O78" s="12"/>
       <c r="P78" s="12"/>
       <c r="Q78" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="R78" s="12"/>
+      <c r="R78" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="S78" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="T78" s="14"/>
     </row>
-    <row r="79" spans="2:32" ht="30">
-      <c r="B79" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="C79" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D79" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>11</v>
-      </c>
+    <row r="79" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B79" s="11"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
       <c r="F79" s="12"/>
       <c r="G79" s="12"/>
-      <c r="H79" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I79" s="12" t="s">
-        <v>67</v>
-      </c>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
       <c r="J79" s="12"/>
-      <c r="K79" s="12" t="s">
-        <v>184</v>
-      </c>
+      <c r="K79" s="12"/>
       <c r="L79" s="12"/>
-      <c r="M79" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="N79" s="12" t="s">
-        <v>186</v>
-      </c>
+      <c r="M79" s="12"/>
+      <c r="N79" s="12"/>
       <c r="O79" s="12"/>
       <c r="P79" s="12"/>
-      <c r="Q79" s="12" t="s">
-        <v>156</v>
-      </c>
+      <c r="Q79" s="12"/>
       <c r="R79" s="12"/>
-      <c r="S79" s="13" t="s">
-        <v>240</v>
-      </c>
+      <c r="S79" s="13"/>
       <c r="T79" s="14"/>
     </row>
-    <row r="80" spans="2:32" ht="30">
-      <c r="B80" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="C80" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D80" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="E80" s="12" t="s">
-        <v>11</v>
-      </c>
+    <row r="80" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B80" s="11"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
       <c r="F80" s="12"/>
       <c r="G80" s="12"/>
-      <c r="H80" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I80" s="12" t="s">
-        <v>67</v>
-      </c>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
       <c r="J80" s="12"/>
-      <c r="K80" s="12" t="s">
-        <v>184</v>
-      </c>
+      <c r="K80" s="12"/>
       <c r="L80" s="12"/>
-      <c r="M80" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="N80" s="12" t="s">
-        <v>186</v>
-      </c>
+      <c r="M80" s="12"/>
+      <c r="N80" s="12"/>
       <c r="O80" s="12"/>
       <c r="P80" s="12"/>
-      <c r="Q80" s="12" t="s">
-        <v>156</v>
-      </c>
+      <c r="Q80" s="12"/>
       <c r="R80" s="12"/>
-      <c r="S80" s="13" t="s">
-        <v>240</v>
-      </c>
+      <c r="S80" s="13"/>
       <c r="T80" s="14"/>
     </row>
-    <row r="81" spans="2:20" ht="30">
-      <c r="B81" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="E81" s="12" t="s">
-        <v>11</v>
-      </c>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B81" s="11"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
-      <c r="H81" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I81" s="12" t="s">
-        <v>67</v>
-      </c>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
       <c r="J81" s="12"/>
-      <c r="K81" s="12" t="s">
-        <v>184</v>
-      </c>
+      <c r="K81" s="12"/>
       <c r="L81" s="12"/>
-      <c r="M81" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="N81" s="12" t="s">
-        <v>186</v>
-      </c>
+      <c r="M81" s="12"/>
+      <c r="N81" s="12"/>
       <c r="O81" s="12"/>
       <c r="P81" s="12"/>
-      <c r="Q81" s="12" t="s">
-        <v>156</v>
-      </c>
+      <c r="Q81" s="12"/>
       <c r="R81" s="12"/>
-      <c r="S81" s="13" t="s">
-        <v>240</v>
-      </c>
+      <c r="S81" s="13"/>
       <c r="T81" s="14"/>
     </row>
-    <row r="82" spans="2:20">
+    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B82" s="11"/>
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
@@ -5912,7 +6422,7 @@
       <c r="S82" s="13"/>
       <c r="T82" s="14"/>
     </row>
-    <row r="83" spans="2:20">
+    <row r="83" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B83" s="11"/>
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
@@ -5933,7 +6443,7 @@
       <c r="S83" s="13"/>
       <c r="T83" s="14"/>
     </row>
-    <row r="84" spans="2:20">
+    <row r="84" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B84" s="11"/>
       <c r="C84" s="12"/>
       <c r="D84" s="12"/>
@@ -5954,7 +6464,7 @@
       <c r="S84" s="13"/>
       <c r="T84" s="14"/>
     </row>
-    <row r="85" spans="2:20">
+    <row r="85" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B85" s="11"/>
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
@@ -5975,7 +6485,7 @@
       <c r="S85" s="13"/>
       <c r="T85" s="14"/>
     </row>
-    <row r="86" spans="2:20">
+    <row r="86" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B86" s="11"/>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
@@ -5996,7 +6506,7 @@
       <c r="S86" s="13"/>
       <c r="T86" s="14"/>
     </row>
-    <row r="87" spans="2:20">
+    <row r="87" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B87" s="11"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
@@ -6017,7 +6527,7 @@
       <c r="S87" s="13"/>
       <c r="T87" s="14"/>
     </row>
-    <row r="88" spans="2:20">
+    <row r="88" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B88" s="11"/>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
@@ -6038,7 +6548,7 @@
       <c r="S88" s="13"/>
       <c r="T88" s="14"/>
     </row>
-    <row r="89" spans="2:20">
+    <row r="89" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B89" s="11"/>
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
@@ -6059,7 +6569,7 @@
       <c r="S89" s="13"/>
       <c r="T89" s="14"/>
     </row>
-    <row r="90" spans="2:20">
+    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B90" s="11"/>
       <c r="C90" s="12"/>
       <c r="D90" s="12"/>
@@ -6080,7 +6590,7 @@
       <c r="S90" s="13"/>
       <c r="T90" s="14"/>
     </row>
-    <row r="91" spans="2:20">
+    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B91" s="11"/>
       <c r="C91" s="12"/>
       <c r="D91" s="12"/>
@@ -6101,7 +6611,7 @@
       <c r="S91" s="13"/>
       <c r="T91" s="14"/>
     </row>
-    <row r="92" spans="2:20">
+    <row r="92" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B92" s="11"/>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
@@ -6122,7 +6632,7 @@
       <c r="S92" s="13"/>
       <c r="T92" s="14"/>
     </row>
-    <row r="93" spans="2:20">
+    <row r="93" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B93" s="11"/>
       <c r="C93" s="12"/>
       <c r="D93" s="12"/>
@@ -6143,7 +6653,7 @@
       <c r="S93" s="13"/>
       <c r="T93" s="14"/>
     </row>
-    <row r="94" spans="2:20">
+    <row r="94" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B94" s="11"/>
       <c r="C94" s="12"/>
       <c r="D94" s="12"/>
@@ -6164,7 +6674,7 @@
       <c r="S94" s="13"/>
       <c r="T94" s="14"/>
     </row>
-    <row r="95" spans="2:20">
+    <row r="95" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B95" s="11"/>
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
@@ -6185,7 +6695,7 @@
       <c r="S95" s="13"/>
       <c r="T95" s="14"/>
     </row>
-    <row r="96" spans="2:20">
+    <row r="96" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B96" s="11"/>
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
@@ -6206,7 +6716,7 @@
       <c r="S96" s="13"/>
       <c r="T96" s="14"/>
     </row>
-    <row r="97" spans="2:20">
+    <row r="97" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B97" s="11"/>
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
@@ -6227,7 +6737,7 @@
       <c r="S97" s="13"/>
       <c r="T97" s="14"/>
     </row>
-    <row r="98" spans="2:20">
+    <row r="98" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B98" s="11"/>
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
@@ -6248,7 +6758,7 @@
       <c r="S98" s="13"/>
       <c r="T98" s="14"/>
     </row>
-    <row r="99" spans="2:20">
+    <row r="99" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B99" s="11"/>
       <c r="C99" s="12"/>
       <c r="D99" s="12"/>
@@ -6269,134 +6779,62 @@
       <c r="S99" s="13"/>
       <c r="T99" s="14"/>
     </row>
-    <row r="100" spans="2:20">
-      <c r="B100" s="11"/>
-      <c r="C100" s="12"/>
-      <c r="D100" s="12"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="12"/>
-      <c r="I100" s="12"/>
-      <c r="J100" s="12"/>
-      <c r="K100" s="12"/>
-      <c r="L100" s="12"/>
-      <c r="M100" s="12"/>
-      <c r="N100" s="12"/>
-      <c r="O100" s="12"/>
-      <c r="P100" s="12"/>
-      <c r="Q100" s="12"/>
-      <c r="R100" s="12"/>
-      <c r="S100" s="13"/>
-      <c r="T100" s="14"/>
-    </row>
-    <row r="101" spans="2:20">
-      <c r="B101" s="11"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="12"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
-      <c r="H101" s="12"/>
-      <c r="I101" s="12"/>
-      <c r="J101" s="12"/>
-      <c r="K101" s="12"/>
-      <c r="L101" s="12"/>
-      <c r="M101" s="12"/>
-      <c r="N101" s="12"/>
-      <c r="O101" s="12"/>
-      <c r="P101" s="12"/>
-      <c r="Q101" s="12"/>
-      <c r="R101" s="12"/>
-      <c r="S101" s="13"/>
-      <c r="T101" s="14"/>
-    </row>
-    <row r="102" spans="2:20">
-      <c r="B102" s="11"/>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-      <c r="G102" s="12"/>
-      <c r="H102" s="12"/>
-      <c r="I102" s="12"/>
-      <c r="J102" s="12"/>
-      <c r="K102" s="12"/>
-      <c r="L102" s="12"/>
-      <c r="M102" s="12"/>
-      <c r="N102" s="12"/>
-      <c r="O102" s="12"/>
-      <c r="P102" s="12"/>
-      <c r="Q102" s="12"/>
-      <c r="R102" s="12"/>
-      <c r="S102" s="13"/>
-      <c r="T102" s="14"/>
-    </row>
-    <row r="103" spans="2:20">
-      <c r="B103" s="16"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="17"/>
-      <c r="E103" s="17"/>
-      <c r="F103" s="17"/>
-      <c r="G103" s="17"/>
-      <c r="H103" s="17"/>
-      <c r="I103" s="17"/>
-      <c r="J103" s="17"/>
-      <c r="K103" s="17"/>
-      <c r="L103" s="17"/>
-      <c r="M103" s="17"/>
-      <c r="N103" s="17"/>
-      <c r="O103" s="17"/>
-      <c r="P103" s="17"/>
-      <c r="Q103" s="17"/>
-      <c r="R103" s="17"/>
-      <c r="S103" s="18"/>
-      <c r="T103" s="19"/>
+    <row r="100" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B100" s="16"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="17"/>
+      <c r="H100" s="17"/>
+      <c r="I100" s="17"/>
+      <c r="J100" s="17"/>
+      <c r="K100" s="17"/>
+      <c r="L100" s="17"/>
+      <c r="M100" s="17"/>
+      <c r="N100" s="17"/>
+      <c r="O100" s="17"/>
+      <c r="P100" s="17"/>
+      <c r="Q100" s="17"/>
+      <c r="R100" s="17"/>
+      <c r="S100" s="18"/>
+      <c r="T100" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="B4:T4"/>
-  <dataValidations count="14">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E27 E61:E75 E82:E103">
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H79:H100 H5:H72">
+      <formula1>$AA$7:$AA$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I79:I100 I5:I72">
+      <formula1>$AB$7:$AB$26</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J27 J60:J72 J79:J100">
+      <formula1>$AC$7:$AC$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R100">
+      <formula1>$AF$7:$AF$13</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H73:H78">
+      <formula1>$AA$5:$AA$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I73:I78">
+      <formula1>$AB$5:$AB$20</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J28:J59 J73:J78">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E100">
       <formula1>$X$7:$X$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F27 F63:F75 F82:F103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F100">
       <formula1>$Y$7:$Y$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G27 G63:G75 G82:G103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G100">
       <formula1>$Z$7:$Z$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H75 H82:H103">
-      <formula1>$AA$7:$AA$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I75 I82:I103">
-      <formula1>$AB$7:$AB$26</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J27 J63:J75 J82:J103">
-      <formula1>$AC$7:$AC$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L27 L63:L75 L82:L103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L100">
       <formula1>$AD$7:$AD$19</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R27 R63:R75 R82:R103">
-      <formula1>$AF$7:$AF$13</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F61:G62 R28:R62 L28:L62 J28:J62 E28:G60">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H76:H81">
-      <formula1>$AA$5:$AA$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I76:I81">
-      <formula1>$AB$5:$AB$20</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J76:J78 L76:L78 R76:R78 E76:G78">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J79:J81 L79:L81 R79:R80 E79:G80 E81">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R81 F81:G81">
-      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Design Form sheet
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -8,10 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Defect Log" sheetId="1" r:id="rId1"/>
+    <sheet name="Design Form" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Defect Log'!$B$4:$T$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Design Form'!$B$4:$T$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Defect Log'!$B$2:$T$100</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Design Form'!$B$2:$T$100</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -484,8 +487,475 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>HP</author>
+  </authors>
+  <commentList>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Created Date:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ngày viết Log</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Title:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tên Log</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Description:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mô tả Log.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Status:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tình trạng của Log</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>QC Activity:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Người viết Log phát hiện bug nhờ hành động nào.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Defect Origin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bug xảy ra do bước nào trong quy trình phát triển</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Priority:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tính cấp thiết của Bug (có phải sửa ngay hay không)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Product Type:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Loại sản phẩm chứa Bug.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Serverity:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mức độ nghiêm trọng của Bug</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Product:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sản phẩm chứa Bug.
+Lưu ý: ghi rõ file nào chứa bug, ở revision nào.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Type:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Phân loại bug.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Detected By:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Người phát hiện hoặc người viết Log.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Assigned To:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Người được giao việc sửa lỗi.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>DeadLine:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hạn chót phải sửa xong.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Corrective Action:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Phải sửa lỗi như thế nào. Nếu có thể xảy ra những lỗi tương tự ở các file khác thì đề nghị sửa luôn ở đây.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cause Analysis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Nguyên nhân gây ra lỗi.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Reason:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Loại nguyên nhân gây ra lỗi.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fixed Date:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ngày sửa xong.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Closed Date:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ngày đóng Bug.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="260">
   <si>
     <t>Project Code:</t>
   </si>
@@ -1275,6 +1745,9 @@
   </si>
   <si>
     <t>Thêm link to CreatedMenu_New_SeclectType</t>
+  </si>
+  <si>
+    <t>Fixed by</t>
   </si>
 </sst>
 </file>
@@ -1288,14 +1761,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1303,7 +1776,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1871,52 +2344,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AF100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B61" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="L1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="3" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="3"/>
+    <col min="4" max="4" width="67.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.125" style="3"/>
     <col min="9" max="9" width="21" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="34.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.125" style="3"/>
+    <col min="11" max="11" width="34.125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.25" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.75" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.75" style="3" customWidth="1"/>
     <col min="16" max="16" width="35" style="3" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="20.125" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" style="5" customWidth="1"/>
-    <col min="21" max="22" width="9.140625" style="3"/>
-    <col min="23" max="23" width="13.42578125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.375" style="5" customWidth="1"/>
+    <col min="21" max="22" width="9.125" style="3"/>
+    <col min="23" max="23" width="13.375" style="3" customWidth="1"/>
+    <col min="24" max="24" width="9.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.25" style="3" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" style="3"/>
-    <col min="30" max="30" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="3"/>
+    <col min="29" max="29" width="9.125" style="3"/>
+    <col min="30" max="30" width="22.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:32" x14ac:dyDescent="0.2">
       <c r="R1" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1925,7 +2398,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>129</v>
       </c>
@@ -1975,7 +2448,7 @@
         <v>7</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>9</v>
+        <v>259</v>
       </c>
       <c r="S4" s="8" t="s">
         <v>141</v>
@@ -1996,7 +2469,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="2:32" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B5" s="11">
         <v>40837</v>
       </c>
@@ -2053,7 +2526,7 @@
         <v>40838</v>
       </c>
     </row>
-    <row r="6" spans="2:32" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B6" s="11">
         <v>40837</v>
       </c>
@@ -2140,7 +2613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B7" s="11">
         <v>40837</v>
       </c>
@@ -2224,7 +2697,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B8" s="11">
         <v>40837</v>
       </c>
@@ -2308,7 +2781,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B9" s="11">
         <v>40837</v>
       </c>
@@ -2392,7 +2865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B10" s="11">
         <v>40837</v>
       </c>
@@ -2476,7 +2949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="11">
         <v>40837</v>
       </c>
@@ -2554,7 +3027,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B12" s="11">
         <v>40837</v>
       </c>
@@ -2632,7 +3105,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="11">
         <v>40837</v>
       </c>
@@ -2710,7 +3183,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -2749,7 +3222,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:32" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:32" ht="57" x14ac:dyDescent="0.2">
       <c r="B15" s="11">
         <v>40837</v>
       </c>
@@ -2824,7 +3297,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11">
         <v>40837</v>
       </c>
@@ -2896,7 +3369,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:31" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:31" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11">
         <v>40837</v>
       </c>
@@ -2968,7 +3441,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:31" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B18" s="11">
         <v>40837</v>
       </c>
@@ -3034,7 +3507,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="2:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="11">
         <v>40837</v>
       </c>
@@ -3100,7 +3573,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="2:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="11">
         <v>40837</v>
       </c>
@@ -3163,7 +3636,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:31" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:31" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="11">
         <v>40837</v>
       </c>
@@ -3226,7 +3699,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:31" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="11">
         <v>40837</v>
       </c>
@@ -3286,7 +3759,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="2:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="11">
         <v>40837</v>
       </c>
@@ -3346,7 +3819,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:31" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:31" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="11">
         <v>40837</v>
       </c>
@@ -3406,7 +3879,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:31" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B25" s="11">
         <v>40837</v>
       </c>
@@ -3466,7 +3939,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:31" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="11">
         <v>40837</v>
       </c>
@@ -3538,7 +4011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B27" s="11"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -3559,7 +4032,7 @@
       <c r="S27" s="13"/>
       <c r="T27" s="14"/>
     </row>
-    <row r="28" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:31" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B28" s="11">
         <v>40837</v>
       </c>
@@ -3612,7 +4085,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="29" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:31" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B29" s="11">
         <v>40837</v>
       </c>
@@ -3665,7 +4138,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="30" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:31" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B30" s="11">
         <v>40837</v>
       </c>
@@ -3718,7 +4191,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="31" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:31" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B31" s="11">
         <v>40837</v>
       </c>
@@ -3771,7 +4244,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="32" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:31" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B32" s="11">
         <v>40837</v>
       </c>
@@ -3824,7 +4297,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="33" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B33" s="11">
         <v>40837</v>
       </c>
@@ -3877,7 +4350,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="34" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B34" s="11">
         <v>40837</v>
       </c>
@@ -3930,7 +4403,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="35" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B35" s="11">
         <v>40837</v>
       </c>
@@ -3983,7 +4456,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="36" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B36" s="11">
         <v>40837</v>
       </c>
@@ -4036,7 +4509,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="37" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="11">
         <v>40837</v>
       </c>
@@ -4089,7 +4562,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="38" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="11">
         <v>40837</v>
       </c>
@@ -4142,7 +4615,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="39" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B39" s="11">
         <v>40837</v>
       </c>
@@ -4195,7 +4668,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="40" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B40" s="11">
         <v>40837</v>
       </c>
@@ -4248,7 +4721,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="41" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B41" s="11">
         <v>40837</v>
       </c>
@@ -4301,7 +4774,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="42" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B42" s="11">
         <v>40837</v>
       </c>
@@ -4354,7 +4827,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="43" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="11">
         <v>40837</v>
       </c>
@@ -4407,7 +4880,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="44" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="11">
         <v>40837</v>
       </c>
@@ -4460,7 +4933,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="45" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B45" s="11">
         <v>40837</v>
       </c>
@@ -4513,7 +4986,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="46" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B46" s="11">
         <v>40837</v>
       </c>
@@ -4566,7 +5039,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="47" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B47" s="11">
         <v>40837</v>
       </c>
@@ -4619,7 +5092,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="48" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B48" s="11">
         <v>40837</v>
       </c>
@@ -4672,7 +5145,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="49" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B49" s="11">
         <v>40837</v>
       </c>
@@ -4725,7 +5198,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="50" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B50" s="11">
         <v>40837</v>
       </c>
@@ -4778,7 +5251,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="51" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B51" s="11">
         <v>40837</v>
       </c>
@@ -4831,7 +5304,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="52" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B52" s="11">
         <v>40837</v>
       </c>
@@ -4884,7 +5357,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="53" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" s="11">
         <v>40837</v>
       </c>
@@ -4937,7 +5410,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="54" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B54" s="11">
         <v>40837</v>
       </c>
@@ -4990,7 +5463,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="55" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B55" s="11">
         <v>40837</v>
       </c>
@@ -5043,7 +5516,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="56" spans="2:32" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B56" s="11">
         <v>40837</v>
       </c>
@@ -5096,7 +5569,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="57" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B57" s="11">
         <v>40837</v>
       </c>
@@ -5149,7 +5622,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="58" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B58" s="11">
         <v>40837</v>
       </c>
@@ -5198,7 +5671,7 @@
       <c r="S58" s="13"/>
       <c r="T58" s="13"/>
     </row>
-    <row r="59" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="11">
         <v>40837</v>
       </c>
@@ -5259,7 +5732,7 @@
       <c r="AE59"/>
       <c r="AF59"/>
     </row>
-    <row r="60" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B60" s="11">
         <v>40837</v>
       </c>
@@ -5320,7 +5793,7 @@
       <c r="AE60"/>
       <c r="AF60"/>
     </row>
-    <row r="61" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B61" s="11">
         <v>40837</v>
       </c>
@@ -5381,7 +5854,7 @@
       <c r="AE61"/>
       <c r="AF61"/>
     </row>
-    <row r="62" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B62" s="11">
         <v>40837</v>
       </c>
@@ -5442,7 +5915,7 @@
       <c r="AE62"/>
       <c r="AF62"/>
     </row>
-    <row r="63" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B63" s="11">
         <v>40837</v>
       </c>
@@ -5503,7 +5976,7 @@
       <c r="AE63"/>
       <c r="AF63"/>
     </row>
-    <row r="64" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B64" s="11">
         <v>40837</v>
       </c>
@@ -5564,7 +6037,7 @@
       <c r="AE64"/>
       <c r="AF64"/>
     </row>
-    <row r="65" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B65" s="11">
         <v>40837</v>
       </c>
@@ -5625,7 +6098,7 @@
       <c r="AE65"/>
       <c r="AF65"/>
     </row>
-    <row r="66" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B66" s="11">
         <v>40837</v>
       </c>
@@ -5686,7 +6159,7 @@
       <c r="AE66"/>
       <c r="AF66"/>
     </row>
-    <row r="67" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B67" s="11">
         <v>40837</v>
       </c>
@@ -5747,7 +6220,7 @@
       <c r="AE67"/>
       <c r="AF67"/>
     </row>
-    <row r="68" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B68" s="11">
         <v>40837</v>
       </c>
@@ -5812,7 +6285,7 @@
       <c r="AE68"/>
       <c r="AF68"/>
     </row>
-    <row r="69" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B69" s="11">
         <v>40837</v>
       </c>
@@ -5873,7 +6346,7 @@
       <c r="AE69"/>
       <c r="AF69"/>
     </row>
-    <row r="70" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B70" s="11">
         <v>40837</v>
       </c>
@@ -5934,7 +6407,7 @@
       <c r="AE70"/>
       <c r="AF70"/>
     </row>
-    <row r="71" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B71" s="11">
         <v>40837</v>
       </c>
@@ -5983,7 +6456,7 @@
       <c r="S71" s="13"/>
       <c r="T71" s="14"/>
     </row>
-    <row r="72" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B72" s="11">
         <v>40837</v>
       </c>
@@ -6032,7 +6505,7 @@
       <c r="S72" s="13"/>
       <c r="T72" s="14"/>
     </row>
-    <row r="73" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B73" s="11" t="s">
         <v>238</v>
       </c>
@@ -6083,7 +6556,7 @@
       </c>
       <c r="T73" s="14"/>
     </row>
-    <row r="74" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B74" s="11" t="s">
         <v>238</v>
       </c>
@@ -6134,7 +6607,7 @@
       </c>
       <c r="T74" s="14"/>
     </row>
-    <row r="75" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B75" s="11" t="s">
         <v>238</v>
       </c>
@@ -6185,7 +6658,7 @@
       </c>
       <c r="T75" s="14"/>
     </row>
-    <row r="76" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B76" s="11" t="s">
         <v>238</v>
       </c>
@@ -6236,7 +6709,7 @@
       </c>
       <c r="T76" s="14"/>
     </row>
-    <row r="77" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B77" s="11" t="s">
         <v>238</v>
       </c>
@@ -6287,7 +6760,7 @@
       </c>
       <c r="T77" s="14"/>
     </row>
-    <row r="78" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:32" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B78" s="11" t="s">
         <v>238</v>
       </c>
@@ -6338,7 +6811,7 @@
       </c>
       <c r="T78" s="14"/>
     </row>
-    <row r="79" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B79" s="11"/>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
@@ -6359,7 +6832,7 @@
       <c r="S79" s="13"/>
       <c r="T79" s="14"/>
     </row>
-    <row r="80" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B80" s="11"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
@@ -6380,7 +6853,7 @@
       <c r="S80" s="13"/>
       <c r="T80" s="14"/>
     </row>
-    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B81" s="11"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
@@ -6401,7 +6874,7 @@
       <c r="S81" s="13"/>
       <c r="T81" s="14"/>
     </row>
-    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B82" s="11"/>
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
@@ -6422,7 +6895,7 @@
       <c r="S82" s="13"/>
       <c r="T82" s="14"/>
     </row>
-    <row r="83" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B83" s="11"/>
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
@@ -6443,7 +6916,7 @@
       <c r="S83" s="13"/>
       <c r="T83" s="14"/>
     </row>
-    <row r="84" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B84" s="11"/>
       <c r="C84" s="12"/>
       <c r="D84" s="12"/>
@@ -6464,7 +6937,7 @@
       <c r="S84" s="13"/>
       <c r="T84" s="14"/>
     </row>
-    <row r="85" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B85" s="11"/>
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
@@ -6485,7 +6958,7 @@
       <c r="S85" s="13"/>
       <c r="T85" s="14"/>
     </row>
-    <row r="86" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B86" s="11"/>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
@@ -6506,7 +6979,7 @@
       <c r="S86" s="13"/>
       <c r="T86" s="14"/>
     </row>
-    <row r="87" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B87" s="11"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
@@ -6527,7 +7000,7 @@
       <c r="S87" s="13"/>
       <c r="T87" s="14"/>
     </row>
-    <row r="88" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B88" s="11"/>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
@@ -6548,7 +7021,7 @@
       <c r="S88" s="13"/>
       <c r="T88" s="14"/>
     </row>
-    <row r="89" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B89" s="11"/>
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
@@ -6569,7 +7042,7 @@
       <c r="S89" s="13"/>
       <c r="T89" s="14"/>
     </row>
-    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B90" s="11"/>
       <c r="C90" s="12"/>
       <c r="D90" s="12"/>
@@ -6590,7 +7063,7 @@
       <c r="S90" s="13"/>
       <c r="T90" s="14"/>
     </row>
-    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B91" s="11"/>
       <c r="C91" s="12"/>
       <c r="D91" s="12"/>
@@ -6611,7 +7084,7 @@
       <c r="S91" s="13"/>
       <c r="T91" s="14"/>
     </row>
-    <row r="92" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B92" s="11"/>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
@@ -6632,7 +7105,7 @@
       <c r="S92" s="13"/>
       <c r="T92" s="14"/>
     </row>
-    <row r="93" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B93" s="11"/>
       <c r="C93" s="12"/>
       <c r="D93" s="12"/>
@@ -6653,7 +7126,7 @@
       <c r="S93" s="13"/>
       <c r="T93" s="14"/>
     </row>
-    <row r="94" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B94" s="11"/>
       <c r="C94" s="12"/>
       <c r="D94" s="12"/>
@@ -6674,7 +7147,7 @@
       <c r="S94" s="13"/>
       <c r="T94" s="14"/>
     </row>
-    <row r="95" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B95" s="11"/>
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
@@ -6695,7 +7168,7 @@
       <c r="S95" s="13"/>
       <c r="T95" s="14"/>
     </row>
-    <row r="96" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B96" s="11"/>
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
@@ -6716,7 +7189,7 @@
       <c r="S96" s="13"/>
       <c r="T96" s="14"/>
     </row>
-    <row r="97" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B97" s="11"/>
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
@@ -6737,7 +7210,7 @@
       <c r="S97" s="13"/>
       <c r="T97" s="14"/>
     </row>
-    <row r="98" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B98" s="11"/>
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
@@ -6758,7 +7231,7 @@
       <c r="S98" s="13"/>
       <c r="T98" s="14"/>
     </row>
-    <row r="99" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B99" s="11"/>
       <c r="C99" s="12"/>
       <c r="D99" s="12"/>
@@ -6779,7 +7252,7 @@
       <c r="S99" s="13"/>
       <c r="T99" s="14"/>
     </row>
-    <row r="100" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B100" s="16"/>
       <c r="C100" s="17"/>
       <c r="D100" s="17"/>
@@ -6844,4 +7317,2349 @@
   </colBreaks>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AF100"/>
+  <sheetViews>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="G1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="3" customWidth="1"/>
+    <col min="4" max="4" width="67.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.125" style="3"/>
+    <col min="9" max="9" width="21" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.125" style="3"/>
+    <col min="11" max="11" width="34.125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.25" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.75" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.75" style="3" customWidth="1"/>
+    <col min="16" max="16" width="35" style="3" customWidth="1"/>
+    <col min="17" max="17" width="14.125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="20.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.375" style="5" customWidth="1"/>
+    <col min="21" max="22" width="9.125" style="3"/>
+    <col min="23" max="23" width="13.375" style="3" customWidth="1"/>
+    <col min="24" max="24" width="9.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="27" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.125" style="3"/>
+    <col min="30" max="30" width="22.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="R1" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="4" spans="2:32" s="10" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="14"/>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="14"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="15"/>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="14"/>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="14"/>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="14"/>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="14"/>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="14"/>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="14"/>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="14"/>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="14"/>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="14"/>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="14"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="14"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="14"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="14"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="14"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="14"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="14"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="14"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="14"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="14"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="14"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="14"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B28" s="11"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="14"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="14"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="14"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="14"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B32" s="11"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="14"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B33" s="11"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="14"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="14"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="14"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="14"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="14"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="14"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B39" s="11"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="14"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B40" s="11"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="14"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B41" s="11"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="14"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="12"/>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="14"/>
+    </row>
+    <row r="43" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="11"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="12"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="14"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B44" s="11"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="14"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="20"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="14"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B46" s="11"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="20"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="14"/>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B47" s="11"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="14"/>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B48" s="11"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="14"/>
+    </row>
+    <row r="49" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B49" s="11"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+      <c r="N49" s="12"/>
+      <c r="O49" s="20"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="14"/>
+    </row>
+    <row r="50" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B50" s="11"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="20"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+      <c r="S50" s="13"/>
+      <c r="T50" s="14"/>
+    </row>
+    <row r="51" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B51" s="11"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+      <c r="S51" s="13"/>
+      <c r="T51" s="14"/>
+    </row>
+    <row r="52" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B52" s="11"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="20"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+      <c r="S52" s="13"/>
+      <c r="T52" s="14"/>
+    </row>
+    <row r="53" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B53" s="11"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="20"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12"/>
+      <c r="S53" s="13"/>
+      <c r="T53" s="14"/>
+    </row>
+    <row r="54" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B54" s="11"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="12"/>
+      <c r="Q54" s="12"/>
+      <c r="R54" s="12"/>
+      <c r="S54" s="13"/>
+      <c r="T54" s="14"/>
+    </row>
+    <row r="55" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B55" s="11"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="12"/>
+      <c r="S55" s="13"/>
+      <c r="T55" s="14"/>
+    </row>
+    <row r="56" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B56" s="11"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="20"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12"/>
+      <c r="S56" s="13"/>
+      <c r="T56" s="14"/>
+    </row>
+    <row r="57" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B57" s="11"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
+      <c r="O57" s="20"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="12"/>
+      <c r="S57" s="13"/>
+      <c r="T57" s="14"/>
+    </row>
+    <row r="58" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B58" s="11"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="12"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12"/>
+      <c r="R58" s="12"/>
+      <c r="S58" s="13"/>
+      <c r="T58" s="14"/>
+    </row>
+    <row r="59" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B59" s="11"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+      <c r="L59" s="12"/>
+      <c r="M59" s="12"/>
+      <c r="N59" s="12"/>
+      <c r="O59" s="20"/>
+      <c r="P59" s="12"/>
+      <c r="Q59" s="12"/>
+      <c r="R59" s="12"/>
+      <c r="S59" s="13"/>
+      <c r="T59" s="14"/>
+      <c r="U59"/>
+      <c r="V59"/>
+      <c r="W59"/>
+      <c r="X59"/>
+      <c r="Y59"/>
+      <c r="Z59"/>
+      <c r="AA59"/>
+      <c r="AB59"/>
+      <c r="AC59"/>
+      <c r="AD59"/>
+      <c r="AE59"/>
+      <c r="AF59"/>
+    </row>
+    <row r="60" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B60" s="11"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="20"/>
+      <c r="P60" s="12"/>
+      <c r="Q60" s="12"/>
+      <c r="R60" s="12"/>
+      <c r="S60" s="13"/>
+      <c r="T60" s="14"/>
+      <c r="U60"/>
+      <c r="V60"/>
+      <c r="W60"/>
+      <c r="X60"/>
+      <c r="Y60"/>
+      <c r="Z60"/>
+      <c r="AA60"/>
+      <c r="AB60"/>
+      <c r="AC60"/>
+      <c r="AD60"/>
+      <c r="AE60"/>
+      <c r="AF60"/>
+    </row>
+    <row r="61" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B61" s="11"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
+      <c r="M61" s="12"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="20"/>
+      <c r="P61" s="12"/>
+      <c r="Q61" s="12"/>
+      <c r="R61" s="12"/>
+      <c r="S61" s="13"/>
+      <c r="T61" s="14"/>
+      <c r="U61"/>
+      <c r="V61"/>
+      <c r="W61"/>
+      <c r="X61"/>
+      <c r="Y61"/>
+      <c r="Z61"/>
+      <c r="AA61"/>
+      <c r="AB61"/>
+      <c r="AC61"/>
+      <c r="AD61"/>
+      <c r="AE61"/>
+      <c r="AF61"/>
+    </row>
+    <row r="62" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B62" s="11"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="12"/>
+      <c r="Q62" s="12"/>
+      <c r="R62" s="12"/>
+      <c r="S62" s="13"/>
+      <c r="T62" s="14"/>
+      <c r="U62"/>
+      <c r="V62"/>
+      <c r="W62"/>
+      <c r="X62"/>
+      <c r="Y62"/>
+      <c r="Z62"/>
+      <c r="AA62"/>
+      <c r="AB62"/>
+      <c r="AC62"/>
+      <c r="AD62"/>
+      <c r="AE62"/>
+      <c r="AF62"/>
+    </row>
+    <row r="63" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B63" s="11"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="20"/>
+      <c r="P63" s="12"/>
+      <c r="Q63" s="12"/>
+      <c r="R63" s="12"/>
+      <c r="S63" s="13"/>
+      <c r="T63" s="14"/>
+      <c r="U63"/>
+      <c r="V63"/>
+      <c r="W63"/>
+      <c r="X63"/>
+      <c r="Y63"/>
+      <c r="Z63"/>
+      <c r="AA63"/>
+      <c r="AB63"/>
+      <c r="AC63"/>
+      <c r="AD63"/>
+      <c r="AE63"/>
+      <c r="AF63"/>
+    </row>
+    <row r="64" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B64" s="11"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="20"/>
+      <c r="P64" s="12"/>
+      <c r="Q64" s="12"/>
+      <c r="R64" s="12"/>
+      <c r="S64" s="13"/>
+      <c r="T64" s="14"/>
+      <c r="U64"/>
+      <c r="V64"/>
+      <c r="W64"/>
+      <c r="X64"/>
+      <c r="Y64"/>
+      <c r="Z64"/>
+      <c r="AA64"/>
+      <c r="AB64"/>
+      <c r="AC64"/>
+      <c r="AD64"/>
+      <c r="AE64"/>
+      <c r="AF64"/>
+    </row>
+    <row r="65" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B65" s="11"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="20"/>
+      <c r="P65" s="12"/>
+      <c r="Q65" s="12"/>
+      <c r="R65" s="12"/>
+      <c r="S65" s="13"/>
+      <c r="T65" s="14"/>
+      <c r="U65"/>
+      <c r="V65"/>
+      <c r="W65"/>
+      <c r="X65"/>
+      <c r="Y65"/>
+      <c r="Z65"/>
+      <c r="AA65"/>
+      <c r="AB65"/>
+      <c r="AC65"/>
+      <c r="AD65"/>
+      <c r="AE65"/>
+      <c r="AF65"/>
+    </row>
+    <row r="66" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B66" s="11"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12"/>
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="20"/>
+      <c r="P66" s="12"/>
+      <c r="Q66" s="12"/>
+      <c r="R66" s="12"/>
+      <c r="S66" s="13"/>
+      <c r="T66" s="14"/>
+      <c r="U66"/>
+      <c r="V66"/>
+      <c r="W66"/>
+      <c r="X66"/>
+      <c r="Y66"/>
+      <c r="Z66"/>
+      <c r="AA66"/>
+      <c r="AB66"/>
+      <c r="AC66"/>
+      <c r="AD66"/>
+      <c r="AE66"/>
+      <c r="AF66"/>
+    </row>
+    <row r="67" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B67" s="11"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="12"/>
+      <c r="M67" s="12"/>
+      <c r="N67" s="12"/>
+      <c r="O67" s="20"/>
+      <c r="P67" s="12"/>
+      <c r="Q67" s="12"/>
+      <c r="R67" s="12"/>
+      <c r="S67" s="13"/>
+      <c r="T67" s="14"/>
+      <c r="U67"/>
+      <c r="V67"/>
+      <c r="W67"/>
+      <c r="X67"/>
+      <c r="Y67"/>
+      <c r="Z67"/>
+      <c r="AA67"/>
+      <c r="AB67"/>
+      <c r="AC67"/>
+      <c r="AD67"/>
+      <c r="AE67"/>
+      <c r="AF67"/>
+    </row>
+    <row r="68" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B68" s="11"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="12"/>
+      <c r="M68" s="12"/>
+      <c r="N68" s="12"/>
+      <c r="O68" s="20"/>
+      <c r="P68" s="12"/>
+      <c r="Q68" s="12"/>
+      <c r="R68" s="12"/>
+      <c r="S68" s="13"/>
+      <c r="T68" s="14"/>
+      <c r="U68"/>
+      <c r="V68"/>
+      <c r="W68"/>
+      <c r="X68"/>
+      <c r="Y68"/>
+      <c r="Z68"/>
+      <c r="AA68"/>
+      <c r="AB68"/>
+      <c r="AC68"/>
+      <c r="AD68"/>
+      <c r="AE68"/>
+      <c r="AF68"/>
+    </row>
+    <row r="69" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B69" s="11"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="12"/>
+      <c r="M69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="20"/>
+      <c r="P69" s="12"/>
+      <c r="Q69" s="12"/>
+      <c r="R69" s="12"/>
+      <c r="S69" s="13"/>
+      <c r="T69" s="14"/>
+      <c r="U69"/>
+      <c r="V69"/>
+      <c r="W69"/>
+      <c r="X69"/>
+      <c r="Y69"/>
+      <c r="Z69"/>
+      <c r="AA69"/>
+      <c r="AB69"/>
+      <c r="AC69"/>
+      <c r="AD69"/>
+      <c r="AE69"/>
+      <c r="AF69"/>
+    </row>
+    <row r="70" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B70" s="11"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="12"/>
+      <c r="M70" s="12"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="20"/>
+      <c r="P70" s="12"/>
+      <c r="Q70" s="12"/>
+      <c r="R70" s="12"/>
+      <c r="S70" s="13"/>
+      <c r="T70" s="14"/>
+      <c r="U70"/>
+      <c r="V70"/>
+      <c r="W70"/>
+      <c r="X70"/>
+      <c r="Y70"/>
+      <c r="Z70"/>
+      <c r="AA70"/>
+      <c r="AB70"/>
+      <c r="AC70"/>
+      <c r="AD70"/>
+      <c r="AE70"/>
+      <c r="AF70"/>
+    </row>
+    <row r="71" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B71" s="11"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="12"/>
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="20"/>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="12"/>
+      <c r="R71" s="12"/>
+      <c r="S71" s="13"/>
+      <c r="T71" s="14"/>
+    </row>
+    <row r="72" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B72" s="11"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
+      <c r="L72" s="12"/>
+      <c r="M72" s="12"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="20"/>
+      <c r="P72" s="12"/>
+      <c r="Q72" s="12"/>
+      <c r="R72" s="12"/>
+      <c r="S72" s="13"/>
+      <c r="T72" s="14"/>
+    </row>
+    <row r="73" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B73" s="11"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="12"/>
+      <c r="K73" s="12"/>
+      <c r="L73" s="12"/>
+      <c r="M73" s="12"/>
+      <c r="N73" s="12"/>
+      <c r="O73" s="20"/>
+      <c r="P73" s="12"/>
+      <c r="Q73" s="12"/>
+      <c r="R73" s="12"/>
+      <c r="S73" s="13"/>
+      <c r="T73" s="14"/>
+    </row>
+    <row r="74" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B74" s="11"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
+      <c r="L74" s="12"/>
+      <c r="M74" s="12"/>
+      <c r="N74" s="12"/>
+      <c r="O74" s="20"/>
+      <c r="P74" s="12"/>
+      <c r="Q74" s="12"/>
+      <c r="R74" s="12"/>
+      <c r="S74" s="13"/>
+      <c r="T74" s="14"/>
+    </row>
+    <row r="75" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B75" s="11"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="12"/>
+      <c r="K75" s="12"/>
+      <c r="L75" s="12"/>
+      <c r="M75" s="12"/>
+      <c r="N75" s="12"/>
+      <c r="O75" s="12"/>
+      <c r="P75" s="12"/>
+      <c r="Q75" s="12"/>
+      <c r="R75" s="12"/>
+      <c r="S75" s="13"/>
+      <c r="T75" s="14"/>
+    </row>
+    <row r="76" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B76" s="11"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12"/>
+      <c r="M76" s="12"/>
+      <c r="N76" s="12"/>
+      <c r="O76" s="12"/>
+      <c r="P76" s="12"/>
+      <c r="Q76" s="12"/>
+      <c r="R76" s="12"/>
+      <c r="S76" s="13"/>
+      <c r="T76" s="14"/>
+    </row>
+    <row r="77" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B77" s="11"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="12"/>
+      <c r="K77" s="12"/>
+      <c r="L77" s="12"/>
+      <c r="M77" s="12"/>
+      <c r="N77" s="12"/>
+      <c r="O77" s="12"/>
+      <c r="P77" s="12"/>
+      <c r="Q77" s="12"/>
+      <c r="R77" s="12"/>
+      <c r="S77" s="13"/>
+      <c r="T77" s="14"/>
+    </row>
+    <row r="78" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B78" s="11"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="12"/>
+      <c r="K78" s="12"/>
+      <c r="L78" s="12"/>
+      <c r="M78" s="12"/>
+      <c r="N78" s="12"/>
+      <c r="O78" s="12"/>
+      <c r="P78" s="12"/>
+      <c r="Q78" s="12"/>
+      <c r="R78" s="12"/>
+      <c r="S78" s="13"/>
+      <c r="T78" s="14"/>
+    </row>
+    <row r="79" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B79" s="11"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
+      <c r="K79" s="12"/>
+      <c r="L79" s="12"/>
+      <c r="M79" s="12"/>
+      <c r="N79" s="12"/>
+      <c r="O79" s="12"/>
+      <c r="P79" s="12"/>
+      <c r="Q79" s="12"/>
+      <c r="R79" s="12"/>
+      <c r="S79" s="13"/>
+      <c r="T79" s="14"/>
+    </row>
+    <row r="80" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B80" s="11"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="12"/>
+      <c r="K80" s="12"/>
+      <c r="L80" s="12"/>
+      <c r="M80" s="12"/>
+      <c r="N80" s="12"/>
+      <c r="O80" s="12"/>
+      <c r="P80" s="12"/>
+      <c r="Q80" s="12"/>
+      <c r="R80" s="12"/>
+      <c r="S80" s="13"/>
+      <c r="T80" s="14"/>
+    </row>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B81" s="11"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="12"/>
+      <c r="K81" s="12"/>
+      <c r="L81" s="12"/>
+      <c r="M81" s="12"/>
+      <c r="N81" s="12"/>
+      <c r="O81" s="12"/>
+      <c r="P81" s="12"/>
+      <c r="Q81" s="12"/>
+      <c r="R81" s="12"/>
+      <c r="S81" s="13"/>
+      <c r="T81" s="14"/>
+    </row>
+    <row r="82" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B82" s="11"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="12"/>
+      <c r="K82" s="12"/>
+      <c r="L82" s="12"/>
+      <c r="M82" s="12"/>
+      <c r="N82" s="12"/>
+      <c r="O82" s="12"/>
+      <c r="P82" s="12"/>
+      <c r="Q82" s="12"/>
+      <c r="R82" s="12"/>
+      <c r="S82" s="13"/>
+      <c r="T82" s="14"/>
+    </row>
+    <row r="83" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B83" s="11"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="12"/>
+      <c r="K83" s="12"/>
+      <c r="L83" s="12"/>
+      <c r="M83" s="12"/>
+      <c r="N83" s="12"/>
+      <c r="O83" s="12"/>
+      <c r="P83" s="12"/>
+      <c r="Q83" s="12"/>
+      <c r="R83" s="12"/>
+      <c r="S83" s="13"/>
+      <c r="T83" s="14"/>
+    </row>
+    <row r="84" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B84" s="11"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
+      <c r="L84" s="12"/>
+      <c r="M84" s="12"/>
+      <c r="N84" s="12"/>
+      <c r="O84" s="12"/>
+      <c r="P84" s="12"/>
+      <c r="Q84" s="12"/>
+      <c r="R84" s="12"/>
+      <c r="S84" s="13"/>
+      <c r="T84" s="14"/>
+    </row>
+    <row r="85" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B85" s="11"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="12"/>
+      <c r="K85" s="12"/>
+      <c r="L85" s="12"/>
+      <c r="M85" s="12"/>
+      <c r="N85" s="12"/>
+      <c r="O85" s="12"/>
+      <c r="P85" s="12"/>
+      <c r="Q85" s="12"/>
+      <c r="R85" s="12"/>
+      <c r="S85" s="13"/>
+      <c r="T85" s="14"/>
+    </row>
+    <row r="86" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B86" s="11"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12"/>
+      <c r="J86" s="12"/>
+      <c r="K86" s="12"/>
+      <c r="L86" s="12"/>
+      <c r="M86" s="12"/>
+      <c r="N86" s="12"/>
+      <c r="O86" s="12"/>
+      <c r="P86" s="12"/>
+      <c r="Q86" s="12"/>
+      <c r="R86" s="12"/>
+      <c r="S86" s="13"/>
+      <c r="T86" s="14"/>
+    </row>
+    <row r="87" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B87" s="11"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="12"/>
+      <c r="J87" s="12"/>
+      <c r="K87" s="12"/>
+      <c r="L87" s="12"/>
+      <c r="M87" s="12"/>
+      <c r="N87" s="12"/>
+      <c r="O87" s="12"/>
+      <c r="P87" s="12"/>
+      <c r="Q87" s="12"/>
+      <c r="R87" s="12"/>
+      <c r="S87" s="13"/>
+      <c r="T87" s="14"/>
+    </row>
+    <row r="88" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B88" s="11"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="12"/>
+      <c r="J88" s="12"/>
+      <c r="K88" s="12"/>
+      <c r="L88" s="12"/>
+      <c r="M88" s="12"/>
+      <c r="N88" s="12"/>
+      <c r="O88" s="12"/>
+      <c r="P88" s="12"/>
+      <c r="Q88" s="12"/>
+      <c r="R88" s="12"/>
+      <c r="S88" s="13"/>
+      <c r="T88" s="14"/>
+    </row>
+    <row r="89" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B89" s="11"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="12"/>
+      <c r="I89" s="12"/>
+      <c r="J89" s="12"/>
+      <c r="K89" s="12"/>
+      <c r="L89" s="12"/>
+      <c r="M89" s="12"/>
+      <c r="N89" s="12"/>
+      <c r="O89" s="12"/>
+      <c r="P89" s="12"/>
+      <c r="Q89" s="12"/>
+      <c r="R89" s="12"/>
+      <c r="S89" s="13"/>
+      <c r="T89" s="14"/>
+    </row>
+    <row r="90" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B90" s="11"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="12"/>
+      <c r="I90" s="12"/>
+      <c r="J90" s="12"/>
+      <c r="K90" s="12"/>
+      <c r="L90" s="12"/>
+      <c r="M90" s="12"/>
+      <c r="N90" s="12"/>
+      <c r="O90" s="12"/>
+      <c r="P90" s="12"/>
+      <c r="Q90" s="12"/>
+      <c r="R90" s="12"/>
+      <c r="S90" s="13"/>
+      <c r="T90" s="14"/>
+    </row>
+    <row r="91" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B91" s="11"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="12"/>
+      <c r="J91" s="12"/>
+      <c r="K91" s="12"/>
+      <c r="L91" s="12"/>
+      <c r="M91" s="12"/>
+      <c r="N91" s="12"/>
+      <c r="O91" s="12"/>
+      <c r="P91" s="12"/>
+      <c r="Q91" s="12"/>
+      <c r="R91" s="12"/>
+      <c r="S91" s="13"/>
+      <c r="T91" s="14"/>
+    </row>
+    <row r="92" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B92" s="11"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="12"/>
+      <c r="J92" s="12"/>
+      <c r="K92" s="12"/>
+      <c r="L92" s="12"/>
+      <c r="M92" s="12"/>
+      <c r="N92" s="12"/>
+      <c r="O92" s="12"/>
+      <c r="P92" s="12"/>
+      <c r="Q92" s="12"/>
+      <c r="R92" s="12"/>
+      <c r="S92" s="13"/>
+      <c r="T92" s="14"/>
+    </row>
+    <row r="93" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B93" s="11"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="12"/>
+      <c r="J93" s="12"/>
+      <c r="K93" s="12"/>
+      <c r="L93" s="12"/>
+      <c r="M93" s="12"/>
+      <c r="N93" s="12"/>
+      <c r="O93" s="12"/>
+      <c r="P93" s="12"/>
+      <c r="Q93" s="12"/>
+      <c r="R93" s="12"/>
+      <c r="S93" s="13"/>
+      <c r="T93" s="14"/>
+    </row>
+    <row r="94" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B94" s="11"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="12"/>
+      <c r="J94" s="12"/>
+      <c r="K94" s="12"/>
+      <c r="L94" s="12"/>
+      <c r="M94" s="12"/>
+      <c r="N94" s="12"/>
+      <c r="O94" s="12"/>
+      <c r="P94" s="12"/>
+      <c r="Q94" s="12"/>
+      <c r="R94" s="12"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="14"/>
+    </row>
+    <row r="95" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B95" s="11"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="12"/>
+      <c r="K95" s="12"/>
+      <c r="L95" s="12"/>
+      <c r="M95" s="12"/>
+      <c r="N95" s="12"/>
+      <c r="O95" s="12"/>
+      <c r="P95" s="12"/>
+      <c r="Q95" s="12"/>
+      <c r="R95" s="12"/>
+      <c r="S95" s="13"/>
+      <c r="T95" s="14"/>
+    </row>
+    <row r="96" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B96" s="11"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12"/>
+      <c r="I96" s="12"/>
+      <c r="J96" s="12"/>
+      <c r="K96" s="12"/>
+      <c r="L96" s="12"/>
+      <c r="M96" s="12"/>
+      <c r="N96" s="12"/>
+      <c r="O96" s="12"/>
+      <c r="P96" s="12"/>
+      <c r="Q96" s="12"/>
+      <c r="R96" s="12"/>
+      <c r="S96" s="13"/>
+      <c r="T96" s="14"/>
+    </row>
+    <row r="97" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B97" s="11"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
+      <c r="L97" s="12"/>
+      <c r="M97" s="12"/>
+      <c r="N97" s="12"/>
+      <c r="O97" s="12"/>
+      <c r="P97" s="12"/>
+      <c r="Q97" s="12"/>
+      <c r="R97" s="12"/>
+      <c r="S97" s="13"/>
+      <c r="T97" s="14"/>
+    </row>
+    <row r="98" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B98" s="11"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+      <c r="I98" s="12"/>
+      <c r="J98" s="12"/>
+      <c r="K98" s="12"/>
+      <c r="L98" s="12"/>
+      <c r="M98" s="12"/>
+      <c r="N98" s="12"/>
+      <c r="O98" s="12"/>
+      <c r="P98" s="12"/>
+      <c r="Q98" s="12"/>
+      <c r="R98" s="12"/>
+      <c r="S98" s="13"/>
+      <c r="T98" s="14"/>
+    </row>
+    <row r="99" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B99" s="11"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="12"/>
+      <c r="I99" s="12"/>
+      <c r="J99" s="12"/>
+      <c r="K99" s="12"/>
+      <c r="L99" s="12"/>
+      <c r="M99" s="12"/>
+      <c r="N99" s="12"/>
+      <c r="O99" s="12"/>
+      <c r="P99" s="12"/>
+      <c r="Q99" s="12"/>
+      <c r="R99" s="12"/>
+      <c r="S99" s="13"/>
+      <c r="T99" s="14"/>
+    </row>
+    <row r="100" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B100" s="16"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="17"/>
+      <c r="H100" s="17"/>
+      <c r="I100" s="17"/>
+      <c r="J100" s="17"/>
+      <c r="K100" s="17"/>
+      <c r="L100" s="17"/>
+      <c r="M100" s="17"/>
+      <c r="N100" s="17"/>
+      <c r="O100" s="17"/>
+      <c r="P100" s="17"/>
+      <c r="Q100" s="17"/>
+      <c r="R100" s="17"/>
+      <c r="S100" s="18"/>
+      <c r="T100" s="19"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B4:T4"/>
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L100">
+      <formula1>$AD$7:$AD$19</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G100">
+      <formula1>$Z$7:$Z$15</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F100">
+      <formula1>$Y$7:$Y$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E100">
+      <formula1>$X$7:$X$17</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J28:J59 J73:J78">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I73:I78">
+      <formula1>$AB$5:$AB$20</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H73:H78">
+      <formula1>$AA$5:$AA$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R100">
+      <formula1>$AF$7:$AF$13</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J27 J60:J72 J79:J100">
+      <formula1>$AC$7:$AC$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I79:I100 I5:I72">
+      <formula1>$AB$7:$AB$26</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H79:H100 H5:H72">
+      <formula1>$AA$7:$AA$10</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="62" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="9" min="1" max="53" man="1"/>
+  </colBreaks>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Sheet Mode into file Defect Log.xlsx
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="8580" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="8580" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Defect Log" sheetId="1" r:id="rId1"/>
-    <sheet name="Design Form" sheetId="5" r:id="rId2"/>
+    <sheet name="Design Form" sheetId="5" r:id="rId1"/>
+    <sheet name="Defect Log" sheetId="1" r:id="rId2"/>
+    <sheet name="Model" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Defect Log'!$B$4:$T$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Design Form'!$B$4:$T$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Defect Log'!$B$2:$T$100</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Design Form'!$B$2:$T$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Defect Log'!$B$4:$T$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Design Form'!$B$4:$T$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Model!$B$4:$T$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Defect Log'!$B$2:$T$100</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Design Form'!$B$2:$T$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Model!$B$2:$T$54</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -34,7 +37,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Created Date:</t>
         </r>
@@ -43,7 +47,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Ngày viết Log</t>
@@ -58,7 +63,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Title:</t>
         </r>
@@ -67,7 +73,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Tên Log</t>
@@ -82,7 +89,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Description:</t>
         </r>
@@ -91,7 +99,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Mô tả Log.</t>
@@ -106,7 +115,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Status:</t>
         </r>
@@ -115,7 +125,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Tình trạng của Log</t>
@@ -130,7 +141,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>QC Activity:</t>
         </r>
@@ -139,7 +151,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Người viết Log phát hiện bug nhờ hành động nào.</t>
@@ -154,7 +167,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Defect Origin:</t>
         </r>
@@ -163,7 +177,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Bug xảy ra do bước nào trong quy trình phát triển</t>
@@ -178,7 +193,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Priority:</t>
         </r>
@@ -187,7 +203,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Tính cấp thiết của Bug (có phải sửa ngay hay không)</t>
@@ -202,7 +219,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Product Type:</t>
         </r>
@@ -211,7 +229,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Loại sản phẩm chứa Bug.</t>
@@ -226,7 +245,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Serverity:</t>
         </r>
@@ -235,7 +255,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Mức độ nghiêm trọng của Bug</t>
@@ -250,7 +271,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Product:</t>
         </r>
@@ -259,7 +281,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Sản phẩm chứa Bug.
@@ -275,7 +298,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Type:</t>
         </r>
@@ -284,7 +308,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Phân loại bug.</t>
@@ -299,7 +324,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Detected By:</t>
         </r>
@@ -308,7 +334,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Người phát hiện hoặc người viết Log.</t>
@@ -323,7 +350,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Assigned To:</t>
         </r>
@@ -332,7 +360,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Người được giao việc sửa lỗi.</t>
@@ -347,7 +376,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>DeadLine:</t>
         </r>
@@ -356,7 +386,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Hạn chót phải sửa xong.</t>
@@ -371,7 +402,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">Corrective Action:
 </t>
@@ -488,7 +520,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="292">
   <si>
     <t>Project Code:</t>
   </si>
@@ -1413,14 +1445,16 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2010,6 +2044,1732 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:AF54"/>
+  <sheetViews>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.625" customWidth="1"/>
+    <col min="2" max="2" width="12.875" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="87.375" customWidth="1"/>
+    <col min="5" max="5" width="7.875" customWidth="1"/>
+    <col min="6" max="6" width="16.125" customWidth="1"/>
+    <col min="7" max="7" width="17.375" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.375" customWidth="1"/>
+    <col min="13" max="13" width="12.25" customWidth="1"/>
+    <col min="14" max="14" width="11.75" customWidth="1"/>
+    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="16.375" customWidth="1"/>
+    <col min="17" max="17" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.375" customWidth="1"/>
+    <col min="19" max="19" width="13.625" style="25" customWidth="1"/>
+    <col min="20" max="20" width="13.375" style="25" customWidth="1"/>
+    <col min="23" max="23" width="13.375" customWidth="1"/>
+    <col min="24" max="24" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="27" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="4" spans="2:32" s="30" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="O4" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="P4" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q4" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="S4" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="T4" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="W4" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B5" s="31">
+        <v>40851</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="S5" s="33">
+        <v>40851</v>
+      </c>
+      <c r="T5" s="34"/>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B6" s="31"/>
+      <c r="C6" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="N6" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="34"/>
+      <c r="W6" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y6" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC6" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF6" s="35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B7" s="31"/>
+      <c r="C7" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="34"/>
+      <c r="X7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B8" s="31"/>
+      <c r="C8" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="34"/>
+      <c r="X8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B9" s="31"/>
+      <c r="C9" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="34"/>
+      <c r="X9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B10" s="31"/>
+      <c r="C10" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="34"/>
+      <c r="X10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B11" s="31"/>
+      <c r="C11" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="34"/>
+      <c r="X11" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B12" s="31"/>
+      <c r="C12" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="N12" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="34"/>
+      <c r="X12" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B13" s="31"/>
+      <c r="C13" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="N13" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="34"/>
+      <c r="X13" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B14" s="31"/>
+      <c r="C14" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="M14" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="N14" s="40" t="s">
+        <v>288</v>
+      </c>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="34"/>
+      <c r="X14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B15" s="31"/>
+      <c r="C15" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" t="s">
+        <v>290</v>
+      </c>
+      <c r="M15" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="N15" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="34"/>
+      <c r="X15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B16" s="31"/>
+      <c r="C16" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" t="s">
+        <v>290</v>
+      </c>
+      <c r="M16" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="N16" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="34"/>
+      <c r="X16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B17" s="31"/>
+      <c r="C17" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="K17" t="s">
+        <v>290</v>
+      </c>
+      <c r="M17" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="N17" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="33"/>
+      <c r="T17" s="34"/>
+      <c r="X17" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B18" s="31"/>
+      <c r="C18" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" t="s">
+        <v>290</v>
+      </c>
+      <c r="M18" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="N18" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="34"/>
+      <c r="Y18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B19" s="31"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="M19" s="40"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="33"/>
+      <c r="T19" s="34"/>
+      <c r="Y19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="34"/>
+      <c r="Y20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="33"/>
+      <c r="S21" s="33"/>
+      <c r="T21" s="34"/>
+      <c r="Y21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B22" s="31"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="33"/>
+      <c r="S22" s="33"/>
+      <c r="T22" s="34"/>
+      <c r="AB22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="33"/>
+      <c r="S23" s="33"/>
+      <c r="T23" s="34"/>
+      <c r="AB23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="34"/>
+      <c r="AB24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="33"/>
+      <c r="S25" s="33"/>
+      <c r="T25" s="34"/>
+      <c r="AB25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="33"/>
+      <c r="S26" s="33"/>
+      <c r="T26" s="34"/>
+      <c r="AB26" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B27" s="31"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="33"/>
+      <c r="S27" s="33"/>
+      <c r="T27" s="34"/>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B28" s="31"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="33"/>
+      <c r="S28" s="33"/>
+      <c r="T28" s="34"/>
+    </row>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B29" s="31"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="33"/>
+      <c r="S29" s="33"/>
+      <c r="T29" s="34"/>
+    </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B30" s="31"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="33"/>
+      <c r="S30" s="33"/>
+      <c r="T30" s="34"/>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B31" s="31"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="33"/>
+      <c r="S31" s="33"/>
+      <c r="T31" s="34"/>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B32" s="31"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="33"/>
+      <c r="S32" s="33"/>
+      <c r="T32" s="34"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B33" s="31"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="33"/>
+      <c r="S33" s="33"/>
+      <c r="T33" s="34"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B34" s="31"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="32"/>
+      <c r="Q34" s="32"/>
+      <c r="R34" s="33"/>
+      <c r="S34" s="33"/>
+      <c r="T34" s="34"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B35" s="31"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="32"/>
+      <c r="Q35" s="32"/>
+      <c r="R35" s="33"/>
+      <c r="S35" s="33"/>
+      <c r="T35" s="34"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B36" s="31"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="33"/>
+      <c r="S36" s="33"/>
+      <c r="T36" s="34"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="32"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="33"/>
+      <c r="S37" s="33"/>
+      <c r="T37" s="34"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B38" s="31"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
+      <c r="M38" s="32"/>
+      <c r="N38" s="32"/>
+      <c r="O38" s="32"/>
+      <c r="P38" s="32"/>
+      <c r="Q38" s="32"/>
+      <c r="R38" s="33"/>
+      <c r="S38" s="33"/>
+      <c r="T38" s="34"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B39" s="31"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="32"/>
+      <c r="L39" s="32"/>
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="P39" s="32"/>
+      <c r="Q39" s="32"/>
+      <c r="R39" s="33"/>
+      <c r="S39" s="33"/>
+      <c r="T39" s="34"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B40" s="31"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="R40" s="33"/>
+      <c r="S40" s="33"/>
+      <c r="T40" s="34"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="33"/>
+      <c r="S41" s="33"/>
+      <c r="T41" s="34"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B42" s="31"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="32"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="32"/>
+      <c r="P42" s="32"/>
+      <c r="Q42" s="32"/>
+      <c r="R42" s="33"/>
+      <c r="S42" s="33"/>
+      <c r="T42" s="34"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B43" s="31"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="32"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32"/>
+      <c r="Q43" s="32"/>
+      <c r="R43" s="33"/>
+      <c r="S43" s="33"/>
+      <c r="T43" s="34"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B44" s="31"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
+      <c r="O44" s="32"/>
+      <c r="P44" s="32"/>
+      <c r="Q44" s="32"/>
+      <c r="R44" s="33"/>
+      <c r="S44" s="33"/>
+      <c r="T44" s="34"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B45" s="31"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="32"/>
+      <c r="P45" s="32"/>
+      <c r="Q45" s="32"/>
+      <c r="R45" s="33"/>
+      <c r="S45" s="33"/>
+      <c r="T45" s="34"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B46" s="31"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
+      <c r="M46" s="32"/>
+      <c r="N46" s="32"/>
+      <c r="O46" s="32"/>
+      <c r="P46" s="32"/>
+      <c r="Q46" s="32"/>
+      <c r="R46" s="33"/>
+      <c r="S46" s="33"/>
+      <c r="T46" s="34"/>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B47" s="31"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="32"/>
+      <c r="L47" s="32"/>
+      <c r="M47" s="32"/>
+      <c r="N47" s="32"/>
+      <c r="O47" s="32"/>
+      <c r="P47" s="32"/>
+      <c r="Q47" s="32"/>
+      <c r="R47" s="33"/>
+      <c r="S47" s="33"/>
+      <c r="T47" s="34"/>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B48" s="31"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
+      <c r="L48" s="32"/>
+      <c r="M48" s="32"/>
+      <c r="N48" s="32"/>
+      <c r="O48" s="32"/>
+      <c r="P48" s="32"/>
+      <c r="Q48" s="32"/>
+      <c r="R48" s="33"/>
+      <c r="S48" s="33"/>
+      <c r="T48" s="34"/>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B49" s="31"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
+      <c r="L49" s="32"/>
+      <c r="M49" s="32"/>
+      <c r="N49" s="32"/>
+      <c r="O49" s="32"/>
+      <c r="P49" s="32"/>
+      <c r="Q49" s="32"/>
+      <c r="R49" s="33"/>
+      <c r="S49" s="33"/>
+      <c r="T49" s="34"/>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B50" s="31"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
+      <c r="L50" s="32"/>
+      <c r="M50" s="32"/>
+      <c r="N50" s="32"/>
+      <c r="O50" s="32"/>
+      <c r="P50" s="32"/>
+      <c r="Q50" s="32"/>
+      <c r="R50" s="33"/>
+      <c r="S50" s="33"/>
+      <c r="T50" s="34"/>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B51" s="31"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
+      <c r="L51" s="32"/>
+      <c r="M51" s="32"/>
+      <c r="N51" s="32"/>
+      <c r="O51" s="32"/>
+      <c r="P51" s="32"/>
+      <c r="Q51" s="32"/>
+      <c r="R51" s="33"/>
+      <c r="S51" s="33"/>
+      <c r="T51" s="34"/>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B52" s="31"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32"/>
+      <c r="L52" s="32"/>
+      <c r="M52" s="32"/>
+      <c r="N52" s="32"/>
+      <c r="O52" s="32"/>
+      <c r="P52" s="32"/>
+      <c r="Q52" s="32"/>
+      <c r="R52" s="33"/>
+      <c r="S52" s="33"/>
+      <c r="T52" s="34"/>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B53" s="31"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="32"/>
+      <c r="L53" s="32"/>
+      <c r="M53" s="32"/>
+      <c r="N53" s="32"/>
+      <c r="O53" s="32"/>
+      <c r="P53" s="32"/>
+      <c r="Q53" s="32"/>
+      <c r="R53" s="33"/>
+      <c r="S53" s="33"/>
+      <c r="T53" s="34"/>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B54" s="36"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
+      <c r="M54" s="37"/>
+      <c r="N54" s="37"/>
+      <c r="O54" s="37"/>
+      <c r="P54" s="37"/>
+      <c r="Q54" s="37"/>
+      <c r="R54" s="38"/>
+      <c r="S54" s="38"/>
+      <c r="T54" s="39"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B4:T4"/>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E13 E21:E54">
+      <formula1>$X$7:$X$17</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F13 F21:F54">
+      <formula1>$Y$7:$Y$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G13 G21:G54">
+      <formula1>$Z$7:$Z$15</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H13 H21:H54">
+      <formula1>$AA$7:$AA$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I13 I21:I54">
+      <formula1>$AB$7:$AB$26</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J13 J21:J54">
+      <formula1>$AC$7:$AC$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L13 L21:L54">
+      <formula1>$AD$7:$AD$19</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="62" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="9" min="1" max="53" man="1"/>
+  </colBreaks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AF100"/>
   <sheetViews>
@@ -6988,12 +8748,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AF54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7008,7 +8768,7 @@
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.375" customWidth="1"/>
     <col min="13" max="13" width="12.25" customWidth="1"/>
     <col min="14" max="14" width="11.75" customWidth="1"/>
@@ -7107,838 +8867,332 @@
       <c r="AE4"/>
       <c r="AF4"/>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B5" s="31">
+    <row r="5" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R5" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="S5" s="31">
         <v>40851</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="E5" s="32" t="s">
+    </row>
+    <row r="6" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W6" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y6" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC6" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF6" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X7" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y7" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z7" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA7" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB7" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC7" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD7" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="AF7" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y8" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z8" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA8" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB8" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC8" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD8" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE8" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF8" s="31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X9" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y9" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z9" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA9" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB9" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC9" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD9" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE9" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF9" s="31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y10" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z10" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA10" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB10" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC10" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD10" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE10" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF10" s="31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X11" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y11" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="Z11" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32" t="s">
-        <v>273</v>
-      </c>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="N5" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="S5" s="33">
-        <v>40851</v>
-      </c>
-      <c r="T5" s="34"/>
-    </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B6" s="31"/>
-      <c r="C6" t="s">
-        <v>275</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>291</v>
-      </c>
-      <c r="E6" s="32" t="s">
+      <c r="AB11" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD11" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE11" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF11" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X12" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y12" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z12" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB12" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD12" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE12" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF12" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X13" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y13" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z13" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB13" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD13" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE13" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF13" s="31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X14" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y14" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z14" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB14" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD14" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE14" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X15" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="N6" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="34"/>
-      <c r="W6" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="X6" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y6" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA6" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB6" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC6" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD6" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE6" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF6" s="35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B7" s="31"/>
-      <c r="C7" t="s">
-        <v>275</v>
-      </c>
-      <c r="D7" t="s">
-        <v>278</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="N7" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="34"/>
-      <c r="X7" t="s">
+      <c r="Y15" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z15" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB15" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD15" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE15" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X16" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB16" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD16" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE16" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:31" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X17" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y17" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB17" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD17" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE17" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="Y7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B8" s="31"/>
-      <c r="C8" t="s">
-        <v>275</v>
-      </c>
-      <c r="D8" t="s">
-        <v>279</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="N8" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="33"/>
-      <c r="T8" s="34"/>
-      <c r="X8" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B9" s="31"/>
-      <c r="C9" t="s">
-        <v>275</v>
-      </c>
-      <c r="D9" t="s">
-        <v>277</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="N9" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="33"/>
-      <c r="T9" s="34"/>
-      <c r="X9" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B10" s="31"/>
-      <c r="C10" t="s">
-        <v>276</v>
-      </c>
-      <c r="D10" t="s">
-        <v>278</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="N10" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="33"/>
-      <c r="T10" s="34"/>
-      <c r="X10" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B11" s="31"/>
-      <c r="C11" t="s">
-        <v>276</v>
-      </c>
-      <c r="D11" t="s">
-        <v>279</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="N11" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="34"/>
-      <c r="X11" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>83</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B12" s="31"/>
-      <c r="C12" t="s">
-        <v>276</v>
-      </c>
-      <c r="D12" t="s">
-        <v>277</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="N12" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="33"/>
-      <c r="T12" s="34"/>
-      <c r="X12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B13" s="31"/>
-      <c r="C13" t="s">
-        <v>280</v>
-      </c>
-      <c r="D13" t="s">
-        <v>287</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32" t="s">
-        <v>289</v>
-      </c>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="N13" s="32" t="s">
-        <v>288</v>
-      </c>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="33"/>
-      <c r="T13" s="34"/>
-      <c r="X13" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B14" s="31"/>
-      <c r="C14" t="s">
-        <v>280</v>
-      </c>
-      <c r="D14" t="s">
-        <v>283</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="I14" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="K14" s="32" t="s">
-        <v>289</v>
-      </c>
-      <c r="M14" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="N14" s="40" t="s">
-        <v>288</v>
-      </c>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="33"/>
-      <c r="T14" s="34"/>
-      <c r="X14" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B15" s="31"/>
-      <c r="C15" t="s">
-        <v>281</v>
-      </c>
-      <c r="D15" t="s">
-        <v>282</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" t="s">
-        <v>290</v>
-      </c>
-      <c r="M15" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="N15" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="34"/>
-      <c r="X15" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B16" s="31"/>
-      <c r="C16" t="s">
-        <v>281</v>
-      </c>
-      <c r="D16" t="s">
-        <v>283</v>
-      </c>
-      <c r="E16" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="K16" t="s">
-        <v>290</v>
-      </c>
-      <c r="M16" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="N16" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="34"/>
-      <c r="X16" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B17" s="31"/>
-      <c r="C17" t="s">
-        <v>281</v>
-      </c>
-      <c r="D17" t="s">
-        <v>285</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="K17" t="s">
-        <v>290</v>
-      </c>
-      <c r="M17" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="N17" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="34"/>
-      <c r="X17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B18" s="31"/>
-      <c r="C18" t="s">
-        <v>284</v>
-      </c>
-      <c r="D18" t="s">
-        <v>286</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="K18" t="s">
-        <v>290</v>
-      </c>
-      <c r="M18" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="N18" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="34"/>
-      <c r="Y18" t="s">
+    </row>
+    <row r="18" spans="2:31" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y18" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AB18" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AD18" s="31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B19" s="31"/>
-      <c r="M19" s="40"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="32"/>
-      <c r="S19" s="33"/>
-      <c r="T19" s="34"/>
-      <c r="Y19" t="s">
+    <row r="19" spans="2:31" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y19" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AB19" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AD19" s="31" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B20" s="31"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="34"/>
-      <c r="Y20" t="s">
+    <row r="20" spans="2:31" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y20" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AB20" s="31" t="s">
         <v>56</v>
       </c>
     </row>
@@ -8680,26 +9934,26 @@
   </sheetData>
   <autoFilter ref="B4:T4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E13 E21:E54">
-      <formula1>$X$7:$X$17</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L13 L21:L54">
+      <formula1>$AD$7:$AD$19</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J13 J21:J54">
+      <formula1>$AC$7:$AC$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I13 I21:I54">
+      <formula1>$AB$7:$AB$26</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H13 H21:H54">
+      <formula1>$AA$7:$AA$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G13 G21:G54">
+      <formula1>$Z$7:$Z$15</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F13 F21:F54">
       <formula1>$Y$7:$Y$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G13 G21:G54">
-      <formula1>$Z$7:$Z$15</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H13 H21:H54">
-      <formula1>$AA$7:$AA$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I13 I21:I54">
-      <formula1>$AB$7:$AB$26</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J13 J21:J54">
-      <formula1>$AC$7:$AC$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L13 L21:L54">
-      <formula1>$AD$7:$AD$19</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E13 E21:E54">
+      <formula1>$X$7:$X$17</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
review phần NewProduct _ KhoaVT
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -523,7 +523,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="322">
   <si>
     <t>Project Code:</t>
   </si>
@@ -1480,16 +1480,28 @@
     <t>Cách đặt tên hàm (hoa, thường) chưa thống nhất</t>
   </si>
   <si>
-    <t>Các trường ngày tháng chưa xử lý tự động</t>
-  </si>
-  <si>
-    <t>Delete Products</t>
-  </si>
-  <si>
-    <t>Viết action xóa một product trong CSDL</t>
-  </si>
-  <si>
-    <t>Khi xóa sản phẩm xong hiện ra 1 trang xóa sản phẩm không biết để làm gì</t>
+    <t>New Product</t>
+  </si>
+  <si>
+    <t>Viết action tạo mới một sản phẩm và lưu vào trong CSDL</t>
+  </si>
+  <si>
+    <t>Chưa kiểm tra giá trị đầu vào ở các mục Name - Model - Price.(Đối với Name và Model chưa kiểm tra các kí tự đặc biệt !@#$%^&amp;*(), còn Price chưa kiểm tra giá trị nhập vào chỉ là số)</t>
+  </si>
+  <si>
+    <t>Mục Order: nên để hiện ngày hiện tại trực tiếp hiện lên.Không nên để khung textbox.</t>
+  </si>
+  <si>
+    <t>Button Save- chưa lưu vào CSDL, chỉ mới hiện lại thông tin nhập vào.</t>
+  </si>
+  <si>
+    <t>Nên tạo thêm đường link để trở về trang trước.</t>
+  </si>
+  <si>
+    <t>Button Cancel- chưa có chức năng cho button này.(chưa thấy trong code)</t>
+  </si>
+  <si>
+    <t>Form trình bày chưa đẹp lắm :D</t>
   </si>
 </sst>
 </file>
@@ -1503,14 +1515,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1518,7 +1530,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1831,7 +1843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1970,6 +1982,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2011,6 +2026,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2317,38 +2344,38 @@
       <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.625" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.375" customWidth="1"/>
-    <col min="5" max="5" width="87.375" customWidth="1"/>
-    <col min="6" max="6" width="7.875" customWidth="1"/>
-    <col min="7" max="7" width="16.125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="17.375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="87.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
     <col min="10" max="10" width="21" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="9" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="12.25" customWidth="1"/>
-    <col min="15" max="15" width="11.75" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
     <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="16.375" customWidth="1"/>
-    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.375" customWidth="1"/>
-    <col min="20" max="20" width="13.625" style="25" customWidth="1"/>
-    <col min="21" max="21" width="13.375" style="25" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="13.375" customWidth="1"/>
-    <col min="25" max="25" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" style="25" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" style="25" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="25" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="27" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:33">
@@ -3278,7 +3305,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="2:32" ht="15" thickBot="1">
+    <row r="19" spans="2:32" ht="15.75" thickBot="1">
       <c r="B19" s="53"/>
       <c r="C19" s="54"/>
       <c r="D19" s="54"/>
@@ -3311,7 +3338,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="2:32" ht="15" thickTop="1">
+    <row r="20" spans="2:32" ht="15.75" thickTop="1">
       <c r="B20" s="31">
         <v>40864</v>
       </c>
@@ -3333,11 +3360,11 @@
       </c>
     </row>
     <row r="21" spans="2:32">
-      <c r="B21" s="66"/>
-      <c r="C21" s="63" t="s">
+      <c r="B21" s="67"/>
+      <c r="C21" s="64" t="s">
         <v>307</v>
       </c>
-      <c r="D21" s="63" t="s">
+      <c r="D21" s="64" t="s">
         <v>308</v>
       </c>
       <c r="E21" s="32" t="s">
@@ -3373,9 +3400,9 @@
       </c>
     </row>
     <row r="22" spans="2:32">
-      <c r="B22" s="67"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
       <c r="E22" s="32" t="s">
         <v>310</v>
       </c>
@@ -3406,9 +3433,9 @@
       </c>
     </row>
     <row r="23" spans="2:32">
-      <c r="B23" s="68"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
       <c r="E23" s="32" t="s">
         <v>311</v>
       </c>
@@ -4171,44 +4198,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AF100"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="E13" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A69" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="3" customWidth="1"/>
-    <col min="4" max="4" width="67.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="7.875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.125" style="3"/>
+    <col min="4" max="4" width="67.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="3"/>
     <col min="9" max="9" width="21" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.125" style="3"/>
-    <col min="11" max="11" width="34.125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="15.875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.25" style="3" customWidth="1"/>
-    <col min="14" max="14" width="11.75" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.75" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="34.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="3" customWidth="1"/>
     <col min="16" max="16" width="35" style="3" customWidth="1"/>
-    <col min="17" max="17" width="14.125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="20.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.375" style="5" customWidth="1"/>
-    <col min="21" max="22" width="9.125" style="3"/>
-    <col min="23" max="23" width="13.375" style="3" customWidth="1"/>
-    <col min="24" max="24" width="9.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="5" customWidth="1"/>
+    <col min="21" max="22" width="9.140625" style="3"/>
+    <col min="23" max="23" width="13.42578125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.125" style="3"/>
-    <col min="30" max="30" width="22.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.125" style="3"/>
+    <col min="29" max="29" width="9.140625" style="3"/>
+    <col min="30" max="30" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:32">
@@ -4296,7 +4323,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="2:32" ht="28.5">
+    <row r="5" spans="2:32" ht="45">
       <c r="B5" s="11">
         <v>40837</v>
       </c>
@@ -4353,7 +4380,7 @@
         <v>40838</v>
       </c>
     </row>
-    <row r="6" spans="2:32" ht="28.5">
+    <row r="6" spans="2:32" ht="45">
       <c r="B6" s="11">
         <v>40837</v>
       </c>
@@ -4440,7 +4467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:32" ht="28.5">
+    <row r="7" spans="2:32" ht="30">
       <c r="B7" s="11">
         <v>40837</v>
       </c>
@@ -4524,7 +4551,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:32" ht="28.5">
+    <row r="8" spans="2:32" ht="30">
       <c r="B8" s="11">
         <v>40837</v>
       </c>
@@ -4608,7 +4635,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:32" ht="28.5">
+    <row r="9" spans="2:32" ht="30">
       <c r="B9" s="11">
         <v>40837</v>
       </c>
@@ -4692,7 +4719,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:32" ht="28.5">
+    <row r="10" spans="2:32" ht="30">
       <c r="B10" s="11">
         <v>40837</v>
       </c>
@@ -4776,7 +4803,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:32" ht="28.5">
+    <row r="11" spans="2:32" ht="30">
       <c r="B11" s="11">
         <v>40837</v>
       </c>
@@ -4854,7 +4881,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:32" ht="28.5">
+    <row r="12" spans="2:32" ht="30">
       <c r="B12" s="11">
         <v>40837</v>
       </c>
@@ -4932,7 +4959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:32" ht="28.5">
+    <row r="13" spans="2:32" ht="30">
       <c r="B13" s="11">
         <v>40837</v>
       </c>
@@ -5049,7 +5076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:32" ht="57">
+    <row r="15" spans="2:32" ht="60">
       <c r="B15" s="11">
         <v>40837</v>
       </c>
@@ -5268,7 +5295,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:31" ht="28.5">
+    <row r="18" spans="2:31" ht="30">
       <c r="B18" s="11">
         <v>40837</v>
       </c>
@@ -5526,7 +5553,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:31" ht="28.5">
+    <row r="22" spans="2:31" ht="30">
       <c r="B22" s="11">
         <v>40837</v>
       </c>
@@ -5706,7 +5733,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:31" ht="28.5">
+    <row r="25" spans="2:31" ht="30">
       <c r="B25" s="11">
         <v>40837</v>
       </c>
@@ -5859,7 +5886,7 @@
       <c r="S27" s="13"/>
       <c r="T27" s="14"/>
     </row>
-    <row r="28" spans="2:31" ht="28.5">
+    <row r="28" spans="2:31" ht="30">
       <c r="B28" s="11">
         <v>40837</v>
       </c>
@@ -5912,7 +5939,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="29" spans="2:31" ht="28.5">
+    <row r="29" spans="2:31" ht="30">
       <c r="B29" s="11">
         <v>40837</v>
       </c>
@@ -5965,7 +5992,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="30" spans="2:31" ht="28.5">
+    <row r="30" spans="2:31" ht="30">
       <c r="B30" s="11">
         <v>40837</v>
       </c>
@@ -6018,7 +6045,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="31" spans="2:31" ht="28.5">
+    <row r="31" spans="2:31" ht="30">
       <c r="B31" s="11">
         <v>40837</v>
       </c>
@@ -6071,7 +6098,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="32" spans="2:31" ht="28.5">
+    <row r="32" spans="2:31" ht="30">
       <c r="B32" s="11">
         <v>40837</v>
       </c>
@@ -6124,7 +6151,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="33" spans="2:20" ht="28.5">
+    <row r="33" spans="2:20" ht="30">
       <c r="B33" s="11">
         <v>40837</v>
       </c>
@@ -6177,7 +6204,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="34" spans="2:20" ht="28.5">
+    <row r="34" spans="2:20" ht="30">
       <c r="B34" s="11">
         <v>40837</v>
       </c>
@@ -6230,7 +6257,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="35" spans="2:20" ht="28.5">
+    <row r="35" spans="2:20" ht="30">
       <c r="B35" s="11">
         <v>40837</v>
       </c>
@@ -6283,7 +6310,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="36" spans="2:20" ht="28.5">
+    <row r="36" spans="2:20" ht="30">
       <c r="B36" s="11">
         <v>40837</v>
       </c>
@@ -6336,7 +6363,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="37" spans="2:20" ht="28.5">
+    <row r="37" spans="2:20" ht="30">
       <c r="B37" s="11">
         <v>40837</v>
       </c>
@@ -6389,7 +6416,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="38" spans="2:20" ht="28.5">
+    <row r="38" spans="2:20" ht="30">
       <c r="B38" s="11">
         <v>40837</v>
       </c>
@@ -6442,7 +6469,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="39" spans="2:20" ht="28.5">
+    <row r="39" spans="2:20" ht="30">
       <c r="B39" s="11">
         <v>40837</v>
       </c>
@@ -6495,7 +6522,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="40" spans="2:20" ht="28.5">
+    <row r="40" spans="2:20" ht="30">
       <c r="B40" s="11">
         <v>40837</v>
       </c>
@@ -6548,7 +6575,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="41" spans="2:20" ht="28.5">
+    <row r="41" spans="2:20" ht="30">
       <c r="B41" s="11">
         <v>40837</v>
       </c>
@@ -6601,7 +6628,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="42" spans="2:20" ht="28.5">
+    <row r="42" spans="2:20" ht="30">
       <c r="B42" s="11">
         <v>40837</v>
       </c>
@@ -6707,7 +6734,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="44" spans="2:20" ht="28.5">
+    <row r="44" spans="2:20" ht="30">
       <c r="B44" s="11">
         <v>40837</v>
       </c>
@@ -6760,7 +6787,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="45" spans="2:20" ht="28.5">
+    <row r="45" spans="2:20" ht="30">
       <c r="B45" s="11">
         <v>40837</v>
       </c>
@@ -6813,7 +6840,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="46" spans="2:20" ht="28.5">
+    <row r="46" spans="2:20" ht="30">
       <c r="B46" s="11">
         <v>40837</v>
       </c>
@@ -6866,7 +6893,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="47" spans="2:20" ht="28.5">
+    <row r="47" spans="2:20" ht="30">
       <c r="B47" s="11">
         <v>40837</v>
       </c>
@@ -6919,7 +6946,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="48" spans="2:20" ht="28.5">
+    <row r="48" spans="2:20" ht="30">
       <c r="B48" s="11">
         <v>40837</v>
       </c>
@@ -6972,7 +6999,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="49" spans="2:32" ht="28.5">
+    <row r="49" spans="2:32" ht="30">
       <c r="B49" s="11">
         <v>40837</v>
       </c>
@@ -7025,7 +7052,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="50" spans="2:32" ht="28.5">
+    <row r="50" spans="2:32" ht="30">
       <c r="B50" s="11">
         <v>40837</v>
       </c>
@@ -7078,7 +7105,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="51" spans="2:32" ht="28.5">
+    <row r="51" spans="2:32" ht="30">
       <c r="B51" s="11">
         <v>40837</v>
       </c>
@@ -7131,7 +7158,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="52" spans="2:32" ht="28.5">
+    <row r="52" spans="2:32" ht="30">
       <c r="B52" s="11">
         <v>40837</v>
       </c>
@@ -7184,7 +7211,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="53" spans="2:32" ht="28.5">
+    <row r="53" spans="2:32" ht="30">
       <c r="B53" s="11">
         <v>40837</v>
       </c>
@@ -7237,7 +7264,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="54" spans="2:32" ht="28.5">
+    <row r="54" spans="2:32" ht="30">
       <c r="B54" s="11">
         <v>40837</v>
       </c>
@@ -7290,7 +7317,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="55" spans="2:32" ht="28.5">
+    <row r="55" spans="2:32" ht="30">
       <c r="B55" s="11">
         <v>40837</v>
       </c>
@@ -7343,7 +7370,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="56" spans="2:32" ht="28.5">
+    <row r="56" spans="2:32" ht="45">
       <c r="B56" s="11">
         <v>40837</v>
       </c>
@@ -7396,7 +7423,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="57" spans="2:32" ht="28.5">
+    <row r="57" spans="2:32" ht="30">
       <c r="B57" s="11">
         <v>40837</v>
       </c>
@@ -7449,7 +7476,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="58" spans="2:32" ht="28.5">
+    <row r="58" spans="2:32" ht="30">
       <c r="B58" s="11">
         <v>40837</v>
       </c>
@@ -7498,7 +7525,7 @@
       <c r="S58" s="13"/>
       <c r="T58" s="13"/>
     </row>
-    <row r="59" spans="2:32" ht="28.5">
+    <row r="59" spans="2:32" ht="30">
       <c r="B59" s="11">
         <v>40837</v>
       </c>
@@ -7559,7 +7586,7 @@
       <c r="AE59"/>
       <c r="AF59"/>
     </row>
-    <row r="60" spans="2:32" ht="28.5">
+    <row r="60" spans="2:32" ht="30">
       <c r="B60" s="11">
         <v>40837</v>
       </c>
@@ -7620,7 +7647,7 @@
       <c r="AE60"/>
       <c r="AF60"/>
     </row>
-    <row r="61" spans="2:32" ht="28.5">
+    <row r="61" spans="2:32" ht="30">
       <c r="B61" s="11">
         <v>40837</v>
       </c>
@@ -7681,7 +7708,7 @@
       <c r="AE61"/>
       <c r="AF61"/>
     </row>
-    <row r="62" spans="2:32" ht="28.5">
+    <row r="62" spans="2:32" ht="30">
       <c r="B62" s="11">
         <v>40837</v>
       </c>
@@ -7742,7 +7769,7 @@
       <c r="AE62"/>
       <c r="AF62"/>
     </row>
-    <row r="63" spans="2:32" ht="28.5">
+    <row r="63" spans="2:32" ht="30">
       <c r="B63" s="11">
         <v>40837</v>
       </c>
@@ -7803,7 +7830,7 @@
       <c r="AE63"/>
       <c r="AF63"/>
     </row>
-    <row r="64" spans="2:32" ht="28.5">
+    <row r="64" spans="2:32" ht="30">
       <c r="B64" s="11">
         <v>40837</v>
       </c>
@@ -7864,7 +7891,7 @@
       <c r="AE64"/>
       <c r="AF64"/>
     </row>
-    <row r="65" spans="2:32" ht="28.5">
+    <row r="65" spans="2:32" ht="30">
       <c r="B65" s="11">
         <v>40837</v>
       </c>
@@ -7925,7 +7952,7 @@
       <c r="AE65"/>
       <c r="AF65"/>
     </row>
-    <row r="66" spans="2:32" ht="28.5">
+    <row r="66" spans="2:32" ht="30">
       <c r="B66" s="11">
         <v>40837</v>
       </c>
@@ -7986,7 +8013,7 @@
       <c r="AE66"/>
       <c r="AF66"/>
     </row>
-    <row r="67" spans="2:32" ht="28.5">
+    <row r="67" spans="2:32" ht="30">
       <c r="B67" s="11">
         <v>40837</v>
       </c>
@@ -8047,7 +8074,7 @@
       <c r="AE67"/>
       <c r="AF67"/>
     </row>
-    <row r="68" spans="2:32" ht="28.5">
+    <row r="68" spans="2:32" ht="30">
       <c r="B68" s="11">
         <v>40837</v>
       </c>
@@ -8112,7 +8139,7 @@
       <c r="AE68"/>
       <c r="AF68"/>
     </row>
-    <row r="69" spans="2:32" ht="28.5">
+    <row r="69" spans="2:32" ht="30">
       <c r="B69" s="11">
         <v>40837</v>
       </c>
@@ -8173,7 +8200,7 @@
       <c r="AE69"/>
       <c r="AF69"/>
     </row>
-    <row r="70" spans="2:32" ht="28.5">
+    <row r="70" spans="2:32" ht="30">
       <c r="B70" s="11">
         <v>40837</v>
       </c>
@@ -8234,7 +8261,7 @@
       <c r="AE70"/>
       <c r="AF70"/>
     </row>
-    <row r="71" spans="2:32" ht="28.5">
+    <row r="71" spans="2:32" ht="30">
       <c r="B71" s="11">
         <v>40837</v>
       </c>
@@ -8283,7 +8310,7 @@
       <c r="S71" s="13"/>
       <c r="T71" s="14"/>
     </row>
-    <row r="72" spans="2:32" ht="28.5">
+    <row r="72" spans="2:32" ht="30">
       <c r="B72" s="11">
         <v>40837</v>
       </c>
@@ -8332,7 +8359,7 @@
       <c r="S72" s="13"/>
       <c r="T72" s="14"/>
     </row>
-    <row r="73" spans="2:32" ht="28.5">
+    <row r="73" spans="2:32" ht="30">
       <c r="B73" s="11" t="s">
         <v>238</v>
       </c>
@@ -8383,7 +8410,7 @@
       </c>
       <c r="T73" s="14"/>
     </row>
-    <row r="74" spans="2:32" ht="28.5">
+    <row r="74" spans="2:32" ht="30">
       <c r="B74" s="11" t="s">
         <v>238</v>
       </c>
@@ -8434,7 +8461,7 @@
       </c>
       <c r="T74" s="14"/>
     </row>
-    <row r="75" spans="2:32" ht="28.5">
+    <row r="75" spans="2:32" ht="30">
       <c r="B75" s="11" t="s">
         <v>238</v>
       </c>
@@ -8485,7 +8512,7 @@
       </c>
       <c r="T75" s="14"/>
     </row>
-    <row r="76" spans="2:32" ht="28.5">
+    <row r="76" spans="2:32" ht="30">
       <c r="B76" s="11" t="s">
         <v>238</v>
       </c>
@@ -8536,7 +8563,7 @@
       </c>
       <c r="T76" s="14"/>
     </row>
-    <row r="77" spans="2:32" ht="28.5">
+    <row r="77" spans="2:32" ht="30">
       <c r="B77" s="11" t="s">
         <v>238</v>
       </c>
@@ -8587,7 +8614,7 @@
       </c>
       <c r="T77" s="14"/>
     </row>
-    <row r="78" spans="2:32" ht="28.5">
+    <row r="78" spans="2:32" ht="30">
       <c r="B78" s="11" t="s">
         <v>238</v>
       </c>
@@ -9151,41 +9178,41 @@
   <dimension ref="B2:AG54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="D9" sqref="D9:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.625" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
-    <col min="4" max="4" width="45.25" customWidth="1"/>
-    <col min="5" max="5" width="50.5" customWidth="1"/>
-    <col min="6" max="6" width="7.875" customWidth="1"/>
-    <col min="7" max="7" width="16.125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="17.375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="81" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="81" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="27.125" customWidth="1"/>
-    <col min="13" max="13" width="12.375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="12.25" customWidth="1"/>
-    <col min="15" max="15" width="11.75" customWidth="1"/>
+    <col min="12" max="12" width="27.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" style="81" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="81" customWidth="1"/>
     <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="16.375" customWidth="1"/>
-    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.375" customWidth="1"/>
-    <col min="20" max="20" width="13.625" style="25" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="13.375" style="25" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="13.375" customWidth="1"/>
-    <col min="25" max="25" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" style="25" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" style="25" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="25" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="27" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:33">
@@ -9193,7 +9220,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="23"/>
-      <c r="F2" s="24"/>
+      <c r="F2" s="80"/>
     </row>
     <row r="4" spans="2:33" s="30" customFormat="1" ht="27.75" customHeight="1">
       <c r="B4" s="26" t="s">
@@ -9208,7 +9235,7 @@
       <c r="E4" s="27" t="s">
         <v>292</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="79" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="27" t="s">
@@ -9217,7 +9244,7 @@
       <c r="H4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="79" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="27" t="s">
@@ -9232,10 +9259,10 @@
       <c r="M4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="79" t="s">
         <v>264</v>
       </c>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="79" t="s">
         <v>265</v>
       </c>
       <c r="P4" s="27" t="s">
@@ -9270,26 +9297,26 @@
       <c r="AG4"/>
     </row>
     <row r="5" spans="2:33" s="31" customFormat="1">
-      <c r="B5" s="69"/>
-      <c r="C5" s="72" t="s">
+      <c r="B5" s="70"/>
+      <c r="C5" s="73" t="s">
         <v>293</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="73" t="s">
         <v>294</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>295</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="O5" s="44" t="s">
         <v>186</v>
       </c>
       <c r="T5" s="31">
@@ -9297,22 +9324,22 @@
       </c>
     </row>
     <row r="6" spans="2:33" s="31" customFormat="1">
-      <c r="B6" s="70"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
       <c r="E6" s="31" t="s">
         <v>296</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="O6" s="31" t="s">
+      <c r="O6" s="44" t="s">
         <v>186</v>
       </c>
       <c r="X6" s="31" t="s">
@@ -9347,22 +9374,22 @@
       </c>
     </row>
     <row r="7" spans="2:33" s="31" customFormat="1">
-      <c r="B7" s="70"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
       <c r="E7" s="31" t="s">
         <v>297</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="31" t="s">
+      <c r="N7" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="O7" s="31" t="s">
+      <c r="O7" s="44" t="s">
         <v>186</v>
       </c>
       <c r="X7" s="31" t="s">
@@ -9397,22 +9424,22 @@
       </c>
     </row>
     <row r="8" spans="2:33" s="31" customFormat="1">
-      <c r="B8" s="71"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
       <c r="E8" s="31" t="s">
         <v>306</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="N8" s="31" t="s">
+      <c r="N8" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="O8" s="31" t="s">
+      <c r="O8" s="44" t="s">
         <v>186</v>
       </c>
       <c r="X8" s="31" t="s">
@@ -9446,28 +9473,27 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:33" s="31" customFormat="1">
-      <c r="B9" s="31">
-        <v>40865</v>
-      </c>
-      <c r="C9" s="31" t="s">
+    <row r="9" spans="2:33" s="31" customFormat="1" ht="60">
+      <c r="B9" s="41"/>
+      <c r="C9" s="73" t="s">
+        <v>314</v>
+      </c>
+      <c r="D9" s="73" t="s">
         <v>315</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="E9" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>317</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="31" t="s">
+      <c r="F9" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="N9" s="31" t="s">
-        <v>145</v>
-      </c>
+      <c r="N9" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="O9" s="44"/>
       <c r="X9" s="31" t="s">
         <v>169</v>
       </c>
@@ -9499,10 +9525,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:33" s="31" customFormat="1">
+    <row r="10" spans="2:33" s="31" customFormat="1" ht="30">
       <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="44"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="O10" s="44"/>
       <c r="X10" s="31" t="s">
         <v>298</v>
       </c>
@@ -9534,10 +9573,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:33" s="31" customFormat="1">
+    <row r="11" spans="2:33" s="31" customFormat="1" ht="30">
       <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="44"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="82" t="s">
+        <v>318</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="N11" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="O11" s="44"/>
       <c r="X11" s="31" t="s">
         <v>185</v>
       </c>
@@ -9565,8 +9617,21 @@
     </row>
     <row r="12" spans="2:33" s="31" customFormat="1">
       <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="44"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="O12" s="44"/>
       <c r="X12" s="31" t="s">
         <v>167</v>
       </c>
@@ -9594,8 +9659,19 @@
     </row>
     <row r="13" spans="2:33" s="31" customFormat="1">
       <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="44"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="31" t="s">
+        <v>319</v>
+      </c>
+      <c r="F13" s="44"/>
+      <c r="I13" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="N13" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="O13" s="44"/>
       <c r="X13" s="31" t="s">
         <v>186</v>
       </c>
@@ -9623,8 +9699,19 @@
     </row>
     <row r="14" spans="2:33" s="31" customFormat="1">
       <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="44"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="31" t="s">
+        <v>321</v>
+      </c>
+      <c r="F14" s="44"/>
+      <c r="I14" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="O14" s="44"/>
       <c r="X14" s="31" t="s">
         <v>145</v>
       </c>
@@ -9651,6 +9738,10 @@
       <c r="B15" s="41"/>
       <c r="C15" s="41"/>
       <c r="D15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
       <c r="X15" s="31" t="s">
         <v>234</v>
       </c>
@@ -9677,6 +9768,10 @@
       <c r="B16" s="41"/>
       <c r="C16" s="41"/>
       <c r="D16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
       <c r="X16" s="31" t="s">
         <v>151</v>
       </c>
@@ -9700,6 +9795,10 @@
       <c r="B17" s="41"/>
       <c r="C17" s="41"/>
       <c r="D17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="44"/>
       <c r="X17" s="31" t="s">
         <v>299</v>
       </c>
@@ -9723,6 +9822,10 @@
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
       <c r="X18" s="31" t="s">
         <v>300</v>
       </c>
@@ -9740,6 +9843,10 @@
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
       <c r="D19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="44"/>
       <c r="X19" s="31" t="s">
         <v>160</v>
       </c>
@@ -9757,6 +9864,10 @@
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
       <c r="D20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="44"/>
       <c r="Z20" s="31" t="s">
         <v>34</v>
       </c>
@@ -9769,16 +9880,16 @@
       <c r="C21" s="42"/>
       <c r="D21" s="45"/>
       <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
+      <c r="F21" s="45"/>
       <c r="G21" s="32"/>
       <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
+      <c r="I21" s="45"/>
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
       <c r="L21" s="32"/>
       <c r="M21" s="32"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
       <c r="P21" s="32"/>
       <c r="Q21" s="32"/>
       <c r="R21" s="32"/>
@@ -9797,16 +9908,16 @@
       <c r="C22" s="42"/>
       <c r="D22" s="45"/>
       <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
+      <c r="F22" s="45"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
+      <c r="I22" s="45"/>
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
       <c r="L22" s="32"/>
       <c r="M22" s="32"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
       <c r="P22" s="32"/>
       <c r="Q22" s="32"/>
       <c r="R22" s="32"/>
@@ -9822,16 +9933,16 @@
       <c r="C23" s="42"/>
       <c r="D23" s="45"/>
       <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="32"/>
       <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
+      <c r="I23" s="45"/>
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
       <c r="L23" s="32"/>
       <c r="M23" s="32"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
       <c r="P23" s="32"/>
       <c r="Q23" s="32"/>
       <c r="R23" s="32"/>
@@ -9847,16 +9958,16 @@
       <c r="C24" s="42"/>
       <c r="D24" s="45"/>
       <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="32"/>
       <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
+      <c r="I24" s="45"/>
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
       <c r="L24" s="32"/>
       <c r="M24" s="32"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
       <c r="P24" s="32"/>
       <c r="Q24" s="32"/>
       <c r="R24" s="32"/>
@@ -9872,16 +9983,16 @@
       <c r="C25" s="42"/>
       <c r="D25" s="45"/>
       <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
+      <c r="F25" s="45"/>
       <c r="G25" s="32"/>
       <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
+      <c r="I25" s="45"/>
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
       <c r="L25" s="32"/>
       <c r="M25" s="32"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
       <c r="P25" s="32"/>
       <c r="Q25" s="32"/>
       <c r="R25" s="32"/>
@@ -9897,16 +10008,16 @@
       <c r="C26" s="42"/>
       <c r="D26" s="45"/>
       <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
+      <c r="F26" s="45"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
+      <c r="I26" s="45"/>
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
       <c r="L26" s="32"/>
       <c r="M26" s="32"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
       <c r="P26" s="32"/>
       <c r="Q26" s="32"/>
       <c r="R26" s="32"/>
@@ -9922,16 +10033,16 @@
       <c r="C27" s="42"/>
       <c r="D27" s="45"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
+      <c r="F27" s="45"/>
       <c r="G27" s="32"/>
       <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
+      <c r="I27" s="45"/>
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
       <c r="L27" s="32"/>
       <c r="M27" s="32"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
       <c r="P27" s="32"/>
       <c r="Q27" s="32"/>
       <c r="R27" s="32"/>
@@ -9944,16 +10055,16 @@
       <c r="C28" s="42"/>
       <c r="D28" s="45"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
+      <c r="F28" s="45"/>
       <c r="G28" s="32"/>
       <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
+      <c r="I28" s="45"/>
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
       <c r="L28" s="32"/>
       <c r="M28" s="32"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
       <c r="P28" s="32"/>
       <c r="Q28" s="32"/>
       <c r="R28" s="32"/>
@@ -9966,16 +10077,16 @@
       <c r="C29" s="42"/>
       <c r="D29" s="45"/>
       <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
+      <c r="F29" s="45"/>
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
+      <c r="I29" s="45"/>
       <c r="J29" s="32"/>
       <c r="K29" s="32"/>
       <c r="L29" s="32"/>
       <c r="M29" s="32"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
       <c r="P29" s="32"/>
       <c r="Q29" s="32"/>
       <c r="R29" s="32"/>
@@ -9988,16 +10099,16 @@
       <c r="C30" s="42"/>
       <c r="D30" s="45"/>
       <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
+      <c r="F30" s="45"/>
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
+      <c r="I30" s="45"/>
       <c r="J30" s="32"/>
       <c r="K30" s="32"/>
       <c r="L30" s="32"/>
       <c r="M30" s="32"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
       <c r="P30" s="32"/>
       <c r="Q30" s="32"/>
       <c r="R30" s="32"/>
@@ -10010,16 +10121,16 @@
       <c r="C31" s="42"/>
       <c r="D31" s="45"/>
       <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="32"/>
       <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
+      <c r="I31" s="45"/>
       <c r="J31" s="32"/>
       <c r="K31" s="32"/>
       <c r="L31" s="32"/>
       <c r="M31" s="32"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="44"/>
       <c r="P31" s="32"/>
       <c r="Q31" s="32"/>
       <c r="R31" s="32"/>
@@ -10032,16 +10143,16 @@
       <c r="C32" s="42"/>
       <c r="D32" s="45"/>
       <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
+      <c r="F32" s="45"/>
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
+      <c r="I32" s="45"/>
       <c r="J32" s="32"/>
       <c r="K32" s="32"/>
       <c r="L32" s="32"/>
       <c r="M32" s="32"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="44"/>
       <c r="P32" s="32"/>
       <c r="Q32" s="32"/>
       <c r="R32" s="32"/>
@@ -10054,16 +10165,16 @@
       <c r="C33" s="42"/>
       <c r="D33" s="45"/>
       <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
+      <c r="F33" s="45"/>
       <c r="G33" s="32"/>
       <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
+      <c r="I33" s="45"/>
       <c r="J33" s="32"/>
       <c r="K33" s="32"/>
       <c r="L33" s="32"/>
       <c r="M33" s="32"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="44"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
       <c r="R33" s="32"/>
@@ -10076,16 +10187,16 @@
       <c r="C34" s="42"/>
       <c r="D34" s="45"/>
       <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
+      <c r="F34" s="45"/>
       <c r="G34" s="32"/>
       <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
+      <c r="I34" s="45"/>
       <c r="J34" s="32"/>
       <c r="K34" s="32"/>
       <c r="L34" s="32"/>
       <c r="M34" s="32"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="44"/>
       <c r="P34" s="32"/>
       <c r="Q34" s="32"/>
       <c r="R34" s="32"/>
@@ -10098,16 +10209,16 @@
       <c r="C35" s="42"/>
       <c r="D35" s="45"/>
       <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
+      <c r="F35" s="45"/>
       <c r="G35" s="32"/>
       <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
+      <c r="I35" s="45"/>
       <c r="J35" s="32"/>
       <c r="K35" s="32"/>
       <c r="L35" s="32"/>
       <c r="M35" s="32"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="44"/>
       <c r="P35" s="32"/>
       <c r="Q35" s="32"/>
       <c r="R35" s="32"/>
@@ -10120,16 +10231,16 @@
       <c r="C36" s="42"/>
       <c r="D36" s="45"/>
       <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
+      <c r="F36" s="45"/>
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
+      <c r="I36" s="45"/>
       <c r="J36" s="32"/>
       <c r="K36" s="32"/>
       <c r="L36" s="32"/>
       <c r="M36" s="32"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="44"/>
       <c r="P36" s="32"/>
       <c r="Q36" s="32"/>
       <c r="R36" s="32"/>
@@ -10142,16 +10253,16 @@
       <c r="C37" s="42"/>
       <c r="D37" s="45"/>
       <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
+      <c r="F37" s="45"/>
       <c r="G37" s="32"/>
       <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
+      <c r="I37" s="45"/>
       <c r="J37" s="32"/>
       <c r="K37" s="32"/>
       <c r="L37" s="32"/>
       <c r="M37" s="32"/>
-      <c r="N37" s="31"/>
-      <c r="O37" s="31"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="44"/>
       <c r="P37" s="32"/>
       <c r="Q37" s="32"/>
       <c r="R37" s="32"/>
@@ -10164,16 +10275,16 @@
       <c r="C38" s="42"/>
       <c r="D38" s="45"/>
       <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
+      <c r="F38" s="45"/>
       <c r="G38" s="32"/>
       <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
+      <c r="I38" s="45"/>
       <c r="J38" s="32"/>
       <c r="K38" s="32"/>
       <c r="L38" s="32"/>
       <c r="M38" s="32"/>
-      <c r="N38" s="31"/>
-      <c r="O38" s="31"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="44"/>
       <c r="P38" s="32"/>
       <c r="Q38" s="32"/>
       <c r="R38" s="32"/>
@@ -10186,16 +10297,16 @@
       <c r="C39" s="42"/>
       <c r="D39" s="45"/>
       <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
+      <c r="F39" s="45"/>
       <c r="G39" s="32"/>
       <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
+      <c r="I39" s="45"/>
       <c r="J39" s="32"/>
       <c r="K39" s="32"/>
       <c r="L39" s="32"/>
       <c r="M39" s="32"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
       <c r="P39" s="32"/>
       <c r="Q39" s="32"/>
       <c r="R39" s="32"/>
@@ -10208,16 +10319,16 @@
       <c r="C40" s="42"/>
       <c r="D40" s="45"/>
       <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
+      <c r="F40" s="45"/>
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
+      <c r="I40" s="45"/>
       <c r="J40" s="32"/>
       <c r="K40" s="32"/>
       <c r="L40" s="32"/>
       <c r="M40" s="32"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
+      <c r="N40" s="44"/>
+      <c r="O40" s="44"/>
       <c r="P40" s="32"/>
       <c r="Q40" s="32"/>
       <c r="R40" s="32"/>
@@ -10230,16 +10341,16 @@
       <c r="C41" s="42"/>
       <c r="D41" s="45"/>
       <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
+      <c r="F41" s="45"/>
       <c r="G41" s="32"/>
       <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
+      <c r="I41" s="45"/>
       <c r="J41" s="32"/>
       <c r="K41" s="32"/>
       <c r="L41" s="32"/>
       <c r="M41" s="32"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="44"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="32"/>
       <c r="R41" s="32"/>
@@ -10252,16 +10363,16 @@
       <c r="C42" s="42"/>
       <c r="D42" s="45"/>
       <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
+      <c r="F42" s="45"/>
       <c r="G42" s="32"/>
       <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
+      <c r="I42" s="45"/>
       <c r="J42" s="32"/>
       <c r="K42" s="32"/>
       <c r="L42" s="32"/>
       <c r="M42" s="32"/>
-      <c r="N42" s="31"/>
-      <c r="O42" s="31"/>
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
       <c r="P42" s="32"/>
       <c r="Q42" s="32"/>
       <c r="R42" s="32"/>
@@ -10274,16 +10385,16 @@
       <c r="C43" s="42"/>
       <c r="D43" s="45"/>
       <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
+      <c r="F43" s="45"/>
       <c r="G43" s="32"/>
       <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
+      <c r="I43" s="45"/>
       <c r="J43" s="32"/>
       <c r="K43" s="32"/>
       <c r="L43" s="32"/>
       <c r="M43" s="32"/>
-      <c r="N43" s="31"/>
-      <c r="O43" s="31"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
       <c r="P43" s="32"/>
       <c r="Q43" s="32"/>
       <c r="R43" s="32"/>
@@ -10296,16 +10407,16 @@
       <c r="C44" s="42"/>
       <c r="D44" s="45"/>
       <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
+      <c r="F44" s="45"/>
       <c r="G44" s="32"/>
       <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
+      <c r="I44" s="45"/>
       <c r="J44" s="32"/>
       <c r="K44" s="32"/>
       <c r="L44" s="32"/>
       <c r="M44" s="32"/>
-      <c r="N44" s="31"/>
-      <c r="O44" s="31"/>
+      <c r="N44" s="44"/>
+      <c r="O44" s="44"/>
       <c r="P44" s="32"/>
       <c r="Q44" s="32"/>
       <c r="R44" s="32"/>
@@ -10318,16 +10429,16 @@
       <c r="C45" s="42"/>
       <c r="D45" s="45"/>
       <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
+      <c r="F45" s="45"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
+      <c r="I45" s="45"/>
       <c r="J45" s="32"/>
       <c r="K45" s="32"/>
       <c r="L45" s="32"/>
       <c r="M45" s="32"/>
-      <c r="N45" s="31"/>
-      <c r="O45" s="31"/>
+      <c r="N45" s="44"/>
+      <c r="O45" s="44"/>
       <c r="P45" s="32"/>
       <c r="Q45" s="32"/>
       <c r="R45" s="32"/>
@@ -10340,16 +10451,16 @@
       <c r="C46" s="42"/>
       <c r="D46" s="45"/>
       <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
+      <c r="F46" s="45"/>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
+      <c r="I46" s="45"/>
       <c r="J46" s="32"/>
       <c r="K46" s="32"/>
       <c r="L46" s="32"/>
       <c r="M46" s="32"/>
-      <c r="N46" s="31"/>
-      <c r="O46" s="31"/>
+      <c r="N46" s="44"/>
+      <c r="O46" s="44"/>
       <c r="P46" s="32"/>
       <c r="Q46" s="32"/>
       <c r="R46" s="32"/>
@@ -10362,16 +10473,16 @@
       <c r="C47" s="42"/>
       <c r="D47" s="45"/>
       <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
+      <c r="F47" s="45"/>
       <c r="G47" s="32"/>
       <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
+      <c r="I47" s="45"/>
       <c r="J47" s="32"/>
       <c r="K47" s="32"/>
       <c r="L47" s="32"/>
       <c r="M47" s="32"/>
-      <c r="N47" s="31"/>
-      <c r="O47" s="31"/>
+      <c r="N47" s="44"/>
+      <c r="O47" s="44"/>
       <c r="P47" s="32"/>
       <c r="Q47" s="32"/>
       <c r="R47" s="32"/>
@@ -10384,16 +10495,16 @@
       <c r="C48" s="42"/>
       <c r="D48" s="45"/>
       <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
+      <c r="F48" s="45"/>
       <c r="G48" s="32"/>
       <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
+      <c r="I48" s="45"/>
       <c r="J48" s="32"/>
       <c r="K48" s="32"/>
       <c r="L48" s="32"/>
       <c r="M48" s="32"/>
-      <c r="N48" s="31"/>
-      <c r="O48" s="31"/>
+      <c r="N48" s="44"/>
+      <c r="O48" s="44"/>
       <c r="P48" s="32"/>
       <c r="Q48" s="32"/>
       <c r="R48" s="32"/>
@@ -10406,16 +10517,16 @@
       <c r="C49" s="42"/>
       <c r="D49" s="45"/>
       <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
+      <c r="F49" s="45"/>
       <c r="G49" s="32"/>
       <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
+      <c r="I49" s="45"/>
       <c r="J49" s="32"/>
       <c r="K49" s="32"/>
       <c r="L49" s="32"/>
       <c r="M49" s="32"/>
-      <c r="N49" s="31"/>
-      <c r="O49" s="31"/>
+      <c r="N49" s="44"/>
+      <c r="O49" s="44"/>
       <c r="P49" s="32"/>
       <c r="Q49" s="32"/>
       <c r="R49" s="32"/>
@@ -10428,16 +10539,16 @@
       <c r="C50" s="42"/>
       <c r="D50" s="45"/>
       <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
+      <c r="F50" s="45"/>
       <c r="G50" s="32"/>
       <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
+      <c r="I50" s="45"/>
       <c r="J50" s="32"/>
       <c r="K50" s="32"/>
       <c r="L50" s="32"/>
       <c r="M50" s="32"/>
-      <c r="N50" s="31"/>
-      <c r="O50" s="31"/>
+      <c r="N50" s="44"/>
+      <c r="O50" s="44"/>
       <c r="P50" s="32"/>
       <c r="Q50" s="32"/>
       <c r="R50" s="32"/>
@@ -10450,16 +10561,16 @@
       <c r="C51" s="42"/>
       <c r="D51" s="45"/>
       <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
+      <c r="F51" s="45"/>
       <c r="G51" s="32"/>
       <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
+      <c r="I51" s="45"/>
       <c r="J51" s="32"/>
       <c r="K51" s="32"/>
       <c r="L51" s="32"/>
       <c r="M51" s="32"/>
-      <c r="N51" s="31"/>
-      <c r="O51" s="31"/>
+      <c r="N51" s="44"/>
+      <c r="O51" s="44"/>
       <c r="P51" s="32"/>
       <c r="Q51" s="32"/>
       <c r="R51" s="32"/>
@@ -10472,16 +10583,16 @@
       <c r="C52" s="42"/>
       <c r="D52" s="45"/>
       <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
+      <c r="F52" s="45"/>
       <c r="G52" s="32"/>
       <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
+      <c r="I52" s="45"/>
       <c r="J52" s="32"/>
       <c r="K52" s="32"/>
       <c r="L52" s="32"/>
       <c r="M52" s="32"/>
-      <c r="N52" s="31"/>
-      <c r="O52" s="31"/>
+      <c r="N52" s="44"/>
+      <c r="O52" s="44"/>
       <c r="P52" s="32"/>
       <c r="Q52" s="32"/>
       <c r="R52" s="32"/>
@@ -10494,16 +10605,16 @@
       <c r="C53" s="42"/>
       <c r="D53" s="45"/>
       <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
+      <c r="F53" s="45"/>
       <c r="G53" s="32"/>
       <c r="H53" s="32"/>
-      <c r="I53" s="32"/>
+      <c r="I53" s="45"/>
       <c r="J53" s="32"/>
       <c r="K53" s="32"/>
       <c r="L53" s="32"/>
       <c r="M53" s="32"/>
-      <c r="N53" s="31"/>
-      <c r="O53" s="31"/>
+      <c r="N53" s="44"/>
+      <c r="O53" s="44"/>
       <c r="P53" s="32"/>
       <c r="Q53" s="32"/>
       <c r="R53" s="32"/>
@@ -10516,16 +10627,16 @@
       <c r="C54" s="43"/>
       <c r="D54" s="46"/>
       <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
+      <c r="F54" s="63"/>
       <c r="G54" s="37"/>
       <c r="H54" s="37"/>
-      <c r="I54" s="37"/>
+      <c r="I54" s="63"/>
       <c r="J54" s="37"/>
       <c r="K54" s="37"/>
       <c r="L54" s="37"/>
       <c r="M54" s="37"/>
-      <c r="N54" s="31"/>
-      <c r="O54" s="31"/>
+      <c r="N54" s="44"/>
+      <c r="O54" s="44"/>
       <c r="P54" s="37"/>
       <c r="Q54" s="37"/>
       <c r="R54" s="37"/>
@@ -10535,10 +10646,12 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:U4"/>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="D9:D14"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5:S54 N5:O54">
@@ -10579,41 +10692,41 @@
   <dimension ref="B2:AG54"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.625" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
-    <col min="4" max="4" width="45.25" customWidth="1"/>
-    <col min="5" max="5" width="50.5" customWidth="1"/>
-    <col min="6" max="6" width="7.875" customWidth="1"/>
-    <col min="7" max="7" width="16.125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="17.375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="21" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="27.125" customWidth="1"/>
-    <col min="13" max="13" width="12.375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="12.25" customWidth="1"/>
-    <col min="15" max="15" width="11.75" customWidth="1"/>
+    <col min="12" max="12" width="27.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
     <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="16.375" customWidth="1"/>
-    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.375" customWidth="1"/>
-    <col min="20" max="20" width="13.625" style="25" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="13.375" style="25" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="13.375" customWidth="1"/>
-    <col min="25" max="25" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" style="25" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" style="25" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="25" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="27" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:33">
@@ -10698,11 +10811,11 @@
       <c r="AG4"/>
     </row>
     <row r="5" spans="2:33" s="31" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B5" s="69"/>
-      <c r="C5" s="72" t="s">
+      <c r="B5" s="70"/>
+      <c r="C5" s="73" t="s">
         <v>301</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="76" t="s">
         <v>302</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -10722,9 +10835,9 @@
       </c>
     </row>
     <row r="6" spans="2:33" s="31" customFormat="1">
-      <c r="B6" s="70"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="76"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="77"/>
       <c r="E6" s="31" t="s">
         <v>305</v>
       </c>
@@ -10769,9 +10882,9 @@
       </c>
     </row>
     <row r="7" spans="2:33" s="31" customFormat="1">
-      <c r="B7" s="70"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="76"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="77"/>
       <c r="E7" s="31" t="s">
         <v>303</v>
       </c>
@@ -10816,9 +10929,9 @@
       </c>
     </row>
     <row r="8" spans="2:33" s="31" customFormat="1">
-      <c r="B8" s="71"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="76"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="77"/>
       <c r="E8" s="31" t="s">
         <v>312</v>
       </c>
@@ -10864,8 +10977,8 @@
     </row>
     <row r="9" spans="2:33" s="31" customFormat="1">
       <c r="B9" s="41"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="76"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="78"/>
       <c r="E9" s="31" t="s">
         <v>313</v>
       </c>
@@ -10911,14 +11024,8 @@
     </row>
     <row r="10" spans="2:33" s="31" customFormat="1">
       <c r="B10" s="41"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="31" t="s">
-        <v>314</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>13</v>
-      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="48"/>
       <c r="N10" s="31" t="s">
         <v>167</v>
       </c>
@@ -10958,14 +11065,8 @@
     </row>
     <row r="11" spans="2:33" s="31" customFormat="1">
       <c r="B11" s="41"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="76"/>
-      <c r="N11" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="O11" s="31" t="s">
-        <v>234</v>
-      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="48"/>
       <c r="X11" s="31" t="s">
         <v>185</v>
       </c>
@@ -10993,8 +11094,8 @@
     </row>
     <row r="12" spans="2:33" s="31" customFormat="1">
       <c r="B12" s="41"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="77"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="48"/>
       <c r="X12" s="31" t="s">
         <v>167</v>
       </c>
@@ -11965,8 +12066,8 @@
   <autoFilter ref="B4:U4"/>
   <mergeCells count="3">
     <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C12"/>
-    <mergeCell ref="D5:D12"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="D5:D9"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:M13 M21:M54">

</xml_diff>

<commit_message>
review phần NewProduct _ KhoaVT_ lần 2
</commit_message>
<xml_diff>
--- a/Document/Defect Log.xlsx
+++ b/Document/Defect Log.xlsx
@@ -523,7 +523,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="326">
   <si>
     <t>Project Code:</t>
   </si>
@@ -1502,6 +1502,18 @@
   </si>
   <si>
     <t>Form trình bày chưa đẹp lắm :D</t>
+  </si>
+  <si>
+    <t>Các trường ngày tháng chưa xử lý tự động</t>
+  </si>
+  <si>
+    <t>Delete Products</t>
+  </si>
+  <si>
+    <t>Viết action xóa một product trong CSDL</t>
+  </si>
+  <si>
+    <t>Khi xóa sản phẩm xong hiện ra 1 trang xóa sản phẩm không biết để làm gì</t>
   </si>
 </sst>
 </file>
@@ -1982,6 +1994,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2026,18 +2050,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3360,11 +3372,11 @@
       </c>
     </row>
     <row r="21" spans="2:32">
-      <c r="B21" s="67"/>
-      <c r="C21" s="64" t="s">
+      <c r="B21" s="71"/>
+      <c r="C21" s="68" t="s">
         <v>307</v>
       </c>
-      <c r="D21" s="64" t="s">
+      <c r="D21" s="68" t="s">
         <v>308</v>
       </c>
       <c r="E21" s="32" t="s">
@@ -3400,9 +3412,9 @@
       </c>
     </row>
     <row r="22" spans="2:32">
-      <c r="B22" s="68"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
       <c r="E22" s="32" t="s">
         <v>310</v>
       </c>
@@ -3433,9 +3445,9 @@
       </c>
     </row>
     <row r="23" spans="2:32">
-      <c r="B23" s="69"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
       <c r="E23" s="32" t="s">
         <v>311</v>
       </c>
@@ -9178,7 +9190,7 @@
   <dimension ref="B2:AG54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D14"/>
+      <selection activeCell="B9" sqref="B9:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9188,16 +9200,16 @@
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
     <col min="5" max="5" width="50.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="81" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="66" customWidth="1"/>
     <col min="7" max="7" width="16.140625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="81" customWidth="1"/>
+    <col min="9" max="9" width="9" style="66" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
     <col min="12" max="12" width="27.140625" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" style="81" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" style="81" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" style="66" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="66" customWidth="1"/>
     <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="16.42578125" customWidth="1"/>
     <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
@@ -9220,7 +9232,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="23"/>
-      <c r="F2" s="80"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="4" spans="2:33" s="30" customFormat="1" ht="27.75" customHeight="1">
       <c r="B4" s="26" t="s">
@@ -9235,7 +9247,7 @@
       <c r="E4" s="27" t="s">
         <v>292</v>
       </c>
-      <c r="F4" s="79" t="s">
+      <c r="F4" s="64" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="27" t="s">
@@ -9244,7 +9256,7 @@
       <c r="H4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="79" t="s">
+      <c r="I4" s="64" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="27" t="s">
@@ -9259,10 +9271,10 @@
       <c r="M4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="64" t="s">
         <v>264</v>
       </c>
-      <c r="O4" s="79" t="s">
+      <c r="O4" s="64" t="s">
         <v>265</v>
       </c>
       <c r="P4" s="27" t="s">
@@ -9297,11 +9309,11 @@
       <c r="AG4"/>
     </row>
     <row r="5" spans="2:33" s="31" customFormat="1">
-      <c r="B5" s="70"/>
-      <c r="C5" s="73" t="s">
+      <c r="B5" s="74"/>
+      <c r="C5" s="77" t="s">
         <v>293</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="77" t="s">
         <v>294</v>
       </c>
       <c r="E5" s="31" t="s">
@@ -9324,9 +9336,9 @@
       </c>
     </row>
     <row r="6" spans="2:33" s="31" customFormat="1">
-      <c r="B6" s="71"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
       <c r="E6" s="31" t="s">
         <v>296</v>
       </c>
@@ -9374,9 +9386,9 @@
       </c>
     </row>
     <row r="7" spans="2:33" s="31" customFormat="1">
-      <c r="B7" s="71"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
       <c r="E7" s="31" t="s">
         <v>297</v>
       </c>
@@ -9424,9 +9436,9 @@
       </c>
     </row>
     <row r="8" spans="2:33" s="31" customFormat="1">
-      <c r="B8" s="72"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
       <c r="E8" s="31" t="s">
         <v>306</v>
       </c>
@@ -9474,11 +9486,13 @@
       </c>
     </row>
     <row r="9" spans="2:33" s="31" customFormat="1" ht="60">
-      <c r="B9" s="41"/>
-      <c r="C9" s="73" t="s">
+      <c r="B9" s="77">
+        <v>40865</v>
+      </c>
+      <c r="C9" s="77" t="s">
         <v>314</v>
       </c>
-      <c r="D9" s="73" t="s">
+      <c r="D9" s="77" t="s">
         <v>315</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -9526,9 +9540,9 @@
       </c>
     </row>
     <row r="10" spans="2:33" s="31" customFormat="1" ht="30">
-      <c r="B10" s="41"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
       <c r="E10" s="11" t="s">
         <v>317</v>
       </c>
@@ -9574,10 +9588,10 @@
       </c>
     </row>
     <row r="11" spans="2:33" s="31" customFormat="1" ht="30">
-      <c r="B11" s="41"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="82" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="67" t="s">
         <v>318</v>
       </c>
       <c r="F11" s="44" t="s">
@@ -9616,9 +9630,9 @@
       </c>
     </row>
     <row r="12" spans="2:33" s="31" customFormat="1">
-      <c r="B12" s="41"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
       <c r="E12" s="31" t="s">
         <v>320</v>
       </c>
@@ -9658,9 +9672,9 @@
       </c>
     </row>
     <row r="13" spans="2:33" s="31" customFormat="1">
-      <c r="B13" s="41"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
       <c r="E13" s="31" t="s">
         <v>319</v>
       </c>
@@ -9698,9 +9712,9 @@
       </c>
     </row>
     <row r="14" spans="2:33" s="31" customFormat="1">
-      <c r="B14" s="41"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
       <c r="E14" s="31" t="s">
         <v>321</v>
       </c>
@@ -9735,13 +9749,27 @@
       </c>
     </row>
     <row r="15" spans="2:33" s="31" customFormat="1">
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
+      <c r="B15" s="31">
+        <v>40865</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>325</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="N15" s="44" t="s">
+        <v>145</v>
+      </c>
       <c r="X15" s="31" t="s">
         <v>234</v>
       </c>
@@ -10646,36 +10674,37 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:U4"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D8"/>
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="D9:D14"/>
+    <mergeCell ref="B9:B14"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5:S54 N5:O54">
       <formula1>$X$7:$X$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21:F54 F5:F13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21:F54 F5:F13 F15">
       <formula1>$Y$7:$Y$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G13 G21:G54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G13 G21:G54 G15">
       <formula1>$Z$7:$Z$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H13 H21:H54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H13 H21:H54 H15">
       <formula1>$AA$7:$AA$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I13 I21:I54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I13 I21:I54 I15">
       <formula1>$AB$7:$AB$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J13 J21:J54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J13 J21:J54 J15">
       <formula1>$AC$7:$AC$26</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K13 K21:K54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K13 K21:K54 K15">
       <formula1>$AD$7:$AD$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:M13 M21:M54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:M13 M21:M54 M15">
       <formula1>$AE$7:$AE$19</formula1>
     </dataValidation>
   </dataValidations>
@@ -10691,8 +10720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AG54"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="D1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10811,11 +10840,11 @@
       <c r="AG4"/>
     </row>
     <row r="5" spans="2:33" s="31" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B5" s="70"/>
-      <c r="C5" s="73" t="s">
+      <c r="B5" s="74"/>
+      <c r="C5" s="77" t="s">
         <v>301</v>
       </c>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="80" t="s">
         <v>302</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -10835,9 +10864,9 @@
       </c>
     </row>
     <row r="6" spans="2:33" s="31" customFormat="1">
-      <c r="B6" s="71"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="77"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="81"/>
       <c r="E6" s="31" t="s">
         <v>305</v>
       </c>
@@ -10882,9 +10911,9 @@
       </c>
     </row>
     <row r="7" spans="2:33" s="31" customFormat="1">
-      <c r="B7" s="71"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="77"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="81"/>
       <c r="E7" s="31" t="s">
         <v>303</v>
       </c>
@@ -10929,9 +10958,9 @@
       </c>
     </row>
     <row r="8" spans="2:33" s="31" customFormat="1">
-      <c r="B8" s="72"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="77"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="81"/>
       <c r="E8" s="31" t="s">
         <v>312</v>
       </c>
@@ -10977,8 +11006,8 @@
     </row>
     <row r="9" spans="2:33" s="31" customFormat="1">
       <c r="B9" s="41"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="81"/>
       <c r="E9" s="31" t="s">
         <v>313</v>
       </c>
@@ -11024,8 +11053,14 @@
     </row>
     <row r="10" spans="2:33" s="31" customFormat="1">
       <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="48"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="31" t="s">
+        <v>322</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>13</v>
+      </c>
       <c r="N10" s="31" t="s">
         <v>167</v>
       </c>
@@ -12066,26 +12101,26 @@
   <autoFilter ref="B4:U4"/>
   <mergeCells count="3">
     <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="D5:D10"/>
+    <mergeCell ref="C5:C10"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:M13 M21:M54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M21:M54 M5:M13">
       <formula1>$AE$7:$AE$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K13 K21:K54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K21:K54 K5:K13">
       <formula1>$AD$7:$AD$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J13 J21:J54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J21:J54 J5:J13">
       <formula1>$AC$7:$AC$26</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I13 I21:I54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I21:I54 I5:I13">
       <formula1>$AB$7:$AB$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H13 H21:H54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H21:H54 H5:H13">
       <formula1>$AA$7:$AA$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G13 G21:G54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G21:G54 G5:G13">
       <formula1>$Z$7:$Z$21</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21:F54 F5:F13">

</xml_diff>